<commit_message>
remove constants.csv, handle errant ref_tag values, deal with integer/float ref_tags
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A6AF27-26CF-7F44-A67E-59406F042A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9A64D9-F8A0-3647-83E2-A8CE4B31AB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31580" yWindow="-2360" windowWidth="28760" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-31580" yWindow="-2380" windowWidth="28760" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="181">
   <si>
     <t>corrected to m/z=44 peak area of 20 Vs</t>
   </si>
@@ -421,9 +421,6 @@
   </si>
   <si>
     <t>COPY AND PASTE IN RAW DATA</t>
-  </si>
-  <si>
-    <t>REF TAG SHOULD MATCH CONSTANTS.CSV</t>
   </si>
   <si>
     <t>USER INPUTS:</t>
@@ -609,13 +606,13 @@
     <t xml:space="preserve"> Both algebraic and least squares methods are also available in the "Scrambling" function of pyisotopomer.</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
     <t>CA06261</t>
   </si>
   <si>
     <t>CA08214</t>
+  </si>
+  <si>
+    <t>"ref_tag" should match scale_normalization tab</t>
   </si>
 </sst>
 </file>
@@ -1364,18 +1361,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1389,6 +1374,18 @@
     <xf numFmtId="169" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -3574,128 +3571,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="14">
-          <cell r="F14">
-            <v>-8.9966974850617758E-4</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="F15">
-            <v>6.4958520159854336E-4</v>
-          </cell>
-          <cell r="H15">
-            <v>-2.6012135306176113E-4</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="F16">
-            <v>4.4463781866937646E-3</v>
-          </cell>
-          <cell r="H16">
-            <v>5.9320472770020231E-3</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="F17">
-            <v>6.3498277796843113E-5</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="F18">
-            <v>-2.0504572115828708E-4</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19">
-            <v>-3.5557699463491049E-2</v>
-          </cell>
-          <cell r="H19">
-            <v>-3.4927970568279593E-2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20">
-            <v>2.311109460617683E-2</v>
-          </cell>
-          <cell r="H20">
-            <v>2.3866694850012186E-2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="F21">
-            <v>-9.434161745802187E-5</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="F22">
-            <v>1.3085015214356208E-4</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="F23">
-            <v>-3.3863114557107131E-2</v>
-          </cell>
-          <cell r="H23">
-            <v>-3.4927970568279593E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="F24">
-            <v>2.2945824482518178E-2</v>
-          </cell>
-          <cell r="H24">
-            <v>2.3866694850012186E-2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="F25">
-            <v>1.8523031837536059E-4</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="F26">
-            <v>1.3890009220120811E-4</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="F27">
-            <v>-3.4725011698547963E-2</v>
-          </cell>
-          <cell r="H27">
-            <v>-3.4927970568279593E-2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="F28">
-            <v>2.1989621732885784E-2</v>
-          </cell>
-          <cell r="H28">
-            <v>2.3866694850012186E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="F29">
-            <v>5.1595548552567936E-3</v>
-          </cell>
-          <cell r="H29">
-            <v>5.9320472770020231E-3</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="F30">
-            <v>-2.1453861240111502E-4</v>
-          </cell>
-          <cell r="H30">
-            <v>-2.6012135306176113E-4</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="F31">
-            <v>-1.6472871032642412E-3</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
     </sheetDataSet>
@@ -4003,7 +3879,7 @@
   <dimension ref="A1:BH54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4028,10 +3904,10 @@
   <sheetData>
     <row r="1" spans="1:60" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>117</v>
@@ -4050,7 +3926,7 @@
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
       <c r="AI1" s="73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AJ1" s="74"/>
       <c r="AL1" s="51" t="s">
@@ -4074,7 +3950,7 @@
         <v>46</v>
       </c>
       <c r="AZ1" s="103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BA1" s="103"/>
       <c r="BB1" s="103"/>
@@ -4178,10 +4054,10 @@
         <v>27</v>
       </c>
       <c r="AI2" s="75" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ2" s="75" t="s">
         <v>121</v>
-      </c>
-      <c r="AJ2" s="75" t="s">
-        <v>122</v>
       </c>
       <c r="AK2" s="23"/>
       <c r="AL2" s="55" t="s">
@@ -4225,31 +4101,31 @@
       </c>
       <c r="AY2" s="44"/>
       <c r="AZ2" s="106" t="s">
+        <v>165</v>
+      </c>
+      <c r="BA2" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="BA2" s="106" t="s">
+      <c r="BB2" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="BB2" s="106" t="s">
+      <c r="BC2" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="BC2" s="106" t="s">
+      <c r="BD2" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="BD2" s="107" t="s">
+      <c r="BE2" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="BE2" s="108" t="s">
+      <c r="BF2" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="BF2" s="109" t="s">
+      <c r="BG2" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="BG2" s="108" t="s">
-        <v>173</v>
-      </c>
       <c r="BH2" s="110" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:60" ht="17" thickBot="1">
@@ -4412,7 +4288,7 @@
         <v>156</v>
       </c>
       <c r="BC3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BD3" s="78">
         <f>BB3*concentration_constants!$B$6</f>
@@ -4948,7 +4824,7 @@
         <v>156</v>
       </c>
       <c r="BC6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BD6" s="78">
         <f>BB6*concentration_constants!$B$6</f>
@@ -5391,7 +5267,7 @@
         <v>0.42850050000000001</v>
       </c>
       <c r="X9" s="71" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y9" s="3"/>
       <c r="AA9" s="28">
@@ -5481,7 +5357,7 @@
         <v>156</v>
       </c>
       <c r="BC9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BD9" s="78">
         <f>BB9*concentration_constants!$B$6</f>
@@ -5835,7 +5711,7 @@
         <v>156</v>
       </c>
       <c r="BC11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BD11" s="78">
         <f>BB11*concentration_constants!$B$6</f>
@@ -6351,7 +6227,7 @@
         <v>156</v>
       </c>
       <c r="BC14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BD14" s="78">
         <f>BB14*concentration_constants!$B$6</f>
@@ -6523,7 +6399,7 @@
         <v>156</v>
       </c>
       <c r="BC15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BD15" s="78">
         <f>BB15*concentration_constants!$B$6</f>
@@ -7813,7 +7689,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7838,71 +7714,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="117" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="118" t="s">
+      <c r="A1" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="125" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="119" t="s">
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="115" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="119"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="115"/>
     </row>
     <row r="2" spans="1:17" ht="17">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="121" t="s">
+      <c r="C2" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="121" t="s">
+      <c r="D2" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="121" t="s">
+      <c r="E2" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="121" t="s">
+      <c r="F2" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="122" t="s">
+      <c r="G2" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="122" t="s">
+      <c r="H2" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="122" t="s">
+      <c r="I2" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="122" t="s">
+      <c r="J2" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="122" t="s">
+      <c r="K2" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="122" t="s">
+      <c r="L2" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="122" t="s">
+      <c r="M2" s="118" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="122" t="s">
+      <c r="N2" s="118" t="s">
         <v>106</v>
       </c>
     </row>
@@ -8070,7 +7946,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="68" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B6" s="69">
         <v>-22.21</v>
@@ -8178,7 +8054,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="68" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B8" s="69">
         <v>17.11</v>
@@ -8231,55 +8107,55 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="123" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="124">
+      <c r="A9" s="119">
+        <v>90454</v>
+      </c>
+      <c r="B9" s="120">
         <v>25.73</v>
       </c>
-      <c r="C9" s="124">
+      <c r="C9" s="120">
         <v>25.44</v>
       </c>
-      <c r="D9" s="124">
+      <c r="D9" s="120">
         <f t="shared" si="6"/>
         <v>25.585000000000001</v>
       </c>
-      <c r="E9" s="124">
+      <c r="E9" s="120">
         <v>35.880000000000003</v>
       </c>
-      <c r="F9" s="124">
+      <c r="F9" s="120">
         <f t="shared" si="0"/>
         <v>0.28999999999999915</v>
       </c>
-      <c r="G9" s="125">
+      <c r="G9" s="121">
         <f t="shared" si="1"/>
         <v>3.7710963450000002E-3</v>
       </c>
-      <c r="H9" s="125">
+      <c r="H9" s="121">
         <f t="shared" si="1"/>
         <v>3.7700301599999995E-3</v>
       </c>
-      <c r="I9" s="125">
+      <c r="I9" s="121">
         <f t="shared" si="2"/>
         <v>2.0771465759999996E-3</v>
       </c>
-      <c r="J9" s="125">
+      <c r="J9" s="121">
         <f t="shared" si="3"/>
         <v>3.8687348777560239E-4</v>
       </c>
-      <c r="K9" s="126">
+      <c r="K9" s="122">
         <f t="shared" si="4"/>
         <v>7.9279999927756029E-3</v>
       </c>
-      <c r="L9" s="126">
+      <c r="L9" s="122">
         <f t="shared" si="5"/>
         <v>2.0942811848696616E-3</v>
       </c>
-      <c r="M9" s="127">
+      <c r="M9" s="123">
         <f>K9/[1]size_correction!X$3</f>
         <v>1.0241537838167138</v>
       </c>
-      <c r="N9" s="127">
+      <c r="N9" s="123">
         <f>L9/[1]size_correction!Y$3</f>
         <v>0.9966620412810443</v>
       </c>
@@ -8303,7 +8179,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="114"/>
       <c r="B11" s="70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11" s="114"/>
@@ -9014,16 +8890,16 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N1">
         <v>3.7990000000000002E-4</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
@@ -9032,10 +8908,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N2">
         <v>2.0052E-3</v>
@@ -9044,24 +8920,24 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="126" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="127" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="116" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
       <c r="M3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N3">
         <v>0.51600000000000001</v>
@@ -9071,52 +8947,52 @@
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="113" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="113" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" s="113" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="113" t="s">
+        <v>144</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="113" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="L4" s="113" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" s="113" t="s">
-        <v>142</v>
-      </c>
-      <c r="N4" s="113" t="s">
-        <v>145</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="Q4" s="113" t="s">
         <v>95</v>
@@ -9610,7 +9486,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -9621,28 +9497,28 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="81">
         <f>B12</f>
         <v>0.4623614635092998</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="81">
         <f>C12</f>
         <v>0.10975712247295455</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G2" s="50">
         <f>1/B2</f>
         <v>2.1628100067208269</v>
       </c>
       <c r="H2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L2" s="80"/>
       <c r="M2" s="80"/>
@@ -9651,7 +9527,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3" s="81">
         <f>B13</f>
@@ -9669,20 +9545,20 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="81">
         <v>1.026</v>
       </c>
       <c r="C4" s="79"/>
       <c r="E4" s="79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4">
         <v>0.99819999999999998</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I4">
         <v>1.002</v>
@@ -9696,7 +9572,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="85">
         <f>1/B4</f>
@@ -9704,14 +9580,14 @@
       </c>
       <c r="C5" s="79"/>
       <c r="E5" s="79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="85">
         <f>1/F4</f>
         <v>1.0018032458425166</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I5" s="85">
         <f>1/I4</f>
@@ -9727,7 +9603,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="88">
         <f>B5/1000</f>
@@ -9735,14 +9611,14 @@
       </c>
       <c r="C6" s="79"/>
       <c r="E6" s="79" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6" s="88">
         <f>F5/1000</f>
         <v>1.0018032458425166E-3</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I6" s="88">
         <f>I5/1000</f>
@@ -9771,7 +9647,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="93" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="93"/>
@@ -9785,10 +9661,10 @@
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="24"/>
@@ -9807,7 +9683,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13">
         <v>8.0186890671505306E-3</v>

</xml_diff>

<commit_message>
update README to reflect removal of constants.csv
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9A64D9-F8A0-3647-83E2-A8CE4B31AB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6748EB9B-AE6D-6E4B-ABF1-CD371AEA03D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31580" yWindow="-2380" windowWidth="28760" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="scrambling" sheetId="4" r:id="rId3"/>
     <sheet name="concentration_constants" sheetId="5" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Rsolve18">_xlfn.LAMBDA(_xlpm.Rsam18,_xlpm.n,_xlpm.Rsam45,_xlpm.Rsam46,_xlpm.D17O,_xlpm.k,_xlpm.RVSMOW18,_xlpm.RVSMOW17,       IF(_xlpm.n&gt;0,Rsolve18(_xlfn.LET(_xlpm.Rsam17,(1 + _xlpm.D17O / 1000) * _xlpm.RVSMOW17 * (_xlpm.Rsam18/_xlpm.RVSMOW18) ^ _xlpm.k,         _xlpm.Rsam46 - (_xlpm.Rsam45 - _xlpm.Rsam17) * _xlpm.Rsam17 - (_xlpm.Rsam45 - _xlpm.Rsam17) ^ 2/4),_xlpm.n-1,_xlpm.Rsam45,_xlpm.Rsam46,_xlpm.D17O,_xlpm.k,_xlpm.RVSMOW18,_xlpm.RVSMOW17),               _xlpm.Rsam18))</definedName>
   </definedNames>
@@ -3551,34 +3548,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="size_correction"/>
-      <sheetName val="scale_normalization"/>
-      <sheetName val="scrambling"/>
-      <sheetName val="concentration_constants"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="X3">
-            <v>7.7410249496226297E-3</v>
-          </cell>
-          <cell r="Y3">
-            <v>2.1012952215756198E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3879,7 +3848,7 @@
   <dimension ref="A1:BH54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8152,11 +8121,9 @@
         <v>2.0942811848696616E-3</v>
       </c>
       <c r="M9" s="123">
-        <f>K9/[1]size_correction!X$3</f>
         <v>1.0241537838167138</v>
       </c>
       <c r="N9" s="123">
-        <f>L9/[1]size_correction!Y$3</f>
         <v>0.9966620412810443</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update README to reflect updated template, update template, rename isotopereferences.py
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6748EB9B-AE6D-6E4B-ABF1-CD371AEA03D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE88AA59-F3FC-9D4E-B625-BBC33787148B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31580" yWindow="-2380" windowWidth="28760" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="20420" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="182">
   <si>
     <t>corrected to m/z=44 peak area of 20 Vs</t>
   </si>
@@ -348,9 +348,6 @@
     <t>run_date</t>
   </si>
   <si>
-    <t>PYTHON/MATLAB INPUTS</t>
-  </si>
-  <si>
     <t>gamma</t>
   </si>
   <si>
@@ -433,9 +430,6 @@
   </si>
   <si>
     <t>scale normalized 45R and 46R</t>
-  </si>
-  <si>
-    <t>USER INPUT: CALIBRATED DELTA VALS FOR EACH REFERENCE MATERIAL</t>
   </si>
   <si>
     <t>USER INPUT: REFERENCE APPROPRIATE VALUES IN COLUMNS M &amp; N</t>
@@ -609,7 +603,16 @@
     <t>CA08214</t>
   </si>
   <si>
-    <t>"ref_tag" should match scale_normalization tab</t>
+    <t>PYTHON INPUTS: CALIBRATED DELTA VALS FOR EACH REFERENCE MATERIAL</t>
+  </si>
+  <si>
+    <t>PYTHON INPUTS</t>
+  </si>
+  <si>
+    <t>D17O</t>
+  </si>
+  <si>
+    <t>SCRAMBLING OUTPUT: CHECK VALUES</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,6 +887,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1146,7 +1155,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1371,6 +1380,9 @@
     <xf numFmtId="169" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1383,6 +1395,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -3845,10 +3861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
-  <dimension ref="A1:BH54"/>
+  <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AU26" sqref="AU26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3864,26 +3880,26 @@
     <col min="35" max="35" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="40" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.6640625" style="61" customWidth="1"/>
-    <col min="42" max="42" width="10.1640625" customWidth="1"/>
-    <col min="43" max="43" width="15.6640625" style="44" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" customWidth="1"/>
-    <col min="46" max="46" width="13.5" customWidth="1"/>
+    <col min="41" max="41" width="7.83203125" customWidth="1"/>
+    <col min="42" max="42" width="9.6640625" style="61" customWidth="1"/>
+    <col min="43" max="43" width="10.1640625" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" style="44" customWidth="1"/>
+    <col min="45" max="45" width="14.33203125" customWidth="1"/>
+    <col min="46" max="48" width="10.83203125" style="50"/>
+    <col min="51" max="51" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="17" thickBot="1">
+    <row r="1" spans="1:65" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>117</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="G1" s="1"/>
       <c r="W1" s="71" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="3"/>
@@ -3895,42 +3911,48 @@
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
       <c r="AI1" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AJ1" s="74"/>
       <c r="AL1" s="51" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="AM1" s="51"/>
       <c r="AN1" s="51"/>
-      <c r="AO1" s="58"/>
-      <c r="AP1" s="51"/>
-      <c r="AQ1" s="45"/>
-      <c r="AS1" s="38" t="s">
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="45"/>
+      <c r="AT1" s="129" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU1" s="129"/>
+      <c r="AV1" s="129"/>
+      <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="38" t="s">
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="38" t="s">
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="103" t="s">
-        <v>164</v>
-      </c>
-      <c r="BA1" s="103"/>
-      <c r="BB1" s="103"/>
-      <c r="BC1" s="103"/>
-      <c r="BD1" s="104"/>
-      <c r="BE1" s="105"/>
-      <c r="BF1" s="105"/>
-      <c r="BG1" s="105"/>
-      <c r="BH1" s="105"/>
-    </row>
-    <row r="2" spans="1:60" ht="52" thickBot="1">
+      <c r="BE1" s="103" t="s">
+        <v>162</v>
+      </c>
+      <c r="BF1" s="103"/>
+      <c r="BG1" s="103"/>
+      <c r="BH1" s="103"/>
+      <c r="BI1" s="104"/>
+      <c r="BJ1" s="105"/>
+      <c r="BK1" s="105"/>
+      <c r="BL1" s="105"/>
+      <c r="BM1" s="105"/>
+    </row>
+    <row r="2" spans="1:65" ht="52" thickBot="1">
       <c r="A2" s="8" t="s">
         <v>93</v>
       </c>
@@ -4023,10 +4045,10 @@
         <v>27</v>
       </c>
       <c r="AI2" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ2" s="75" t="s">
         <v>120</v>
-      </c>
-      <c r="AJ2" s="75" t="s">
-        <v>121</v>
       </c>
       <c r="AK2" s="23"/>
       <c r="AL2" s="55" t="s">
@@ -4038,66 +4060,78 @@
       <c r="AN2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AO2" s="59" t="s">
+      <c r="AO2" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="AP2" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="AP2" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ2" s="46" t="s">
+      <c r="AR2" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AS2" s="39" t="s">
+      <c r="AT2" s="130" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU2" s="131" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" s="132" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX2" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="AT2" s="39" t="s">
+      <c r="AY2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AU2" s="39" t="s">
+      <c r="AZ2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="AV2" s="39" t="s">
+      <c r="BA2" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="AW2" s="39" t="s">
+      <c r="BB2" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="40" t="s">
+      <c r="BC2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="106" t="s">
+      <c r="BD2" s="44"/>
+      <c r="BE2" s="106" t="s">
+        <v>163</v>
+      </c>
+      <c r="BF2" s="106" t="s">
+        <v>164</v>
+      </c>
+      <c r="BG2" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="BA2" s="106" t="s">
+      <c r="BH2" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="BB2" s="106" t="s">
+      <c r="BI2" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="BC2" s="106" t="s">
+      <c r="BJ2" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="BD2" s="107" t="s">
+      <c r="BK2" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="BE2" s="108" t="s">
+      <c r="BL2" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="BF2" s="109" t="s">
-        <v>171</v>
-      </c>
-      <c r="BG2" s="108" t="s">
-        <v>172</v>
-      </c>
-      <c r="BH2" s="110" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:60" ht="17" thickBot="1">
+      <c r="BM2" s="110" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" ht="17" thickBot="1">
       <c r="A3">
         <v>201204</v>
       </c>
@@ -4213,74 +4247,86 @@
         <f>AJ3*$Y$3</f>
         <v>2.1161148587211971E-3</v>
       </c>
-      <c r="AO3" s="56">
+      <c r="AO3" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP3" s="57">
+      <c r="AQ3" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ3" s="47">
+      <c r="AR3" s="47">
         <f>A3</f>
         <v>201204</v>
       </c>
-      <c r="AR3" t="str">
+      <c r="AS3" t="str">
         <f>D3</f>
         <v>ATM_EQ_SW</v>
       </c>
-      <c r="AS3" s="50">
+      <c r="AT3" s="50">
+        <v>6.1837131146746902</v>
+      </c>
+      <c r="AU3" s="50">
+        <v>24.279175342507699</v>
+      </c>
+      <c r="AV3" s="50">
+        <v>47.588174908592201</v>
+      </c>
+      <c r="AX3" s="50">
         <v>15.105455486877901</v>
       </c>
-      <c r="AT3" s="50">
+      <c r="AY3" s="50">
         <v>-2.7098456777153701</v>
       </c>
-      <c r="AU3" s="50">
+      <c r="AZ3" s="50">
         <v>17.815301164593201</v>
       </c>
-      <c r="AV3" s="50">
+      <c r="BA3" s="50">
         <v>6.19780490458127</v>
       </c>
-      <c r="AW3" s="50">
+      <c r="BB3" s="50">
         <v>24.009727067820499</v>
       </c>
-      <c r="AX3" s="50">
+      <c r="BC3" s="50">
         <v>47.054171086232202</v>
       </c>
-      <c r="AY3" s="44"/>
-      <c r="AZ3">
+      <c r="BD3" s="44"/>
+      <c r="BE3">
         <v>265</v>
       </c>
-      <c r="BA3">
+      <c r="BF3">
         <v>109</v>
       </c>
-      <c r="BB3">
-        <f>AZ3-BA3</f>
+      <c r="BG3">
+        <f>BE3-BF3</f>
         <v>156</v>
       </c>
-      <c r="BC3" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD3" s="78">
-        <f>BB3*concentration_constants!$B$6</f>
+      <c r="BH3" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI3" s="78">
+        <f>BG3*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE3" s="50">
+      <c r="BJ3" s="50">
         <f>I3*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.3147589419488055</v>
       </c>
-      <c r="BF3" s="50">
-        <f>BE3*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK3" s="50">
+        <f>BJ3*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32759693848642901</v>
       </c>
-      <c r="BG3" s="50">
-        <f>BE3/BD3</f>
+      <c r="BL3" s="50">
+        <f>BJ3/BI3</f>
         <v>15.223991502817144</v>
       </c>
-      <c r="BH3" s="50">
-        <f>BF3/BD3</f>
+      <c r="BM3" s="50">
+        <f>BK3/BI3</f>
         <v>2.1545798646607448</v>
       </c>
     </row>
-    <row r="4" spans="1:60" ht="17" thickBot="1">
+    <row r="4" spans="1:65" ht="17" thickBot="1">
       <c r="A4">
         <v>201205</v>
       </c>
@@ -4387,74 +4433,86 @@
         <f t="shared" ref="AN4:AN17" si="9">AJ4*$Y$3</f>
         <v>2.09139498425152E-3</v>
       </c>
-      <c r="AO4" s="56">
+      <c r="AO4" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP4" s="57">
+      <c r="AQ4" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ4" s="47">
-        <f t="shared" ref="AQ4:AQ17" si="10">A4</f>
+      <c r="AR4" s="47">
+        <f t="shared" ref="AR4:AR17" si="10">A4</f>
         <v>201205</v>
       </c>
-      <c r="AR4" s="41" t="str">
-        <f t="shared" ref="AR4:AR17" si="11">D4</f>
+      <c r="AS4" s="41" t="str">
+        <f t="shared" ref="AS4:AS17" si="11">D4</f>
         <v>S2_ref_1</v>
       </c>
-      <c r="AS4" s="50">
+      <c r="AT4" s="50">
+        <v>-3.5025945279739599</v>
+      </c>
+      <c r="AU4" s="50">
+        <v>17.995404021976</v>
+      </c>
+      <c r="AV4" s="50">
+        <v>35.169038165624201</v>
+      </c>
+      <c r="AX4" s="50">
         <v>6.8736240880515798</v>
       </c>
-      <c r="AT4" s="50">
+      <c r="AY4" s="50">
         <v>-13.881471917271901</v>
       </c>
-      <c r="AU4" s="50">
+      <c r="AZ4" s="50">
         <v>20.755096005323502</v>
       </c>
-      <c r="AV4" s="50">
+      <c r="BA4" s="50">
         <v>-3.5039239146101799</v>
       </c>
-      <c r="AW4" s="50">
+      <c r="BB4" s="50">
         <v>17.848649659933699</v>
       </c>
-      <c r="AX4" s="50">
+      <c r="BC4" s="50">
         <v>34.879852068524698</v>
       </c>
-      <c r="AY4" s="44"/>
-      <c r="AZ4">
+      <c r="BD4" s="44"/>
+      <c r="BE4">
         <v>265</v>
       </c>
-      <c r="BA4">
+      <c r="BF4">
         <v>109</v>
       </c>
-      <c r="BB4">
-        <f t="shared" ref="BB4:BB5" si="12">AZ4-BA4</f>
+      <c r="BG4">
+        <f t="shared" ref="BG4:BG5" si="12">BE4-BF4</f>
         <v>156</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BH4" t="s">
         <v>39</v>
       </c>
-      <c r="BD4" s="78">
-        <f>BB4*concentration_constants!$F$6</f>
+      <c r="BI4" s="78">
+        <f>BG4*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE4" s="50">
+      <c r="BJ4" s="50">
         <f>I4*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.0120000289208293</v>
       </c>
-      <c r="BF4" s="50">
-        <f>BE4*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK4" s="50">
+        <f>BJ4*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.33318789796769971</v>
       </c>
-      <c r="BG4" s="50">
-        <f t="shared" ref="BG4:BG5" si="13">BE4/BD4</f>
+      <c r="BL4" s="50">
+        <f t="shared" ref="BL4:BL5" si="13">BJ4/BI4</f>
         <v>19.272938646594689</v>
       </c>
-      <c r="BH4" s="50">
-        <f t="shared" ref="BH4:BH5" si="14">BF4/BD4</f>
+      <c r="BM4" s="50">
+        <f t="shared" ref="BM4:BM5" si="14">BK4/BI4</f>
         <v>2.1319753830215245</v>
       </c>
     </row>
-    <row r="5" spans="1:60">
+    <row r="5" spans="1:65">
       <c r="A5">
         <v>201205</v>
       </c>
@@ -4517,7 +4575,7 @@
         <v>0.42933650000000001</v>
       </c>
       <c r="W5" s="71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="3"/>
@@ -4566,74 +4624,86 @@
         <f t="shared" si="9"/>
         <v>2.1097889665454826E-3</v>
       </c>
-      <c r="AO5" s="56">
+      <c r="AO5" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP5" s="57">
+      <c r="AQ5" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ5" s="47">
+      <c r="AR5" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR5" s="41" t="str">
+      <c r="AS5" s="41" t="str">
         <f t="shared" si="11"/>
         <v>B6_ref_1</v>
       </c>
-      <c r="AS5" s="50">
+      <c r="AT5" s="50">
+        <v>0.359221158885425</v>
+      </c>
+      <c r="AU5" s="50">
+        <v>22.697206561636399</v>
+      </c>
+      <c r="AV5" s="50">
+        <v>44.4548477102446</v>
+      </c>
+      <c r="AX5" s="50">
         <v>-0.53970856962448599</v>
       </c>
-      <c r="AT5" s="50">
+      <c r="AY5" s="50">
         <v>1.2825215740412901</v>
       </c>
-      <c r="AU5" s="50">
+      <c r="AZ5" s="50">
         <v>-1.82223014366578</v>
       </c>
-      <c r="AV5" s="50">
+      <c r="BA5" s="50">
         <v>0.37140650220840399</v>
       </c>
-      <c r="AW5" s="50">
+      <c r="BB5" s="50">
         <v>22.461390435589401</v>
       </c>
-      <c r="AX5" s="50">
+      <c r="BC5" s="50">
         <v>43.988167450184299</v>
       </c>
-      <c r="AY5" s="44"/>
-      <c r="AZ5">
+      <c r="BD5" s="44"/>
+      <c r="BE5">
         <v>265</v>
       </c>
-      <c r="BA5">
+      <c r="BF5">
         <v>109</v>
       </c>
-      <c r="BB5">
+      <c r="BG5">
         <f t="shared" si="12"/>
         <v>156</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BH5" t="s">
         <v>39</v>
       </c>
-      <c r="BD5" s="78">
-        <f>BB5*concentration_constants!$F$6</f>
+      <c r="BI5" s="78">
+        <f>BG5*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE5" s="50">
+      <c r="BJ5" s="50">
         <f>I5*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.9048847269174694</v>
       </c>
-      <c r="BF5" s="50">
-        <f>BE5*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK5" s="50">
+        <f>BJ5*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.38845979713665457</v>
       </c>
-      <c r="BG5" s="50">
+      <c r="BL5" s="50">
         <f t="shared" si="13"/>
         <v>63.378563682109089</v>
       </c>
-      <c r="BH5" s="50">
+      <c r="BM5" s="50">
         <f t="shared" si="14"/>
         <v>2.4856446762936448</v>
       </c>
     </row>
-    <row r="6" spans="1:60">
+    <row r="6" spans="1:65">
       <c r="A6">
         <v>201205</v>
       </c>
@@ -4749,74 +4819,86 @@
         <f t="shared" si="9"/>
         <v>2.1164798861162187E-3</v>
       </c>
-      <c r="AO6" s="56">
+      <c r="AO6" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP6" s="57">
+      <c r="AQ6" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ6" s="47">
+      <c r="AR6" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR6" t="str">
+      <c r="AS6" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="AS6" s="50">
+      <c r="AT6" s="50">
+        <v>6.9823553262469096</v>
+      </c>
+      <c r="AU6" s="50">
+        <v>24.3669184468542</v>
+      </c>
+      <c r="AV6" s="50">
+        <v>47.762096293894203</v>
+      </c>
+      <c r="AX6" s="50">
         <v>14.851574153242799</v>
       </c>
-      <c r="AT6" s="50">
+      <c r="AY6" s="50">
         <v>-0.85838254078074405</v>
       </c>
-      <c r="AU6" s="50">
+      <c r="AZ6" s="50">
         <v>15.7099566940236</v>
       </c>
-      <c r="AV6" s="50">
+      <c r="BA6" s="50">
         <v>6.9965958062310696</v>
       </c>
-      <c r="AW6" s="50">
+      <c r="BB6" s="50">
         <v>24.095420378555701</v>
       </c>
-      <c r="AX6" s="50">
+      <c r="BC6" s="50">
         <v>47.223987370547697</v>
       </c>
-      <c r="AY6" s="44"/>
-      <c r="AZ6">
+      <c r="BD6" s="44"/>
+      <c r="BE6">
         <v>265</v>
       </c>
-      <c r="BA6">
+      <c r="BF6">
         <v>109</v>
       </c>
-      <c r="BB6">
-        <f t="shared" ref="BB6:BB17" si="15">AZ6-BA6</f>
+      <c r="BG6">
+        <f t="shared" ref="BG6:BG17" si="15">BE6-BF6</f>
         <v>156</v>
       </c>
-      <c r="BC6" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD6" s="78">
-        <f>BB6*concentration_constants!$B$6</f>
+      <c r="BH6" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI6" s="78">
+        <f>BG6*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE6" s="50">
+      <c r="BJ6" s="50">
         <f>I6*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.4178655483113793</v>
       </c>
-      <c r="BF6" s="50">
-        <f>BE6*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK6" s="50">
+        <f>BJ6*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32842371830361955</v>
       </c>
-      <c r="BG6" s="50">
-        <f t="shared" ref="BG6:BG17" si="16">BE6/BD6</f>
+      <c r="BL6" s="50">
+        <f t="shared" ref="BL6:BL17" si="16">BJ6/BI6</f>
         <v>15.90211572158638</v>
       </c>
-      <c r="BH6" s="50">
-        <f t="shared" ref="BH6:BH17" si="17">BF6/BD6</f>
+      <c r="BM6" s="50">
+        <f t="shared" ref="BM6:BM17" si="17">BK6/BI6</f>
         <v>2.1600175319199595</v>
       </c>
     </row>
-    <row r="7" spans="1:60" ht="17" thickBot="1">
+    <row r="7" spans="1:65" ht="17" thickBot="1">
       <c r="A7">
         <v>201205</v>
       </c>
@@ -4932,74 +5014,86 @@
         <f t="shared" si="9"/>
         <v>2.0917613635465034E-3</v>
       </c>
-      <c r="AO7" s="56">
+      <c r="AO7" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP7" s="57">
+      <c r="AQ7" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ7" s="47">
+      <c r="AR7" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR7" t="str">
+      <c r="AS7" t="str">
         <f t="shared" si="11"/>
         <v>S2_ref_2</v>
       </c>
-      <c r="AS7" s="50">
+      <c r="AT7" s="50">
+        <v>-3.5713502434924198</v>
+      </c>
+      <c r="AU7" s="50">
+        <v>18.090066846573698</v>
+      </c>
+      <c r="AV7" s="50">
+        <v>35.355596284351698</v>
+      </c>
+      <c r="AX7" s="50">
         <v>6.6566362138331598</v>
       </c>
-      <c r="AT7" s="50">
+      <c r="AY7" s="50">
         <v>-13.8026489120794</v>
       </c>
-      <c r="AU7" s="50">
+      <c r="AZ7" s="50">
         <v>20.459285125912601</v>
       </c>
-      <c r="AV7" s="50">
+      <c r="BA7" s="50">
         <v>-3.5730063491231601</v>
       </c>
-      <c r="AW7" s="50">
+      <c r="BB7" s="50">
         <v>17.941820061995799</v>
       </c>
-      <c r="AX7" s="50">
+      <c r="BC7" s="50">
         <v>35.063444020270097</v>
       </c>
-      <c r="AY7" s="44"/>
-      <c r="AZ7">
+      <c r="BD7" s="44"/>
+      <c r="BE7">
         <v>265</v>
       </c>
-      <c r="BA7">
+      <c r="BF7">
         <v>109</v>
       </c>
-      <c r="BB7">
+      <c r="BG7">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BH7" t="s">
         <v>39</v>
       </c>
-      <c r="BD7" s="78">
-        <f>BB7*concentration_constants!$F$6</f>
+      <c r="BI7" s="78">
+        <f>BG7*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE7" s="50">
+      <c r="BJ7" s="50">
         <f>I7*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>17.089981869851989</v>
       </c>
-      <c r="BF7" s="50">
-        <f>BE7*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK7" s="50">
+        <f>BJ7*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.44607485704311811</v>
       </c>
-      <c r="BG7" s="50">
+      <c r="BL7" s="50">
         <f t="shared" si="16"/>
         <v>109.35397373388625</v>
       </c>
-      <c r="BH7" s="50">
+      <c r="BM7" s="50">
         <f t="shared" si="17"/>
         <v>2.8543071942335927</v>
       </c>
     </row>
-    <row r="8" spans="1:60" ht="17" thickBot="1">
+    <row r="8" spans="1:65" ht="17" thickBot="1">
       <c r="A8">
         <v>201205</v>
       </c>
@@ -5106,74 +5200,86 @@
         <f t="shared" si="9"/>
         <v>2.1059970799231576E-3</v>
       </c>
-      <c r="AO8" s="56">
+      <c r="AO8" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP8" s="57">
+      <c r="AQ8" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ8" s="47">
+      <c r="AR8" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR8" t="str">
+      <c r="AS8" t="str">
         <f t="shared" si="11"/>
         <v>B6_ref_2</v>
       </c>
-      <c r="AS8" s="50">
+      <c r="AT8" s="50">
+        <v>-0.94152706968220201</v>
+      </c>
+      <c r="AU8" s="50">
+        <v>21.732150005308199</v>
+      </c>
+      <c r="AV8" s="50">
+        <v>42.5456389567846</v>
+      </c>
+      <c r="AX8" s="50">
         <v>-1.15628904358433</v>
       </c>
-      <c r="AT8" s="50">
+      <c r="AY8" s="50">
         <v>-0.70441124849329695</v>
       </c>
-      <c r="AU8" s="50">
+      <c r="AZ8" s="50">
         <v>-0.45187779509103798</v>
       </c>
-      <c r="AV8" s="50">
+      <c r="BA8" s="50">
         <v>-0.93035014603881605</v>
       </c>
-      <c r="AW8" s="50">
+      <c r="BB8" s="50">
         <v>21.5157968077277</v>
       </c>
-      <c r="AX8" s="50">
+      <c r="BC8" s="50">
         <v>42.117851051899301</v>
       </c>
-      <c r="AY8" s="44"/>
-      <c r="AZ8">
+      <c r="BD8" s="44"/>
+      <c r="BE8">
         <v>265</v>
       </c>
-      <c r="BA8">
+      <c r="BF8">
         <v>109</v>
       </c>
-      <c r="BB8">
+      <c r="BG8">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC8" t="s">
+      <c r="BH8" t="s">
         <v>39</v>
       </c>
-      <c r="BD8" s="78">
-        <f>BB8*concentration_constants!$F$6</f>
+      <c r="BI8" s="78">
+        <f>BG8*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE8" s="50">
+      <c r="BJ8" s="50">
         <f>I8*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.8350681459275666</v>
       </c>
-      <c r="BF8" s="50">
-        <f>BE8*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK8" s="50">
+        <f>BJ8*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.387899959681965</v>
       </c>
-      <c r="BG8" s="50">
+      <c r="BL8" s="50">
         <f t="shared" si="16"/>
         <v>62.931827072210872</v>
       </c>
-      <c r="BH8" s="50">
+      <c r="BM8" s="50">
         <f t="shared" si="17"/>
         <v>2.4820624343239581</v>
       </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:65">
       <c r="A9">
         <v>201205</v>
       </c>
@@ -5236,7 +5342,7 @@
         <v>0.42850050000000001</v>
       </c>
       <c r="X9" s="71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y9" s="3"/>
       <c r="AA9" s="28">
@@ -5283,73 +5389,85 @@
         <f t="shared" si="9"/>
         <v>2.1125489546459449E-3</v>
       </c>
-      <c r="AO9" s="56">
+      <c r="AO9" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP9" s="57">
+      <c r="AQ9" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ9" s="47">
+      <c r="AR9" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR9" s="41" t="str">
+      <c r="AS9" s="41" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="AS9" s="50">
+      <c r="AT9" s="50">
+        <v>5.57244533353684</v>
+      </c>
+      <c r="AU9" s="50">
+        <v>23.366934635269601</v>
+      </c>
+      <c r="AV9" s="50">
+        <v>45.7807904317755</v>
+      </c>
+      <c r="AX9" s="50">
         <v>16.036656468840999</v>
       </c>
-      <c r="AT9" s="50">
+      <c r="AY9" s="50">
         <v>-4.8656873390863202</v>
       </c>
-      <c r="AU9" s="50">
+      <c r="AZ9" s="50">
         <v>20.902343807927299</v>
       </c>
-      <c r="AV9" s="50">
+      <c r="BA9" s="50">
         <v>5.5854845648773397</v>
       </c>
-      <c r="AW9" s="50">
+      <c r="BB9" s="50">
         <v>23.117269398744899</v>
       </c>
-      <c r="AX9" s="50">
+      <c r="BC9" s="50">
         <v>45.286402388126902</v>
       </c>
-      <c r="AZ9">
+      <c r="BE9">
         <v>265</v>
       </c>
-      <c r="BA9">
+      <c r="BF9">
         <v>109</v>
       </c>
-      <c r="BB9">
+      <c r="BG9">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC9" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD9" s="78">
-        <f>BB9*concentration_constants!$B$6</f>
+      <c r="BH9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI9" s="78">
+        <f>BG9*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE9" s="50">
+      <c r="BJ9" s="50">
         <f>I9*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.4132419336762863</v>
       </c>
-      <c r="BF9" s="50">
-        <f>BE9*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK9" s="50">
+        <f>BJ9*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32838664297549441</v>
       </c>
-      <c r="BG9" s="50">
+      <c r="BL9" s="50">
         <f t="shared" si="16"/>
         <v>15.871706563794037</v>
       </c>
-      <c r="BH9" s="50">
+      <c r="BM9" s="50">
         <f t="shared" si="17"/>
         <v>2.1597736903388287</v>
       </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:65">
       <c r="A10">
         <v>201205</v>
       </c>
@@ -5457,73 +5575,85 @@
         <f t="shared" si="9"/>
         <v>2.1110245425008428E-3</v>
       </c>
-      <c r="AO10" s="56">
+      <c r="AO10" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP10" s="57">
+      <c r="AQ10" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ10" s="47">
+      <c r="AR10" s="47">
         <f t="shared" si="10"/>
         <v>201205</v>
       </c>
-      <c r="AR10" t="str">
+      <c r="AS10" t="str">
         <f t="shared" si="11"/>
         <v>DI</v>
       </c>
-      <c r="AS10" s="50">
+      <c r="AT10" s="50">
+        <v>-10.0998672074388</v>
+      </c>
+      <c r="AU10" s="50">
+        <v>23.078452800784302</v>
+      </c>
+      <c r="AV10" s="50">
+        <v>45.209547777639301</v>
+      </c>
+      <c r="AX10" s="50">
         <v>14.4579715364672</v>
       </c>
-      <c r="AT10" s="50">
+      <c r="AY10" s="50">
         <v>-34.815304667159701</v>
       </c>
-      <c r="AU10" s="50">
+      <c r="AZ10" s="50">
         <v>49.273276203626899</v>
       </c>
-      <c r="AV10" s="50">
+      <c r="BA10" s="50">
         <v>-10.1786665653462</v>
       </c>
-      <c r="AW10" s="50">
+      <c r="BB10" s="50">
         <v>22.853627356464699</v>
       </c>
-      <c r="AX10" s="50">
+      <c r="BC10" s="50">
         <v>44.764460247631298</v>
       </c>
-      <c r="AZ10">
+      <c r="BE10">
         <v>265</v>
       </c>
-      <c r="BA10">
+      <c r="BF10">
         <v>109</v>
       </c>
-      <c r="BB10">
+      <c r="BG10">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC10" t="s">
+      <c r="BH10" t="s">
         <v>39</v>
       </c>
-      <c r="BD10" s="78">
-        <f>BB10*concentration_constants!$F$6</f>
+      <c r="BI10" s="78">
+        <f>BG10*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE10" s="50">
+      <c r="BJ10" s="50">
         <f>I10*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>7.9745256167661447</v>
       </c>
-      <c r="BF10" s="50">
-        <f>BE10*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK10" s="50">
+        <f>BJ10*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.3729808476444097</v>
       </c>
-      <c r="BG10" s="50">
+      <c r="BL10" s="50">
         <f t="shared" si="16"/>
         <v>51.026740196512598</v>
       </c>
-      <c r="BH10" s="50">
+      <c r="BM10" s="50">
         <f t="shared" si="17"/>
         <v>2.386599244350319</v>
       </c>
     </row>
-    <row r="11" spans="1:60" ht="17" thickBot="1">
+    <row r="11" spans="1:65" ht="17" thickBot="1">
       <c r="A11">
         <v>201207</v>
       </c>
@@ -5637,73 +5767,85 @@
         <f t="shared" si="9"/>
         <v>2.11205838421125E-3</v>
       </c>
-      <c r="AO11" s="56">
+      <c r="AO11" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP11" s="57">
+      <c r="AQ11" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ11" s="47">
+      <c r="AR11" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR11" s="41" t="str">
+      <c r="AS11" s="41" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_1</v>
       </c>
-      <c r="AS11" s="50">
+      <c r="AT11" s="50">
+        <v>6.2757163469961901</v>
+      </c>
+      <c r="AU11" s="50">
+        <v>23.235402273854501</v>
+      </c>
+      <c r="AV11" s="50">
+        <v>45.520315450628203</v>
+      </c>
+      <c r="AX11" s="50">
         <v>17.1518234709566</v>
       </c>
-      <c r="AT11" s="50">
+      <c r="AY11" s="50">
         <v>-4.5745335204508901</v>
       </c>
-      <c r="AU11" s="50">
+      <c r="AZ11" s="50">
         <v>21.726356991407499</v>
       </c>
-      <c r="AV11" s="50">
+      <c r="BA11" s="50">
         <v>6.2886449752528799</v>
       </c>
-      <c r="AW11" s="50">
+      <c r="BB11" s="50">
         <v>22.988533215933799</v>
       </c>
-      <c r="AX11" s="50">
+      <c r="BC11" s="50">
         <v>45.031522726332703</v>
       </c>
-      <c r="AZ11">
+      <c r="BE11">
         <v>265</v>
       </c>
-      <c r="BA11">
+      <c r="BF11">
         <v>109</v>
       </c>
-      <c r="BB11">
+      <c r="BG11">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC11" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD11" s="78">
-        <f>BB11*concentration_constants!$B$6</f>
+      <c r="BH11" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI11" s="78">
+        <f>BG11*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE11" s="50">
+      <c r="BJ11" s="50">
         <f>I11*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.2611250121817261</v>
       </c>
-      <c r="BF11" s="50">
-        <f>BE11*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK11" s="50">
+        <f>BJ11*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32716686468017736</v>
       </c>
-      <c r="BG11" s="50">
+      <c r="BL11" s="50">
         <f t="shared" si="16"/>
         <v>14.871245272425968</v>
       </c>
-      <c r="BH11" s="50">
+      <c r="BM11" s="50">
         <f t="shared" si="17"/>
         <v>2.151751302319628</v>
       </c>
     </row>
-    <row r="12" spans="1:60">
+    <row r="12" spans="1:65">
       <c r="A12">
         <v>201207</v>
       </c>
@@ -5809,73 +5951,85 @@
         <f t="shared" si="9"/>
         <v>2.0890378267892978E-3</v>
       </c>
-      <c r="AO12" s="56">
+      <c r="AO12" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP12" s="57">
+      <c r="AQ12" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ12" s="47">
+      <c r="AR12" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR12" s="41" t="str">
+      <c r="AS12" s="41" t="str">
         <f t="shared" si="11"/>
         <v>S2_ref_1</v>
       </c>
-      <c r="AS12" s="50">
+      <c r="AT12" s="50">
+        <v>-3.7789086077021299</v>
+      </c>
+      <c r="AU12" s="50">
+        <v>17.3910621684267</v>
+      </c>
+      <c r="AV12" s="50">
+        <v>33.978406326581499</v>
+      </c>
+      <c r="AX12" s="50">
         <v>7.0098620813652204</v>
       </c>
-      <c r="AT12" s="50">
+      <c r="AY12" s="50">
         <v>-14.5751415214816</v>
       </c>
-      <c r="AU12" s="50">
+      <c r="AZ12" s="50">
         <v>21.5850036028468</v>
       </c>
-      <c r="AV12" s="50">
+      <c r="BA12" s="50">
         <v>-3.78263972005821</v>
       </c>
-      <c r="AW12" s="50">
+      <c r="BB12" s="50">
         <v>17.254451999306699</v>
       </c>
-      <c r="AX12" s="50">
+      <c r="BC12" s="50">
         <v>33.709358475152598</v>
       </c>
-      <c r="AZ12">
+      <c r="BE12">
         <v>265</v>
       </c>
-      <c r="BA12">
+      <c r="BF12">
         <v>109</v>
       </c>
-      <c r="BB12">
+      <c r="BG12">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC12" t="s">
+      <c r="BH12" t="s">
         <v>39</v>
       </c>
-      <c r="BD12" s="78">
-        <f>BB12*concentration_constants!$F$6</f>
+      <c r="BI12" s="78">
+        <f>BG12*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE12" s="50">
+      <c r="BJ12" s="50">
         <f>I12*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.6625426080784145</v>
       </c>
-      <c r="BF12" s="50">
-        <f>BE12*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK12" s="50">
+        <f>BJ12*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.33840439663490651</v>
       </c>
-      <c r="BG12" s="50">
+      <c r="BL12" s="50">
         <f t="shared" si="16"/>
         <v>23.435577124255598</v>
       </c>
-      <c r="BH12" s="50">
+      <c r="BM12" s="50">
         <f t="shared" si="17"/>
         <v>2.1653542866728439</v>
       </c>
     </row>
-    <row r="13" spans="1:60">
+    <row r="13" spans="1:65">
       <c r="A13">
         <v>201207</v>
       </c>
@@ -5981,73 +6135,85 @@
         <f t="shared" si="9"/>
         <v>2.1092446228371492E-3</v>
       </c>
-      <c r="AO13" s="56">
+      <c r="AO13" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP13" s="57">
+      <c r="AQ13" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ13" s="47">
+      <c r="AR13" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR13" s="41" t="str">
+      <c r="AS13" s="41" t="str">
         <f t="shared" si="11"/>
         <v>B6_ref_1</v>
       </c>
-      <c r="AS13" s="50">
+      <c r="AT13" s="50">
+        <v>0.13959532425555901</v>
+      </c>
+      <c r="AU13" s="50">
+        <v>22.5589202485119</v>
+      </c>
+      <c r="AV13" s="50">
+        <v>44.181166769186902</v>
+      </c>
+      <c r="AX13" s="50">
         <v>8.2241945278393999E-2</v>
       </c>
-      <c r="AT13" s="50">
+      <c r="AY13" s="50">
         <v>0.22102332359041901</v>
       </c>
-      <c r="AU13" s="50">
+      <c r="AZ13" s="50">
         <v>-0.138781378312025</v>
       </c>
-      <c r="AV13" s="50">
+      <c r="BA13" s="50">
         <v>0.151632634434406</v>
       </c>
-      <c r="AW13" s="50">
+      <c r="BB13" s="50">
         <v>22.3259423648012</v>
       </c>
-      <c r="AX13" s="50">
+      <c r="BC13" s="50">
         <v>43.720161276728597</v>
       </c>
-      <c r="AZ13">
+      <c r="BE13">
         <v>265</v>
       </c>
-      <c r="BA13">
+      <c r="BF13">
         <v>109</v>
       </c>
-      <c r="BB13">
+      <c r="BG13">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC13" t="s">
+      <c r="BH13" t="s">
         <v>39</v>
       </c>
-      <c r="BD13" s="78">
-        <f>BB13*concentration_constants!$F$6</f>
+      <c r="BI13" s="78">
+        <f>BG13*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE13" s="50">
+      <c r="BJ13" s="50">
         <f>I13*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>9.6085110288080102</v>
       </c>
-      <c r="BF13" s="50">
-        <f>BE13*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK13" s="50">
+        <f>BJ13*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.38608326860383324</v>
       </c>
-      <c r="BG13" s="50">
+      <c r="BL13" s="50">
         <f t="shared" si="16"/>
         <v>61.482151980488176</v>
       </c>
-      <c r="BH13" s="50">
+      <c r="BM13" s="50">
         <f t="shared" si="17"/>
         <v>2.4704379405150405</v>
       </c>
     </row>
-    <row r="14" spans="1:60">
+    <row r="14" spans="1:65">
       <c r="A14">
         <v>201207</v>
       </c>
@@ -6153,73 +6319,85 @@
         <f t="shared" si="9"/>
         <v>2.1118562233900973E-3</v>
       </c>
-      <c r="AO14" s="56">
+      <c r="AO14" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP14" s="57">
+      <c r="AQ14" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ14" s="47">
+      <c r="AR14" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR14" s="41" t="str">
+      <c r="AS14" s="41" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_2</v>
       </c>
-      <c r="AS14" s="50">
+      <c r="AT14" s="50">
+        <v>5.3435875779892497</v>
+      </c>
+      <c r="AU14" s="50">
+        <v>23.190561718908899</v>
+      </c>
+      <c r="AV14" s="50">
+        <v>45.431524384704502</v>
+      </c>
+      <c r="AX14" s="50">
         <v>14.393773542834699</v>
       </c>
-      <c r="AT14" s="50">
+      <c r="AY14" s="50">
         <v>-3.6809189289388402</v>
       </c>
-      <c r="AU14" s="50">
+      <c r="AZ14" s="50">
         <v>18.074692471773599</v>
       </c>
-      <c r="AV14" s="50">
+      <c r="BA14" s="50">
         <v>5.3564273069479604</v>
       </c>
-      <c r="AW14" s="50">
+      <c r="BB14" s="50">
         <v>22.94455532836</v>
       </c>
-      <c r="AX14" s="50">
+      <c r="BC14" s="50">
         <v>44.944459545090702</v>
       </c>
-      <c r="AZ14">
+      <c r="BE14">
         <v>265</v>
       </c>
-      <c r="BA14">
+      <c r="BF14">
         <v>109</v>
       </c>
-      <c r="BB14">
+      <c r="BG14">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC14" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD14" s="78">
-        <f>BB14*concentration_constants!$B$6</f>
+      <c r="BH14" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI14" s="78">
+        <f>BG14*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE14" s="50">
+      <c r="BJ14" s="50">
         <f>I14*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.3526725819565679</v>
       </c>
-      <c r="BF14" s="50">
-        <f>BE14*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK14" s="50">
+        <f>BJ14*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.32790095617705511</v>
       </c>
-      <c r="BG14" s="50">
+      <c r="BL14" s="50">
         <f t="shared" si="16"/>
         <v>15.473346596714352</v>
       </c>
-      <c r="BH14" s="50">
+      <c r="BM14" s="50">
         <f t="shared" si="17"/>
         <v>2.1565793656260164</v>
       </c>
     </row>
-    <row r="15" spans="1:60">
+    <row r="15" spans="1:65">
       <c r="A15">
         <v>201207</v>
       </c>
@@ -6325,73 +6503,85 @@
         <f t="shared" si="9"/>
         <v>2.1140383039962136E-3</v>
       </c>
-      <c r="AO15" s="56">
+      <c r="AO15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP15" s="57">
+      <c r="AQ15" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ15" s="47">
+      <c r="AR15" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR15" t="str">
+      <c r="AS15" t="str">
         <f t="shared" si="11"/>
         <v>ATM_EQ_SW_3</v>
       </c>
-      <c r="AS15" s="50">
+      <c r="AT15" s="50">
+        <v>6.1596227211071497</v>
+      </c>
+      <c r="AU15" s="50">
+        <v>23.745401762334801</v>
+      </c>
+      <c r="AV15" s="50">
+        <v>46.530448225756899</v>
+      </c>
+      <c r="AX15" s="50">
         <v>16.679833428360201</v>
       </c>
-      <c r="AT15" s="50">
+      <c r="AY15" s="50">
         <v>-4.3336183513273898</v>
       </c>
-      <c r="AU15" s="50">
+      <c r="AZ15" s="50">
         <v>21.0134517796876</v>
       </c>
-      <c r="AV15" s="50">
+      <c r="BA15" s="50">
         <v>6.1731075385164003</v>
       </c>
-      <c r="AW15" s="50">
+      <c r="BB15" s="50">
         <v>23.487665779901398</v>
       </c>
-      <c r="AX15" s="50">
+      <c r="BC15" s="50">
         <v>46.019903286484897</v>
       </c>
-      <c r="AZ15">
+      <c r="BE15">
         <v>265</v>
       </c>
-      <c r="BA15">
+      <c r="BF15">
         <v>109</v>
       </c>
-      <c r="BB15">
+      <c r="BG15">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC15" t="s">
-        <v>173</v>
-      </c>
-      <c r="BD15" s="78">
-        <f>BB15*concentration_constants!$B$6</f>
+      <c r="BH15" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI15" s="78">
+        <f>BG15*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
-      <c r="BE15" s="50">
+      <c r="BJ15" s="50">
         <f>I15*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>2.2375445775427525</v>
       </c>
-      <c r="BF15" s="50">
-        <f>BE15*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK15" s="50">
+        <f>BJ15*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.3269777805067392</v>
       </c>
-      <c r="BG15" s="50">
+      <c r="BL15" s="50">
         <f t="shared" si="16"/>
         <v>14.716158567685026</v>
       </c>
-      <c r="BH15" s="50">
+      <c r="BM15" s="50">
         <f t="shared" si="17"/>
         <v>2.1505077102558618</v>
       </c>
     </row>
-    <row r="16" spans="1:60">
+    <row r="16" spans="1:65">
       <c r="A16">
         <v>201207</v>
       </c>
@@ -6497,73 +6687,85 @@
         <f t="shared" si="9"/>
         <v>2.0909357320700551E-3</v>
       </c>
-      <c r="AO16" s="56">
+      <c r="AO16" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP16" s="57">
+      <c r="AQ16" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ16" s="47">
+      <c r="AR16" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR16" t="str">
+      <c r="AS16" t="str">
         <f t="shared" si="11"/>
         <v>S2_ref_2</v>
       </c>
-      <c r="AS16" s="50">
+      <c r="AT16" s="50">
+        <v>-3.8910374902335598</v>
+      </c>
+      <c r="AU16" s="50">
+        <v>17.879824476930899</v>
+      </c>
+      <c r="AV16" s="50">
+        <v>34.941280181798497</v>
+      </c>
+      <c r="AX16" s="50">
         <v>7.1029978910310803</v>
       </c>
-      <c r="AT16" s="50">
+      <c r="AY16" s="50">
         <v>-14.893050092214599</v>
       </c>
-      <c r="AU16" s="50">
+      <c r="AZ16" s="50">
         <v>21.996047983245699</v>
       </c>
-      <c r="AV16" s="50">
+      <c r="BA16" s="50">
         <v>-3.8950261005917799</v>
       </c>
-      <c r="AW16" s="50">
+      <c r="BB16" s="50">
         <v>17.735485742880101</v>
       </c>
-      <c r="AX16" s="50">
+      <c r="BC16" s="50">
         <v>34.656884164523802</v>
       </c>
-      <c r="AZ16">
+      <c r="BE16">
         <v>265</v>
       </c>
-      <c r="BA16">
+      <c r="BF16">
         <v>109</v>
       </c>
-      <c r="BB16">
+      <c r="BG16">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC16" t="s">
+      <c r="BH16" t="s">
         <v>39</v>
       </c>
-      <c r="BD16" s="78">
-        <f>BB16*concentration_constants!$F$6</f>
+      <c r="BI16" s="78">
+        <f>BG16*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE16" s="50">
+      <c r="BJ16" s="50">
         <f>I16*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>3.9394971247204844</v>
       </c>
-      <c r="BF16" s="50">
-        <f>BE16*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK16" s="50">
+        <f>BJ16*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.34062520878960229</v>
       </c>
-      <c r="BG16" s="50">
+      <c r="BL16" s="50">
         <f t="shared" si="16"/>
         <v>25.207730960871714</v>
       </c>
-      <c r="BH16" s="50">
+      <c r="BM16" s="50">
         <f t="shared" si="17"/>
         <v>2.179564637267827</v>
       </c>
     </row>
-    <row r="17" spans="1:60">
+    <row r="17" spans="1:65">
       <c r="A17">
         <v>201207</v>
       </c>
@@ -6665,73 +6867,85 @@
         <f t="shared" si="9"/>
         <v>2.1099653819650526E-3</v>
       </c>
-      <c r="AO17" s="56">
+      <c r="AO17" s="124">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="56">
         <v>0.18325645634287266</v>
       </c>
-      <c r="AP17" s="57">
+      <c r="AQ17" s="57">
         <v>9.0490249769565087E-2</v>
       </c>
-      <c r="AQ17" s="47">
+      <c r="AR17" s="47">
         <f t="shared" si="10"/>
         <v>201207</v>
       </c>
-      <c r="AR17" s="41" t="str">
+      <c r="AS17" s="41" t="str">
         <f t="shared" si="11"/>
         <v>DI</v>
       </c>
-      <c r="AS17" s="50">
+      <c r="AT17" s="50">
+        <v>-7.2725212903335104</v>
+      </c>
+      <c r="AU17" s="50">
+        <v>22.792929757643901</v>
+      </c>
+      <c r="AV17" s="50">
+        <v>44.644312779463498</v>
+      </c>
+      <c r="AX17" s="50">
         <v>13.725240315331099</v>
       </c>
-      <c r="AT17" s="50">
+      <c r="AY17" s="50">
         <v>-28.3353648321477</v>
       </c>
-      <c r="AU17" s="50">
+      <c r="AZ17" s="50">
         <v>42.060605147478803</v>
       </c>
-      <c r="AV17" s="50">
+      <c r="BA17" s="50">
         <v>-7.3050622584082596</v>
       </c>
-      <c r="AW17" s="50">
+      <c r="BB17" s="50">
         <v>22.565126816266901</v>
       </c>
-      <c r="AX17" s="50">
+      <c r="BC17" s="50">
         <v>44.193449376003002</v>
       </c>
-      <c r="AZ17">
+      <c r="BE17">
         <v>265</v>
       </c>
-      <c r="BA17">
+      <c r="BF17">
         <v>109</v>
       </c>
-      <c r="BB17">
+      <c r="BG17">
         <f t="shared" si="15"/>
         <v>156</v>
       </c>
-      <c r="BC17" t="s">
+      <c r="BH17" t="s">
         <v>39</v>
       </c>
-      <c r="BD17" s="78">
-        <f>BB17*concentration_constants!$F$6</f>
+      <c r="BI17" s="78">
+        <f>BG17*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
-      <c r="BE17" s="50">
+      <c r="BJ17" s="50">
         <f>I17*concentration_constants!$B$2+concentration_constants!$D$2</f>
         <v>6.3978730261994317</v>
       </c>
-      <c r="BF17" s="50">
-        <f>BE17*concentration_constants!$B$3+concentration_constants!$D$3</f>
+      <c r="BK17" s="50">
+        <f>BJ17*concentration_constants!$B$3+concentration_constants!$D$3</f>
         <v>0.36033816075373781</v>
       </c>
-      <c r="BG17" s="50">
+      <c r="BL17" s="50">
         <f t="shared" si="16"/>
         <v>40.938184966360723</v>
       </c>
-      <c r="BH17" s="50">
+      <c r="BM17" s="50">
         <f t="shared" si="17"/>
         <v>2.3057022568229555</v>
       </c>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:65">
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -6761,18 +6975,19 @@
       <c r="AL18" s="33"/>
       <c r="AM18" s="33"/>
       <c r="AN18" s="33"/>
-      <c r="AO18" s="56"/>
-      <c r="AP18" s="54"/>
-      <c r="AQ18" s="49"/>
-      <c r="AR18" s="48"/>
+      <c r="AO18" s="33"/>
+      <c r="AP18" s="56"/>
+      <c r="AQ18" s="54"/>
+      <c r="AR18" s="49"/>
       <c r="AS18" s="48"/>
-      <c r="AT18" s="48"/>
-      <c r="AU18" s="48"/>
-      <c r="AV18" s="48"/>
-      <c r="AW18" s="48"/>
       <c r="AX18" s="48"/>
-    </row>
-    <row r="19" spans="1:60">
+      <c r="AY18" s="48"/>
+      <c r="AZ18" s="48"/>
+      <c r="BA18" s="48"/>
+      <c r="BB18" s="48"/>
+      <c r="BC18" s="48"/>
+    </row>
+    <row r="19" spans="1:65">
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -6802,18 +7017,19 @@
       <c r="AL19" s="33"/>
       <c r="AM19" s="33"/>
       <c r="AN19" s="33"/>
-      <c r="AO19" s="56"/>
-      <c r="AP19" s="54"/>
-      <c r="AQ19" s="49"/>
-      <c r="AR19" s="48"/>
+      <c r="AO19" s="33"/>
+      <c r="AP19" s="56"/>
+      <c r="AQ19" s="54"/>
+      <c r="AR19" s="49"/>
       <c r="AS19" s="48"/>
-      <c r="AT19" s="48"/>
-      <c r="AU19" s="48"/>
-      <c r="AV19" s="48"/>
-      <c r="AW19" s="48"/>
       <c r="AX19" s="48"/>
-    </row>
-    <row r="20" spans="1:60">
+      <c r="AY19" s="48"/>
+      <c r="AZ19" s="48"/>
+      <c r="BA19" s="48"/>
+      <c r="BB19" s="48"/>
+      <c r="BC19" s="48"/>
+    </row>
+    <row r="20" spans="1:65">
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -6843,18 +7059,19 @@
       <c r="AL20" s="33"/>
       <c r="AM20" s="33"/>
       <c r="AN20" s="33"/>
-      <c r="AO20" s="56"/>
-      <c r="AP20" s="54"/>
-      <c r="AQ20" s="49"/>
-      <c r="AR20" s="48"/>
+      <c r="AO20" s="33"/>
+      <c r="AP20" s="56"/>
+      <c r="AQ20" s="54"/>
+      <c r="AR20" s="49"/>
       <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="48"/>
-      <c r="AV20" s="48"/>
-      <c r="AW20" s="48"/>
       <c r="AX20" s="48"/>
-    </row>
-    <row r="21" spans="1:60">
+      <c r="AY20" s="48"/>
+      <c r="AZ20" s="48"/>
+      <c r="BA20" s="48"/>
+      <c r="BB20" s="48"/>
+      <c r="BC20" s="48"/>
+    </row>
+    <row r="21" spans="1:65">
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -6884,18 +7101,19 @@
       <c r="AL21" s="33"/>
       <c r="AM21" s="33"/>
       <c r="AN21" s="33"/>
-      <c r="AO21" s="56"/>
-      <c r="AP21" s="54"/>
-      <c r="AQ21" s="49"/>
-      <c r="AR21" s="48"/>
+      <c r="AO21" s="33"/>
+      <c r="AP21" s="56"/>
+      <c r="AQ21" s="54"/>
+      <c r="AR21" s="49"/>
       <c r="AS21" s="48"/>
-      <c r="AT21" s="48"/>
-      <c r="AU21" s="48"/>
-      <c r="AV21" s="48"/>
-      <c r="AW21" s="48"/>
       <c r="AX21" s="48"/>
-    </row>
-    <row r="22" spans="1:60">
+      <c r="AY21" s="48"/>
+      <c r="AZ21" s="48"/>
+      <c r="BA21" s="48"/>
+      <c r="BB21" s="48"/>
+      <c r="BC21" s="48"/>
+    </row>
+    <row r="22" spans="1:65">
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -6925,18 +7143,19 @@
       <c r="AL22" s="33"/>
       <c r="AM22" s="33"/>
       <c r="AN22" s="33"/>
-      <c r="AO22" s="56"/>
-      <c r="AP22" s="54"/>
-      <c r="AQ22" s="49"/>
-      <c r="AR22" s="48"/>
+      <c r="AO22" s="33"/>
+      <c r="AP22" s="56"/>
+      <c r="AQ22" s="54"/>
+      <c r="AR22" s="49"/>
       <c r="AS22" s="48"/>
-      <c r="AT22" s="48"/>
-      <c r="AU22" s="48"/>
-      <c r="AV22" s="48"/>
-      <c r="AW22" s="48"/>
       <c r="AX22" s="48"/>
-    </row>
-    <row r="23" spans="1:60">
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="48"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48"/>
+    </row>
+    <row r="23" spans="1:65">
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -6966,18 +7185,19 @@
       <c r="AL23" s="33"/>
       <c r="AM23" s="33"/>
       <c r="AN23" s="33"/>
-      <c r="AO23" s="56"/>
-      <c r="AP23" s="54"/>
-      <c r="AQ23" s="49"/>
-      <c r="AR23" s="48"/>
+      <c r="AO23" s="33"/>
+      <c r="AP23" s="56"/>
+      <c r="AQ23" s="54"/>
+      <c r="AR23" s="49"/>
       <c r="AS23" s="48"/>
-      <c r="AT23" s="48"/>
-      <c r="AU23" s="48"/>
-      <c r="AV23" s="48"/>
-      <c r="AW23" s="48"/>
       <c r="AX23" s="48"/>
-    </row>
-    <row r="24" spans="1:60">
+      <c r="AY23" s="48"/>
+      <c r="AZ23" s="48"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="48"/>
+      <c r="BC23" s="48"/>
+    </row>
+    <row r="24" spans="1:65">
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -7007,18 +7227,19 @@
       <c r="AL24" s="33"/>
       <c r="AM24" s="33"/>
       <c r="AN24" s="33"/>
-      <c r="AO24" s="56"/>
-      <c r="AP24" s="54"/>
-      <c r="AQ24" s="49"/>
-      <c r="AR24" s="48"/>
+      <c r="AO24" s="33"/>
+      <c r="AP24" s="56"/>
+      <c r="AQ24" s="54"/>
+      <c r="AR24" s="49"/>
       <c r="AS24" s="48"/>
-      <c r="AT24" s="48"/>
-      <c r="AU24" s="48"/>
-      <c r="AV24" s="48"/>
-      <c r="AW24" s="48"/>
       <c r="AX24" s="48"/>
-    </row>
-    <row r="25" spans="1:60">
+      <c r="AY24" s="48"/>
+      <c r="AZ24" s="48"/>
+      <c r="BA24" s="48"/>
+      <c r="BB24" s="48"/>
+      <c r="BC24" s="48"/>
+    </row>
+    <row r="25" spans="1:65">
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
@@ -7048,18 +7269,19 @@
       <c r="AL25" s="33"/>
       <c r="AM25" s="33"/>
       <c r="AN25" s="33"/>
-      <c r="AO25" s="56"/>
-      <c r="AP25" s="54"/>
-      <c r="AQ25" s="49"/>
-      <c r="AR25" s="48"/>
+      <c r="AO25" s="33"/>
+      <c r="AP25" s="56"/>
+      <c r="AQ25" s="54"/>
+      <c r="AR25" s="49"/>
       <c r="AS25" s="48"/>
-      <c r="AT25" s="48"/>
-      <c r="AU25" s="48"/>
-      <c r="AV25" s="48"/>
-      <c r="AW25" s="48"/>
       <c r="AX25" s="48"/>
-    </row>
-    <row r="26" spans="1:60">
+      <c r="AY25" s="48"/>
+      <c r="AZ25" s="48"/>
+      <c r="BA25" s="48"/>
+      <c r="BB25" s="48"/>
+      <c r="BC25" s="48"/>
+    </row>
+    <row r="26" spans="1:65">
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
@@ -7089,18 +7311,19 @@
       <c r="AL26" s="33"/>
       <c r="AM26" s="33"/>
       <c r="AN26" s="33"/>
-      <c r="AO26" s="56"/>
-      <c r="AP26" s="54"/>
-      <c r="AQ26" s="49"/>
-      <c r="AR26" s="48"/>
+      <c r="AO26" s="33"/>
+      <c r="AP26" s="56"/>
+      <c r="AQ26" s="54"/>
+      <c r="AR26" s="49"/>
       <c r="AS26" s="48"/>
-      <c r="AT26" s="48"/>
-      <c r="AU26" s="48"/>
-      <c r="AV26" s="48"/>
-      <c r="AW26" s="48"/>
       <c r="AX26" s="48"/>
-    </row>
-    <row r="27" spans="1:60">
+      <c r="AY26" s="48"/>
+      <c r="AZ26" s="48"/>
+      <c r="BA26" s="48"/>
+      <c r="BB26" s="48"/>
+      <c r="BC26" s="48"/>
+    </row>
+    <row r="27" spans="1:65">
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
@@ -7130,18 +7353,19 @@
       <c r="AL27" s="33"/>
       <c r="AM27" s="33"/>
       <c r="AN27" s="33"/>
-      <c r="AO27" s="56"/>
-      <c r="AP27" s="54"/>
-      <c r="AQ27" s="49"/>
-      <c r="AR27" s="48"/>
+      <c r="AO27" s="33"/>
+      <c r="AP27" s="56"/>
+      <c r="AQ27" s="54"/>
+      <c r="AR27" s="49"/>
       <c r="AS27" s="48"/>
-      <c r="AT27" s="48"/>
-      <c r="AU27" s="48"/>
-      <c r="AV27" s="48"/>
-      <c r="AW27" s="48"/>
       <c r="AX27" s="48"/>
-    </row>
-    <row r="28" spans="1:60">
+      <c r="AY27" s="48"/>
+      <c r="AZ27" s="48"/>
+      <c r="BA27" s="48"/>
+      <c r="BB27" s="48"/>
+      <c r="BC27" s="48"/>
+    </row>
+    <row r="28" spans="1:65">
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
@@ -7171,18 +7395,19 @@
       <c r="AL28" s="33"/>
       <c r="AM28" s="33"/>
       <c r="AN28" s="33"/>
-      <c r="AO28" s="56"/>
-      <c r="AP28" s="54"/>
-      <c r="AQ28" s="49"/>
-      <c r="AR28" s="48"/>
+      <c r="AO28" s="33"/>
+      <c r="AP28" s="56"/>
+      <c r="AQ28" s="54"/>
+      <c r="AR28" s="49"/>
       <c r="AS28" s="48"/>
-      <c r="AT28" s="48"/>
-      <c r="AU28" s="48"/>
-      <c r="AV28" s="48"/>
-      <c r="AW28" s="48"/>
       <c r="AX28" s="48"/>
-    </row>
-    <row r="29" spans="1:60">
+      <c r="AY28" s="48"/>
+      <c r="AZ28" s="48"/>
+      <c r="BA28" s="48"/>
+      <c r="BB28" s="48"/>
+      <c r="BC28" s="48"/>
+    </row>
+    <row r="29" spans="1:65">
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
@@ -7212,18 +7437,19 @@
       <c r="AL29" s="33"/>
       <c r="AM29" s="33"/>
       <c r="AN29" s="33"/>
-      <c r="AO29" s="56"/>
-      <c r="AP29" s="54"/>
-      <c r="AQ29" s="49"/>
-      <c r="AR29" s="48"/>
+      <c r="AO29" s="33"/>
+      <c r="AP29" s="56"/>
+      <c r="AQ29" s="54"/>
+      <c r="AR29" s="49"/>
       <c r="AS29" s="48"/>
-      <c r="AT29" s="48"/>
-      <c r="AU29" s="48"/>
-      <c r="AV29" s="48"/>
-      <c r="AW29" s="48"/>
       <c r="AX29" s="48"/>
-    </row>
-    <row r="30" spans="1:60">
+      <c r="AY29" s="48"/>
+      <c r="AZ29" s="48"/>
+      <c r="BA29" s="48"/>
+      <c r="BB29" s="48"/>
+      <c r="BC29" s="48"/>
+    </row>
+    <row r="30" spans="1:65">
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
@@ -7253,18 +7479,19 @@
       <c r="AL30" s="33"/>
       <c r="AM30" s="33"/>
       <c r="AN30" s="33"/>
-      <c r="AO30" s="60"/>
-      <c r="AP30" s="32"/>
-      <c r="AQ30" s="49"/>
-      <c r="AR30" s="48"/>
-      <c r="AS30" s="45"/>
-      <c r="AT30" s="45"/>
-      <c r="AU30" s="45"/>
-      <c r="AV30" s="45"/>
-      <c r="AW30" s="45"/>
+      <c r="AO30" s="33"/>
+      <c r="AP30" s="60"/>
+      <c r="AQ30" s="32"/>
+      <c r="AR30" s="49"/>
+      <c r="AS30" s="48"/>
       <c r="AX30" s="45"/>
-    </row>
-    <row r="31" spans="1:60">
+      <c r="AY30" s="45"/>
+      <c r="AZ30" s="45"/>
+      <c r="BA30" s="45"/>
+      <c r="BB30" s="45"/>
+      <c r="BC30" s="45"/>
+    </row>
+    <row r="31" spans="1:65">
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -7294,16 +7521,17 @@
       <c r="AL31" s="33"/>
       <c r="AM31" s="33"/>
       <c r="AN31" s="33"/>
-      <c r="AQ31" s="49"/>
-      <c r="AR31" s="48"/>
-      <c r="AS31" s="45"/>
-      <c r="AT31" s="45"/>
-      <c r="AU31" s="45"/>
-      <c r="AV31" s="45"/>
-      <c r="AW31" s="45"/>
+      <c r="AO31" s="33"/>
+      <c r="AR31" s="49"/>
+      <c r="AS31" s="48"/>
       <c r="AX31" s="45"/>
-    </row>
-    <row r="32" spans="1:60">
+      <c r="AY31" s="45"/>
+      <c r="AZ31" s="45"/>
+      <c r="BA31" s="45"/>
+      <c r="BB31" s="45"/>
+      <c r="BC31" s="45"/>
+    </row>
+    <row r="32" spans="1:65">
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
@@ -7333,16 +7561,17 @@
       <c r="AL32" s="33"/>
       <c r="AM32" s="33"/>
       <c r="AN32" s="33"/>
-      <c r="AQ32" s="49"/>
-      <c r="AR32" s="48"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="45"/>
-      <c r="AU32" s="45"/>
-      <c r="AV32" s="45"/>
-      <c r="AW32" s="45"/>
+      <c r="AO32" s="33"/>
+      <c r="AR32" s="49"/>
+      <c r="AS32" s="48"/>
       <c r="AX32" s="45"/>
-    </row>
-    <row r="33" spans="3:50">
+      <c r="AY32" s="45"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="45"/>
+      <c r="BB32" s="45"/>
+      <c r="BC32" s="45"/>
+    </row>
+    <row r="33" spans="3:55">
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
@@ -7360,16 +7589,17 @@
       <c r="AL33" s="33"/>
       <c r="AM33" s="33"/>
       <c r="AN33" s="33"/>
-      <c r="AQ33" s="49"/>
-      <c r="AR33" s="48"/>
-      <c r="AS33" s="45"/>
-      <c r="AT33" s="45"/>
-      <c r="AU33" s="45"/>
-      <c r="AV33" s="45"/>
-      <c r="AW33" s="45"/>
+      <c r="AO33" s="33"/>
+      <c r="AR33" s="49"/>
+      <c r="AS33" s="48"/>
       <c r="AX33" s="45"/>
-    </row>
-    <row r="34" spans="3:50">
+      <c r="AY33" s="45"/>
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="45"/>
+      <c r="BB33" s="45"/>
+      <c r="BC33" s="45"/>
+    </row>
+    <row r="34" spans="3:55">
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
@@ -7387,16 +7617,17 @@
       <c r="AL34" s="33"/>
       <c r="AM34" s="33"/>
       <c r="AN34" s="33"/>
-      <c r="AQ34" s="49"/>
-      <c r="AR34" s="48"/>
-      <c r="AS34" s="45"/>
-      <c r="AT34" s="45"/>
-      <c r="AU34" s="45"/>
-      <c r="AV34" s="45"/>
-      <c r="AW34" s="45"/>
+      <c r="AO34" s="33"/>
+      <c r="AR34" s="49"/>
+      <c r="AS34" s="48"/>
       <c r="AX34" s="45"/>
-    </row>
-    <row r="35" spans="3:50">
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
+      <c r="BB34" s="45"/>
+      <c r="BC34" s="45"/>
+    </row>
+    <row r="35" spans="3:55">
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
@@ -7414,16 +7645,17 @@
       <c r="AL35" s="33"/>
       <c r="AM35" s="33"/>
       <c r="AN35" s="33"/>
-      <c r="AQ35" s="49"/>
-      <c r="AR35" s="48"/>
-      <c r="AS35" s="45"/>
-      <c r="AT35" s="45"/>
-      <c r="AU35" s="45"/>
-      <c r="AV35" s="45"/>
-      <c r="AW35" s="45"/>
+      <c r="AO35" s="33"/>
+      <c r="AR35" s="49"/>
+      <c r="AS35" s="48"/>
       <c r="AX35" s="45"/>
-    </row>
-    <row r="36" spans="3:50">
+      <c r="AY35" s="45"/>
+      <c r="AZ35" s="45"/>
+      <c r="BA35" s="45"/>
+      <c r="BB35" s="45"/>
+      <c r="BC35" s="45"/>
+    </row>
+    <row r="36" spans="3:55">
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -7453,16 +7685,17 @@
       <c r="AL36" s="33"/>
       <c r="AM36" s="33"/>
       <c r="AN36" s="33"/>
-      <c r="AQ36" s="49"/>
-      <c r="AR36" s="48"/>
-      <c r="AS36" s="45"/>
-      <c r="AT36" s="45"/>
-      <c r="AU36" s="45"/>
-      <c r="AV36" s="45"/>
-      <c r="AW36" s="45"/>
+      <c r="AO36" s="33"/>
+      <c r="AR36" s="49"/>
+      <c r="AS36" s="48"/>
       <c r="AX36" s="45"/>
-    </row>
-    <row r="37" spans="3:50">
+      <c r="AY36" s="45"/>
+      <c r="AZ36" s="45"/>
+      <c r="BA36" s="45"/>
+      <c r="BB36" s="45"/>
+      <c r="BC36" s="45"/>
+    </row>
+    <row r="37" spans="3:55">
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
@@ -7492,16 +7725,17 @@
       <c r="AL37" s="33"/>
       <c r="AM37" s="33"/>
       <c r="AN37" s="33"/>
-      <c r="AQ37" s="49"/>
-      <c r="AR37" s="48"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="45"/>
-      <c r="AU37" s="45"/>
-      <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
+      <c r="AO37" s="33"/>
+      <c r="AR37" s="49"/>
+      <c r="AS37" s="48"/>
       <c r="AX37" s="45"/>
-    </row>
-    <row r="38" spans="3:50">
+      <c r="AY37" s="45"/>
+      <c r="AZ37" s="45"/>
+      <c r="BA37" s="45"/>
+      <c r="BB37" s="45"/>
+      <c r="BC37" s="45"/>
+    </row>
+    <row r="38" spans="3:55">
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -7531,16 +7765,17 @@
       <c r="AL38" s="33"/>
       <c r="AM38" s="33"/>
       <c r="AN38" s="33"/>
-      <c r="AQ38" s="49"/>
-      <c r="AR38" s="48"/>
-      <c r="AS38" s="45"/>
-      <c r="AT38" s="45"/>
-      <c r="AU38" s="45"/>
-      <c r="AV38" s="45"/>
-      <c r="AW38" s="45"/>
+      <c r="AO38" s="33"/>
+      <c r="AR38" s="49"/>
+      <c r="AS38" s="48"/>
       <c r="AX38" s="45"/>
-    </row>
-    <row r="39" spans="3:50">
+      <c r="AY38" s="45"/>
+      <c r="AZ38" s="45"/>
+      <c r="BA38" s="45"/>
+      <c r="BB38" s="45"/>
+      <c r="BC38" s="45"/>
+    </row>
+    <row r="39" spans="3:55">
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
@@ -7570,57 +7805,58 @@
       <c r="AL39" s="33"/>
       <c r="AM39" s="33"/>
       <c r="AN39" s="33"/>
-      <c r="AQ39" s="49"/>
-      <c r="AR39" s="48"/>
-      <c r="AS39" s="45"/>
-      <c r="AT39" s="45"/>
-      <c r="AU39" s="45"/>
-      <c r="AV39" s="45"/>
-      <c r="AW39" s="45"/>
+      <c r="AO39" s="33"/>
+      <c r="AR39" s="49"/>
+      <c r="AS39" s="48"/>
       <c r="AX39" s="45"/>
-    </row>
-    <row r="40" spans="3:50">
+      <c r="AY39" s="45"/>
+      <c r="AZ39" s="45"/>
+      <c r="BA39" s="45"/>
+      <c r="BB39" s="45"/>
+      <c r="BC39" s="45"/>
+    </row>
+    <row r="40" spans="3:55">
       <c r="AA40" s="28"/>
       <c r="AI40" s="74"/>
       <c r="AJ40" s="74"/>
-      <c r="AQ40" s="45"/>
       <c r="AR40" s="45"/>
       <c r="AS40" s="45"/>
-      <c r="AT40" s="45"/>
-      <c r="AU40" s="45"/>
-      <c r="AV40" s="45"/>
-      <c r="AW40" s="45"/>
       <c r="AX40" s="45"/>
-    </row>
-    <row r="41" spans="3:50">
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="45"/>
+      <c r="BA40" s="45"/>
+      <c r="BB40" s="45"/>
+      <c r="BC40" s="45"/>
+    </row>
+    <row r="41" spans="3:55">
       <c r="AI41" s="74"/>
       <c r="AJ41" s="74"/>
     </row>
-    <row r="42" spans="3:50">
+    <row r="42" spans="3:55">
       <c r="AI42" s="74"/>
       <c r="AJ42" s="74"/>
     </row>
-    <row r="43" spans="3:50">
+    <row r="43" spans="3:55">
       <c r="AI43" s="74"/>
       <c r="AJ43" s="74"/>
     </row>
-    <row r="44" spans="3:50">
+    <row r="44" spans="3:55">
       <c r="AI44" s="74"/>
       <c r="AJ44" s="74"/>
     </row>
-    <row r="45" spans="3:50">
+    <row r="45" spans="3:55">
       <c r="AI45" s="74"/>
       <c r="AJ45" s="74"/>
     </row>
-    <row r="46" spans="3:50">
+    <row r="46" spans="3:55">
       <c r="AI46" s="74"/>
       <c r="AJ46" s="74"/>
     </row>
-    <row r="47" spans="3:50">
+    <row r="47" spans="3:55">
       <c r="AI47" s="74"/>
       <c r="AJ47" s="74"/>
     </row>
-    <row r="48" spans="3:50">
+    <row r="48" spans="3:55">
       <c r="AI48" s="74"/>
       <c r="AJ48" s="74"/>
     </row>
@@ -7650,6 +7886,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7658,7 +7895,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7683,26 +7920,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="124" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="125" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
+      <c r="A1" s="125" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="126" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
       <c r="O1" s="115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P1" s="116"/>
       <c r="Q1" s="115"/>
@@ -7727,28 +7964,28 @@
         <v>35</v>
       </c>
       <c r="G2" s="118" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="118" t="s">
+      <c r="I2" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="J2" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="118" t="s">
+      <c r="K2" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="118" t="s">
+      <c r="L2" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="118" t="s">
+      <c r="M2" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="118" t="s">
+      <c r="N2" s="118" t="s">
         <v>105</v>
-      </c>
-      <c r="N2" s="118" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -7915,7 +8152,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="68" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B6" s="69">
         <v>-22.21</v>
@@ -8023,7 +8260,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="68" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8" s="69">
         <v>17.11</v>
@@ -8146,7 +8383,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="114"/>
       <c r="B11" s="70" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="70"/>
       <c r="D11" s="114"/>
@@ -8162,10 +8399,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="63" t="s">
         <v>109</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>110</v>
       </c>
       <c r="D12" s="63" t="s">
         <v>26</v>
@@ -8174,22 +8411,22 @@
         <v>27</v>
       </c>
       <c r="F12" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="H12" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="I12" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="63" t="s">
-        <v>114</v>
-      </c>
       <c r="J12" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="41" t="s">
         <v>107</v>
-      </c>
-      <c r="K12" s="41" t="s">
-        <v>108</v>
       </c>
       <c r="M12" s="63"/>
       <c r="O12" s="63"/>
@@ -8843,7 +9080,7 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8857,16 +9094,16 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N1">
         <v>3.7990000000000002E-4</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
@@ -8875,10 +9112,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N2">
         <v>2.0052E-3</v>
@@ -8887,24 +9124,24 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="126" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="127" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
+      <c r="A3" s="127" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="127"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="128" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
       <c r="M3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N3">
         <v>0.51600000000000001</v>
@@ -8914,58 +9151,58 @@
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="113" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="113" t="s">
+        <v>141</v>
+      </c>
+      <c r="M4" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="N4" s="113" t="s">
+        <v>142</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="113" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L4" s="113" t="s">
-        <v>143</v>
-      </c>
-      <c r="M4" s="113" t="s">
-        <v>141</v>
-      </c>
-      <c r="N4" s="113" t="s">
-        <v>144</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="Q4" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="113" t="s">
         <v>95</v>
-      </c>
-      <c r="R4" s="113" t="s">
-        <v>96</v>
       </c>
       <c r="V4" s="113"/>
       <c r="Y4" s="113"/>
@@ -9453,7 +9690,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -9464,28 +9701,28 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B2" s="81">
         <f>B12</f>
         <v>0.4623614635092998</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="81">
         <f>C12</f>
         <v>0.10975712247295455</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G2" s="50">
         <f>1/B2</f>
         <v>2.1628100067208269</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L2" s="80"/>
       <c r="M2" s="80"/>
@@ -9494,7 +9731,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B3" s="81">
         <f>B13</f>
@@ -9512,20 +9749,20 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="81">
         <v>1.026</v>
       </c>
       <c r="C4" s="79"/>
       <c r="E4" s="79" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4">
         <v>0.99819999999999998</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I4">
         <v>1.002</v>
@@ -9539,7 +9776,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="85">
         <f>1/B4</f>
@@ -9547,14 +9784,14 @@
       </c>
       <c r="C5" s="79"/>
       <c r="E5" s="79" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5" s="85">
         <f>1/F4</f>
         <v>1.0018032458425166</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I5" s="85">
         <f>1/I4</f>
@@ -9570,7 +9807,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" s="88">
         <f>B5/1000</f>
@@ -9578,14 +9815,14 @@
       </c>
       <c r="C6" s="79"/>
       <c r="E6" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F6" s="88">
         <f>F5/1000</f>
         <v>1.0018032458425166E-3</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I6" s="88">
         <f>I5/1000</f>
@@ -9614,7 +9851,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="93" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" s="93"/>
       <c r="C10" s="93"/>
@@ -9628,10 +9865,10 @@
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="24"/>
@@ -9650,7 +9887,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13">
         <v>8.0186890671505306E-3</v>

</xml_diff>

<commit_message>
fix typos in README
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE88AA59-F3FC-9D4E-B625-BBC33787148B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45135908-E6B2-DE47-8D70-9D83191D56CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37200" yWindow="-5500" windowWidth="20420" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -3863,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AU26" sqref="AU26"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7895,7 +7895,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
update axis titles on template
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45135908-E6B2-DE47-8D70-9D83191D56CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2ED6DB-7243-E345-98E0-41F48718910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="20420" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="37200" windowHeight="21780" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -1383,6 +1383,10 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1395,10 +1399,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -2234,6 +2234,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ln(size corrected 46rR/46rR)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2282,6 +2342,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ln(known 46rR/46rR)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3863,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3923,11 +4043,11 @@
       <c r="AP1" s="58"/>
       <c r="AQ1" s="51"/>
       <c r="AR1" s="45"/>
-      <c r="AT1" s="129" t="s">
+      <c r="AT1" s="125" t="s">
         <v>181</v>
       </c>
-      <c r="AU1" s="129"/>
-      <c r="AV1" s="129"/>
+      <c r="AU1" s="125"/>
+      <c r="AV1" s="125"/>
       <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
@@ -4075,13 +4195,13 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="130" t="s">
+      <c r="AT2" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="131" t="s">
+      <c r="AU2" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="132" t="s">
+      <c r="AV2" s="128" t="s">
         <v>34</v>
       </c>
       <c r="AX2" s="39" t="s">
@@ -7894,8 +8014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7920,24 +8040,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="129" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="126" t="s">
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
       <c r="O1" s="115" t="s">
         <v>114</v>
       </c>
@@ -9124,22 +9244,22 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="131" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="128" t="s">
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="132" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
       <c r="M3" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
trying to figure out how to reset, no idea what i'm doing
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45135908-E6B2-DE47-8D70-9D83191D56CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2ED6DB-7243-E345-98E0-41F48718910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="20420" windowHeight="15820" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="37200" windowHeight="21780" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -1383,6 +1383,10 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1395,10 +1399,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -2234,6 +2234,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ln(size corrected 46rR/46rR)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2282,6 +2342,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ln(known 46rR/46rR)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3863,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3923,11 +4043,11 @@
       <c r="AP1" s="58"/>
       <c r="AQ1" s="51"/>
       <c r="AR1" s="45"/>
-      <c r="AT1" s="129" t="s">
+      <c r="AT1" s="125" t="s">
         <v>181</v>
       </c>
-      <c r="AU1" s="129"/>
-      <c r="AV1" s="129"/>
+      <c r="AU1" s="125"/>
+      <c r="AV1" s="125"/>
       <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
@@ -4075,13 +4195,13 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="130" t="s">
+      <c r="AT2" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="131" t="s">
+      <c r="AU2" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="132" t="s">
+      <c r="AV2" s="128" t="s">
         <v>34</v>
       </c>
       <c r="AX2" s="39" t="s">
@@ -7894,8 +8014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7920,24 +8040,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="129" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="126" t="s">
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
       <c r="O1" s="115" t="s">
         <v>114</v>
       </c>
@@ -9124,22 +9244,22 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="131" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="128" t="s">
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="132" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
       <c r="M3" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
add linearity correction template and notebook
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2ED6DB-7243-E345-98E0-41F48718910E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D4EF05-02C8-404E-A2BE-E63A68E3B500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="-5500" windowWidth="37200" windowHeight="21780" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -3983,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AQ12" sqref="AQ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4394,22 +4394,22 @@
         <v>47.588174908592201</v>
       </c>
       <c r="AX3" s="50">
-        <v>15.105455486877901</v>
+        <v>15.105455490000001</v>
       </c>
       <c r="AY3" s="50">
-        <v>-2.7098456777153701</v>
+        <v>-2.7098456780000002</v>
       </c>
       <c r="AZ3" s="50">
-        <v>17.815301164593201</v>
+        <v>17.815301160000001</v>
       </c>
       <c r="BA3" s="50">
-        <v>6.19780490458127</v>
+        <v>6.1978049049999999</v>
       </c>
       <c r="BB3" s="50">
-        <v>24.009727067820499</v>
+        <v>24.00972707</v>
       </c>
       <c r="BC3" s="50">
-        <v>47.054171086232202</v>
+        <v>47.054171089999997</v>
       </c>
       <c r="BD3" s="44"/>
       <c r="BE3">
@@ -4580,22 +4580,22 @@
         <v>35.169038165624201</v>
       </c>
       <c r="AX4" s="50">
-        <v>6.8736240880515798</v>
+        <v>6.8736240879999997</v>
       </c>
       <c r="AY4" s="50">
-        <v>-13.881471917271901</v>
+        <v>-13.881471919999999</v>
       </c>
       <c r="AZ4" s="50">
-        <v>20.755096005323502</v>
+        <v>20.755096009999999</v>
       </c>
       <c r="BA4" s="50">
-        <v>-3.5039239146101799</v>
+        <v>-3.5039239150000001</v>
       </c>
       <c r="BB4" s="50">
-        <v>17.848649659933699</v>
+        <v>17.84864966</v>
       </c>
       <c r="BC4" s="50">
-        <v>34.879852068524698</v>
+        <v>34.879852069999998</v>
       </c>
       <c r="BD4" s="44"/>
       <c r="BE4">
@@ -4771,22 +4771,22 @@
         <v>44.4548477102446</v>
       </c>
       <c r="AX5" s="50">
-        <v>-0.53970856962448599</v>
+        <v>-0.53970856960000002</v>
       </c>
       <c r="AY5" s="50">
-        <v>1.2825215740412901</v>
+        <v>1.282521574</v>
       </c>
       <c r="AZ5" s="50">
-        <v>-1.82223014366578</v>
+        <v>-1.8222301439999999</v>
       </c>
       <c r="BA5" s="50">
-        <v>0.37140650220840399</v>
+        <v>0.37140650219999999</v>
       </c>
       <c r="BB5" s="50">
-        <v>22.461390435589401</v>
+        <v>22.461390439999999</v>
       </c>
       <c r="BC5" s="50">
-        <v>43.988167450184299</v>
+        <v>43.988167449999999</v>
       </c>
       <c r="BD5" s="44"/>
       <c r="BE5">
@@ -4966,22 +4966,22 @@
         <v>47.762096293894203</v>
       </c>
       <c r="AX6" s="50">
-        <v>14.851574153242799</v>
+        <v>14.851574149999999</v>
       </c>
       <c r="AY6" s="50">
-        <v>-0.85838254078074405</v>
+        <v>-0.85838254079999998</v>
       </c>
       <c r="AZ6" s="50">
-        <v>15.7099566940236</v>
+        <v>15.70995669</v>
       </c>
       <c r="BA6" s="50">
-        <v>6.9965958062310696</v>
+        <v>6.9965958060000002</v>
       </c>
       <c r="BB6" s="50">
-        <v>24.095420378555701</v>
+        <v>24.09542038</v>
       </c>
       <c r="BC6" s="50">
-        <v>47.223987370547697</v>
+        <v>47.223987370000003</v>
       </c>
       <c r="BD6" s="44"/>
       <c r="BE6">
@@ -5161,22 +5161,22 @@
         <v>35.355596284351698</v>
       </c>
       <c r="AX7" s="50">
-        <v>6.6566362138331598</v>
+        <v>6.6566362139999997</v>
       </c>
       <c r="AY7" s="50">
-        <v>-13.8026489120794</v>
+        <v>-13.80264891</v>
       </c>
       <c r="AZ7" s="50">
-        <v>20.459285125912601</v>
+        <v>20.459285130000001</v>
       </c>
       <c r="BA7" s="50">
-        <v>-3.5730063491231601</v>
+        <v>-3.5730063489999999</v>
       </c>
       <c r="BB7" s="50">
-        <v>17.941820061995799</v>
+        <v>17.941820060000001</v>
       </c>
       <c r="BC7" s="50">
-        <v>35.063444020270097</v>
+        <v>35.063444019999999</v>
       </c>
       <c r="BD7" s="44"/>
       <c r="BE7">
@@ -5347,22 +5347,22 @@
         <v>42.5456389567846</v>
       </c>
       <c r="AX8" s="50">
-        <v>-1.15628904358433</v>
+        <v>-1.156289044</v>
       </c>
       <c r="AY8" s="50">
-        <v>-0.70441124849329695</v>
+        <v>-0.70441124850000003</v>
       </c>
       <c r="AZ8" s="50">
-        <v>-0.45187779509103798</v>
+        <v>-0.45187779509999998</v>
       </c>
       <c r="BA8" s="50">
-        <v>-0.93035014603881605</v>
+        <v>-0.93035014599999999</v>
       </c>
       <c r="BB8" s="50">
-        <v>21.5157968077277</v>
+        <v>21.515796810000001</v>
       </c>
       <c r="BC8" s="50">
-        <v>42.117851051899301</v>
+        <v>42.117851049999999</v>
       </c>
       <c r="BD8" s="44"/>
       <c r="BE8">
@@ -5536,22 +5536,22 @@
         <v>45.7807904317755</v>
       </c>
       <c r="AX9" s="50">
-        <v>16.036656468840999</v>
+        <v>16.03665647</v>
       </c>
       <c r="AY9" s="50">
-        <v>-4.8656873390863202</v>
+        <v>-4.8656873389999999</v>
       </c>
       <c r="AZ9" s="50">
-        <v>20.902343807927299</v>
+        <v>20.902343810000001</v>
       </c>
       <c r="BA9" s="50">
-        <v>5.5854845648773397</v>
+        <v>5.5854845649999998</v>
       </c>
       <c r="BB9" s="50">
-        <v>23.117269398744899</v>
+        <v>23.117269400000001</v>
       </c>
       <c r="BC9" s="50">
-        <v>45.286402388126902</v>
+        <v>45.286402389999999</v>
       </c>
       <c r="BE9">
         <v>265</v>
@@ -5722,22 +5722,22 @@
         <v>45.209547777639301</v>
       </c>
       <c r="AX10" s="50">
-        <v>14.4579715364672</v>
+        <v>14.457971540000001</v>
       </c>
       <c r="AY10" s="50">
-        <v>-34.815304667159701</v>
+        <v>-34.815304670000003</v>
       </c>
       <c r="AZ10" s="50">
-        <v>49.273276203626899</v>
+        <v>49.273276199999998</v>
       </c>
       <c r="BA10" s="50">
-        <v>-10.1786665653462</v>
+        <v>-10.178666570000001</v>
       </c>
       <c r="BB10" s="50">
-        <v>22.853627356464699</v>
+        <v>22.853627360000001</v>
       </c>
       <c r="BC10" s="50">
-        <v>44.764460247631298</v>
+        <v>44.764460249999999</v>
       </c>
       <c r="BE10">
         <v>265</v>
@@ -5914,22 +5914,22 @@
         <v>45.520315450628203</v>
       </c>
       <c r="AX11" s="50">
-        <v>17.1518234709566</v>
+        <v>17.15182347</v>
       </c>
       <c r="AY11" s="50">
-        <v>-4.5745335204508901</v>
+        <v>-4.5745335200000001</v>
       </c>
       <c r="AZ11" s="50">
-        <v>21.726356991407499</v>
+        <v>21.726356989999999</v>
       </c>
       <c r="BA11" s="50">
-        <v>6.2886449752528799</v>
+        <v>6.2886449750000004</v>
       </c>
       <c r="BB11" s="50">
-        <v>22.988533215933799</v>
+        <v>22.988533220000001</v>
       </c>
       <c r="BC11" s="50">
-        <v>45.031522726332703</v>
+        <v>45.031522729999999</v>
       </c>
       <c r="BE11">
         <v>265</v>
@@ -6098,22 +6098,22 @@
         <v>33.978406326581499</v>
       </c>
       <c r="AX12" s="50">
-        <v>7.0098620813652204</v>
+        <v>7.0098620809999996</v>
       </c>
       <c r="AY12" s="50">
-        <v>-14.5751415214816</v>
+        <v>-14.575141520000001</v>
       </c>
       <c r="AZ12" s="50">
-        <v>21.5850036028468</v>
+        <v>21.5850036</v>
       </c>
       <c r="BA12" s="50">
-        <v>-3.78263972005821</v>
+        <v>-3.7826397200000001</v>
       </c>
       <c r="BB12" s="50">
-        <v>17.254451999306699</v>
+        <v>17.254452000000001</v>
       </c>
       <c r="BC12" s="50">
-        <v>33.709358475152598</v>
+        <v>33.709358479999999</v>
       </c>
       <c r="BE12">
         <v>265</v>
@@ -6282,22 +6282,22 @@
         <v>44.181166769186902</v>
       </c>
       <c r="AX13" s="50">
-        <v>8.2241945278393999E-2</v>
+        <v>8.2241945280000006E-2</v>
       </c>
       <c r="AY13" s="50">
-        <v>0.22102332359041901</v>
+        <v>0.22102332359999999</v>
       </c>
       <c r="AZ13" s="50">
-        <v>-0.138781378312025</v>
+        <v>-0.13878137830000001</v>
       </c>
       <c r="BA13" s="50">
-        <v>0.151632634434406</v>
+        <v>0.15163263439999999</v>
       </c>
       <c r="BB13" s="50">
-        <v>22.3259423648012</v>
+        <v>22.325942359999999</v>
       </c>
       <c r="BC13" s="50">
-        <v>43.720161276728597</v>
+        <v>43.720161279999999</v>
       </c>
       <c r="BE13">
         <v>265</v>
@@ -6466,22 +6466,22 @@
         <v>45.431524384704502</v>
       </c>
       <c r="AX14" s="50">
-        <v>14.393773542834699</v>
+        <v>14.39377354</v>
       </c>
       <c r="AY14" s="50">
-        <v>-3.6809189289388402</v>
+        <v>-3.6809189290000002</v>
       </c>
       <c r="AZ14" s="50">
-        <v>18.074692471773599</v>
+        <v>18.074692469999999</v>
       </c>
       <c r="BA14" s="50">
-        <v>5.3564273069479604</v>
+        <v>5.3564273069999997</v>
       </c>
       <c r="BB14" s="50">
-        <v>22.94455532836</v>
+        <v>22.94455533</v>
       </c>
       <c r="BC14" s="50">
-        <v>44.944459545090702</v>
+        <v>44.944459549999998</v>
       </c>
       <c r="BE14">
         <v>265</v>
@@ -6650,22 +6650,22 @@
         <v>46.530448225756899</v>
       </c>
       <c r="AX15" s="50">
-        <v>16.679833428360201</v>
+        <v>16.679833429999999</v>
       </c>
       <c r="AY15" s="50">
-        <v>-4.3336183513273898</v>
+        <v>-4.3336183510000001</v>
       </c>
       <c r="AZ15" s="50">
-        <v>21.0134517796876</v>
+        <v>21.01345178</v>
       </c>
       <c r="BA15" s="50">
-        <v>6.1731075385164003</v>
+        <v>6.1731075390000001</v>
       </c>
       <c r="BB15" s="50">
-        <v>23.487665779901398</v>
+        <v>23.48766578</v>
       </c>
       <c r="BC15" s="50">
-        <v>46.019903286484897</v>
+        <v>46.019903290000002</v>
       </c>
       <c r="BE15">
         <v>265</v>
@@ -6834,22 +6834,22 @@
         <v>34.941280181798497</v>
       </c>
       <c r="AX16" s="50">
-        <v>7.1029978910310803</v>
+        <v>7.1029978910000002</v>
       </c>
       <c r="AY16" s="50">
-        <v>-14.893050092214599</v>
+        <v>-14.893050089999999</v>
       </c>
       <c r="AZ16" s="50">
-        <v>21.996047983245699</v>
+        <v>21.99604798</v>
       </c>
       <c r="BA16" s="50">
-        <v>-3.8950261005917799</v>
+        <v>-3.895026101</v>
       </c>
       <c r="BB16" s="50">
-        <v>17.735485742880101</v>
+        <v>17.735485740000001</v>
       </c>
       <c r="BC16" s="50">
-        <v>34.656884164523802</v>
+        <v>34.656884159999997</v>
       </c>
       <c r="BE16">
         <v>265</v>
@@ -7014,22 +7014,22 @@
         <v>44.644312779463498</v>
       </c>
       <c r="AX17" s="50">
-        <v>13.725240315331099</v>
+        <v>13.725240319999999</v>
       </c>
       <c r="AY17" s="50">
-        <v>-28.3353648321477</v>
+        <v>-28.33536483</v>
       </c>
       <c r="AZ17" s="50">
-        <v>42.060605147478803</v>
+        <v>42.060605150000001</v>
       </c>
       <c r="BA17" s="50">
-        <v>-7.3050622584082596</v>
+        <v>-7.3050622580000004</v>
       </c>
       <c r="BB17" s="50">
-        <v>22.565126816266901</v>
+        <v>22.56512682</v>
       </c>
       <c r="BC17" s="50">
-        <v>44.193449376003002</v>
+        <v>44.193449379999997</v>
       </c>
       <c r="BE17">
         <v>265</v>
@@ -8014,8 +8014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8557,11 +8557,11 @@
         <v>ATM_EQ_SW</v>
       </c>
       <c r="B13" s="68">
-        <f t="shared" ref="B13:C15" si="7">M3</f>
+        <f>M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="C13" s="68">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="B13:C15" si="7">N3</f>
         <v>1.0044225086731247</v>
       </c>
       <c r="D13" s="111">
@@ -8603,7 +8603,7 @@
         <v>S2_ref_1</v>
       </c>
       <c r="B14" s="68">
-        <f t="shared" si="7"/>
+        <f>M4</f>
         <v>0.99629623559207692</v>
       </c>
       <c r="C14" s="68">

</xml_diff>

<commit_message>
Add column names to scrambling input, update spreadsheet template to avoid float error, add version 0.0.6 build to dist archives
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D4EF05-02C8-404E-A2BE-E63A68E3B500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3785D82D-1678-7142-9063-ADD568A6369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="13140" yWindow="500" windowWidth="15660" windowHeight="15880" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -632,7 +632,7 @@
     <numFmt numFmtId="173" formatCode="0.0000E+00"/>
     <numFmt numFmtId="174" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -770,10 +770,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1155,7 +1151,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1368,18 +1364,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="24" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="25" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="23" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="24" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="24" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1580,7 +1575,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>scale_normalization!$F$13:$F$27</c:f>
+              <c:f>scale_normalization!$U$3:$U$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1634,7 +1629,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scale_normalization!$H$13:$H$27</c:f>
+              <c:f>scale_normalization!$W$3:$W$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2109,7 +2104,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>scale_normalization!$G$13:$G$27</c:f>
+              <c:f>scale_normalization!$V$3:$V$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2163,7 +2158,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scale_normalization!$I$13:$I$27</c:f>
+              <c:f>scale_normalization!$X$3:$X$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3611,16 +3606,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3647,16 +3642,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3983,7 +3978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
       <selection activeCell="AQ12" sqref="AQ12"/>
     </sheetView>
   </sheetViews>
@@ -4043,11 +4038,11 @@
       <c r="AP1" s="58"/>
       <c r="AQ1" s="51"/>
       <c r="AR1" s="45"/>
-      <c r="AT1" s="125" t="s">
+      <c r="AT1" s="124" t="s">
         <v>181</v>
       </c>
-      <c r="AU1" s="125"/>
-      <c r="AV1" s="125"/>
+      <c r="AU1" s="124"/>
+      <c r="AV1" s="124"/>
       <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
@@ -4195,13 +4190,13 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="126" t="s">
+      <c r="AT2" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="127" t="s">
+      <c r="AU2" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="128" t="s">
+      <c r="AV2" s="127" t="s">
         <v>34</v>
       </c>
       <c r="AX2" s="39" t="s">
@@ -4367,7 +4362,7 @@
         <f>AJ3*$Y$3</f>
         <v>2.1161148587211971E-3</v>
       </c>
-      <c r="AO3" s="124">
+      <c r="AO3" s="123">
         <v>0</v>
       </c>
       <c r="AP3" s="56">
@@ -4553,7 +4548,7 @@
         <f t="shared" ref="AN4:AN17" si="9">AJ4*$Y$3</f>
         <v>2.09139498425152E-3</v>
       </c>
-      <c r="AO4" s="124">
+      <c r="AO4" s="123">
         <v>0</v>
       </c>
       <c r="AP4" s="56">
@@ -4744,7 +4739,7 @@
         <f t="shared" si="9"/>
         <v>2.1097889665454826E-3</v>
       </c>
-      <c r="AO5" s="124">
+      <c r="AO5" s="123">
         <v>0</v>
       </c>
       <c r="AP5" s="56">
@@ -4939,7 +4934,7 @@
         <f t="shared" si="9"/>
         <v>2.1164798861162187E-3</v>
       </c>
-      <c r="AO6" s="124">
+      <c r="AO6" s="123">
         <v>0</v>
       </c>
       <c r="AP6" s="56">
@@ -5134,7 +5129,7 @@
         <f t="shared" si="9"/>
         <v>2.0917613635465034E-3</v>
       </c>
-      <c r="AO7" s="124">
+      <c r="AO7" s="123">
         <v>0</v>
       </c>
       <c r="AP7" s="56">
@@ -5320,7 +5315,7 @@
         <f t="shared" si="9"/>
         <v>2.1059970799231576E-3</v>
       </c>
-      <c r="AO8" s="124">
+      <c r="AO8" s="123">
         <v>0</v>
       </c>
       <c r="AP8" s="56">
@@ -5509,7 +5504,7 @@
         <f t="shared" si="9"/>
         <v>2.1125489546459449E-3</v>
       </c>
-      <c r="AO9" s="124">
+      <c r="AO9" s="123">
         <v>0</v>
       </c>
       <c r="AP9" s="56">
@@ -5695,7 +5690,7 @@
         <f t="shared" si="9"/>
         <v>2.1110245425008428E-3</v>
       </c>
-      <c r="AO10" s="124">
+      <c r="AO10" s="123">
         <v>0</v>
       </c>
       <c r="AP10" s="56">
@@ -5836,11 +5831,11 @@
         <v>0.42918780000000001</v>
       </c>
       <c r="X11" s="34">
-        <f>scale_normalization!J13</f>
+        <f>scale_normalization!Y3</f>
         <v>1.058002378564959</v>
       </c>
       <c r="Y11" s="36">
-        <f>scale_normalization!K13</f>
+        <f>scale_normalization!Z3</f>
         <v>0.9378376950888252</v>
       </c>
       <c r="AA11" s="28">
@@ -5887,7 +5882,7 @@
         <f t="shared" si="9"/>
         <v>2.11205838421125E-3</v>
       </c>
-      <c r="AO11" s="124">
+      <c r="AO11" s="123">
         <v>0</v>
       </c>
       <c r="AP11" s="56">
@@ -6071,7 +6066,7 @@
         <f t="shared" si="9"/>
         <v>2.0890378267892978E-3</v>
       </c>
-      <c r="AO12" s="124">
+      <c r="AO12" s="123">
         <v>0</v>
       </c>
       <c r="AP12" s="56">
@@ -6255,7 +6250,7 @@
         <f t="shared" si="9"/>
         <v>2.1092446228371492E-3</v>
       </c>
-      <c r="AO13" s="124">
+      <c r="AO13" s="123">
         <v>0</v>
       </c>
       <c r="AP13" s="56">
@@ -6439,7 +6434,7 @@
         <f t="shared" si="9"/>
         <v>2.1118562233900973E-3</v>
       </c>
-      <c r="AO14" s="124">
+      <c r="AO14" s="123">
         <v>0</v>
       </c>
       <c r="AP14" s="56">
@@ -6623,7 +6618,7 @@
         <f t="shared" si="9"/>
         <v>2.1140383039962136E-3</v>
       </c>
-      <c r="AO15" s="124">
+      <c r="AO15" s="123">
         <v>0</v>
       </c>
       <c r="AP15" s="56">
@@ -6807,7 +6802,7 @@
         <f t="shared" si="9"/>
         <v>2.0909357320700551E-3</v>
       </c>
-      <c r="AO16" s="124">
+      <c r="AO16" s="123">
         <v>0</v>
       </c>
       <c r="AP16" s="56">
@@ -6987,7 +6982,7 @@
         <f t="shared" si="9"/>
         <v>2.1099653819650526E-3</v>
       </c>
-      <c r="AO17" s="124">
+      <c r="AO17" s="123">
         <v>0</v>
       </c>
       <c r="AP17" s="56">
@@ -8012,10 +8007,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8039,76 +8034,117 @@
     <col min="19" max="20" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="129" t="s">
+    <row r="1" spans="1:26">
+      <c r="A1" s="128" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130" t="s">
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="129" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
       <c r="O1" s="115" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="115"/>
-    </row>
-    <row r="2" spans="1:17" ht="17">
-      <c r="A2" s="117" t="s">
+      <c r="P1" s="114"/>
+      <c r="Q1" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" s="70"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="62"/>
+    </row>
+    <row r="2" spans="1:26" ht="17">
+      <c r="A2" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="117" t="s">
+      <c r="C2" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="117" t="s">
+      <c r="D2" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="117" t="s">
+      <c r="E2" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="117" t="s">
+      <c r="F2" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="118" t="s">
+      <c r="G2" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="118" t="s">
+      <c r="H2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="117" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="118" t="s">
+      <c r="J2" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="118" t="s">
+      <c r="K2" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="L2" s="118" t="s">
+      <c r="L2" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="118" t="s">
+      <c r="M2" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="N2" s="118" t="s">
+      <c r="N2" s="117" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="P2" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="S2" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="W2" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="X2" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="17" thickBot="1">
       <c r="A3" s="68" t="s">
         <v>36</v>
       </c>
@@ -8161,8 +8197,52 @@
         <f>L3/size_correction!Y$3</f>
         <v>1.0044225086731247</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="P3" s="63" t="str">
+        <f>size_correction!D3</f>
+        <v>ATM_EQ_SW</v>
+      </c>
+      <c r="Q3" s="68">
+        <f>M3</f>
+        <v>1.0059496767117579</v>
+      </c>
+      <c r="R3" s="68">
+        <f>N3</f>
+        <v>1.0044225086731247</v>
+      </c>
+      <c r="S3" s="111">
+        <f>size_correction!AF3</f>
+        <v>1.0056851052976181</v>
+      </c>
+      <c r="T3" s="111">
+        <f>size_correction!AG3</f>
+        <v>1.0075218399408568</v>
+      </c>
+      <c r="U3" s="67">
+        <f t="shared" ref="U3:U17" si="0">LN(S3)</f>
+        <v>5.6690060748599133E-3</v>
+      </c>
+      <c r="V3" s="67">
+        <f t="shared" ref="V3:V17" si="1">LN(T3)</f>
+        <v>7.4936919644022753E-3</v>
+      </c>
+      <c r="W3" s="67">
+        <f t="shared" ref="W3:X10" si="2">LN(Q3)</f>
+        <v>5.9320472770020231E-3</v>
+      </c>
+      <c r="X3" s="67">
+        <f t="shared" si="2"/>
+        <v>4.412758119012896E-3</v>
+      </c>
+      <c r="Y3" s="72">
+        <f>SLOPE(W3:W17,U3:U17)</f>
+        <v>1.058002378564959</v>
+      </c>
+      <c r="Z3" s="72">
+        <f>SLOPE(X3:X17,V3:V17)</f>
+        <v>0.9378376950888252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A4" s="68" t="s">
         <v>38</v>
       </c>
@@ -8180,7 +8260,7 @@
         <v>32.729999999999997</v>
       </c>
       <c r="F4" s="69">
-        <f t="shared" ref="F4:F9" si="0">B4-C4</f>
+        <f t="shared" ref="F4:F9" si="3">B4-C4</f>
         <v>18.419999999999998</v>
       </c>
       <c r="G4" s="65">
@@ -8215,8 +8295,44 @@
         <f>L4/size_correction!Y$3</f>
         <v>0.99323347721175648</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="P4" s="63" t="str">
+        <f>size_correction!D4</f>
+        <v>S2_ref_1</v>
+      </c>
+      <c r="Q4" s="68">
+        <f>M4</f>
+        <v>0.99629623559207692</v>
+      </c>
+      <c r="R4" s="68">
+        <f>N4</f>
+        <v>0.99323347721175648</v>
+      </c>
+      <c r="S4" s="111">
+        <f>size_correction!AF4</f>
+        <v>0.99668972770557829</v>
+      </c>
+      <c r="T4" s="111">
+        <f>size_correction!AG4</f>
+        <v>0.99497700286985102</v>
+      </c>
+      <c r="U4" s="67">
+        <f t="shared" si="0"/>
+        <v>-3.3157633670658081E-3</v>
+      </c>
+      <c r="V4" s="67">
+        <f t="shared" si="1"/>
+        <v>-5.0356547842637621E-3</v>
+      </c>
+      <c r="W4" s="67">
+        <f t="shared" si="2"/>
+        <v>-3.7106403264231301E-3</v>
+      </c>
+      <c r="X4" s="67">
+        <f t="shared" si="2"/>
+        <v>-6.7895195007928941E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A5" s="68" t="s">
         <v>37</v>
       </c>
@@ -8234,31 +8350,31 @@
         <v>41.949257311111111</v>
       </c>
       <c r="F5" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.25581632613833338</v>
       </c>
       <c r="G5" s="65">
-        <f t="shared" ref="G5:H9" si="1">(B5/1000+1)*0.0036765</f>
+        <f t="shared" ref="G5:H9" si="4">(B5/1000+1)*0.0036765</f>
         <v>3.6750148213719339E-3</v>
       </c>
       <c r="H5" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I5" s="65">
-        <f t="shared" ref="I5:I9" si="2">(E5/1000+1)*0.0020052</f>
+        <f t="shared" ref="I5:I9" si="5">(E5/1000+1)*0.0020052</f>
         <v>2.0893166507602399E-3</v>
       </c>
       <c r="J5" s="65">
-        <f t="shared" ref="J5:J9" si="3">(I5/0.0020052)^0.516*0.0003799</f>
+        <f t="shared" ref="J5:J9" si="6">(I5/0.0020052)^0.516*0.0003799</f>
         <v>3.8804145413997107E-4</v>
       </c>
       <c r="K5" s="66">
-        <f t="shared" ref="K5:K9" si="4">G5+H5+J5</f>
+        <f t="shared" ref="K5:K9" si="7">G5+H5+J5</f>
         <v>7.7390116056068863E-3</v>
       </c>
       <c r="L5" s="66">
-        <f t="shared" ref="L5:L9" si="5">(G5+H5)*J5+I5+G5*H5</f>
+        <f t="shared" ref="L5:L9" si="8">(G5+H5)*J5+I5+G5*H5</f>
         <v>2.1056783222279545E-3</v>
       </c>
       <c r="M5" s="67">
@@ -8269,8 +8385,44 @@
         <f>L5/size_correction!Y$3</f>
         <v>1.0020859042591113</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="P5" s="63" t="str">
+        <f>size_correction!D5</f>
+        <v>B6_ref_1</v>
+      </c>
+      <c r="Q5" s="68">
+        <f>M5</f>
+        <v>0.99973991247556415</v>
+      </c>
+      <c r="R5" s="68">
+        <f>N5</f>
+        <v>1.0020859042591113</v>
+      </c>
+      <c r="S5" s="111">
+        <f>size_correction!AF5</f>
+        <v>1.0003832772874761</v>
+      </c>
+      <c r="T5" s="111">
+        <f>size_correction!AG5</f>
+        <v>1.0043106480077921</v>
+      </c>
+      <c r="U5" s="67">
+        <f t="shared" si="0"/>
+        <v>3.8320385549917295E-4</v>
+      </c>
+      <c r="V5" s="67">
+        <f t="shared" si="1"/>
+        <v>4.3013837783483656E-3</v>
+      </c>
+      <c r="W5" s="67">
+        <f t="shared" si="2"/>
+        <v>-2.6012135306176113E-4</v>
+      </c>
+      <c r="X5" s="67">
+        <f t="shared" si="2"/>
+        <v>2.0837317813513596E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A6" s="68" t="s">
         <v>176</v>
       </c>
@@ -8281,38 +8433,38 @@
         <v>-49.28</v>
       </c>
       <c r="D6" s="69">
-        <f t="shared" ref="D6:D9" si="6">AVERAGE(B6:C6)</f>
+        <f t="shared" ref="D6:D9" si="9">AVERAGE(B6:C6)</f>
         <v>-35.745000000000005</v>
       </c>
       <c r="E6" s="69">
         <v>26.94</v>
       </c>
       <c r="F6" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>27.07</v>
       </c>
       <c r="G6" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.5948449350000004E-3</v>
       </c>
       <c r="H6" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.49532208E-3</v>
       </c>
       <c r="I6" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.0592200879999997E-3</v>
       </c>
       <c r="J6" s="65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.8514702697154833E-4</v>
       </c>
       <c r="K6" s="66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.4753140419715489E-3</v>
       </c>
       <c r="L6" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0745159856220404E-3</v>
       </c>
       <c r="M6" s="67">
@@ -8323,8 +8475,44 @@
         <f>L6/size_correction!Y$3</f>
         <v>0.98725584312065418</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="P6" s="63" t="str">
+        <f>size_correction!D6</f>
+        <v>ATM_EQ_SW_1</v>
+      </c>
+      <c r="Q6" s="68">
+        <f>M3</f>
+        <v>1.0059496767117579</v>
+      </c>
+      <c r="R6" s="68">
+        <f>N3</f>
+        <v>1.0044225086731247</v>
+      </c>
+      <c r="S6" s="111">
+        <f>size_correction!AF6</f>
+        <v>1.0064059824102283</v>
+      </c>
+      <c r="T6" s="111">
+        <f>size_correction!AG6</f>
+        <v>1.0077071570383731</v>
+      </c>
+      <c r="U6" s="67">
+        <f t="shared" si="0"/>
+        <v>6.3855513126554056E-3</v>
+      </c>
+      <c r="V6" s="67">
+        <f t="shared" si="1"/>
+        <v>7.6776086292741075E-3</v>
+      </c>
+      <c r="W6" s="67">
+        <f t="shared" si="2"/>
+        <v>5.9320472770020231E-3</v>
+      </c>
+      <c r="X6" s="67">
+        <f t="shared" si="2"/>
+        <v>4.412758119012896E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A7" s="68">
         <v>53504</v>
       </c>
@@ -8335,14 +8523,14 @@
         <v>94.44</v>
       </c>
       <c r="D7" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>48.074999999999996</v>
       </c>
       <c r="E7" s="69">
         <v>36.01</v>
       </c>
       <c r="F7" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-92.73</v>
       </c>
       <c r="G7" s="65">
@@ -8350,23 +8538,23 @@
         <v>3.6827868150000006E-3</v>
       </c>
       <c r="H7" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.0237086600000008E-3</v>
       </c>
       <c r="I7" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.0774072520000002E-3</v>
       </c>
       <c r="J7" s="65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.8689853960154226E-4</v>
       </c>
       <c r="K7" s="66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.0933940146015442E-3</v>
       </c>
       <c r="L7" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0952073450451725E-3</v>
       </c>
       <c r="M7" s="67">
@@ -8377,8 +8565,44 @@
         <f>L7/size_correction!Y$3</f>
         <v>0.99710279808951241</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="P7" s="63" t="str">
+        <f>size_correction!D7</f>
+        <v>S2_ref_2</v>
+      </c>
+      <c r="Q7" s="68">
+        <f>M4</f>
+        <v>0.99629623559207692</v>
+      </c>
+      <c r="R7" s="68">
+        <f>N4</f>
+        <v>0.99323347721175648</v>
+      </c>
+      <c r="S7" s="111">
+        <f>size_correction!AF7</f>
+        <v>0.99663201609671503</v>
+      </c>
+      <c r="T7" s="111">
+        <f>size_correction!AG7</f>
+        <v>0.9951628615034982</v>
+      </c>
+      <c r="U7" s="67">
+        <f t="shared" si="0"/>
+        <v>-3.3736683280273967E-3</v>
+      </c>
+      <c r="V7" s="67">
+        <f t="shared" si="1"/>
+        <v>-4.8488753146248009E-3</v>
+      </c>
+      <c r="W7" s="67">
+        <f t="shared" si="2"/>
+        <v>-3.7106403264231301E-3</v>
+      </c>
+      <c r="X7" s="67">
+        <f t="shared" si="2"/>
+        <v>-6.7895195007928941E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A8" s="68" t="s">
         <v>177</v>
       </c>
@@ -8389,38 +8613,38 @@
         <v>-3.43</v>
       </c>
       <c r="D8" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6.84</v>
       </c>
       <c r="E8" s="69">
         <v>35.29</v>
       </c>
       <c r="F8" s="69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>20.54</v>
       </c>
       <c r="G8" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.7394049149999998E-3</v>
       </c>
       <c r="H8" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.6638896049999998E-3</v>
       </c>
       <c r="I8" s="65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.0759635080000003E-3</v>
       </c>
       <c r="J8" s="65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.8675977189798279E-4</v>
       </c>
       <c r="K8" s="66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.7900542918979817E-3</v>
       </c>
       <c r="L8" s="66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0925275712968031E-3</v>
       </c>
       <c r="M8" s="67">
@@ -8431,60 +8655,132 @@
         <f>L8/size_correction!Y$3</f>
         <v>0.99582750191939118</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="119">
+      <c r="P8" s="63" t="str">
+        <f>size_correction!D8</f>
+        <v>B6_ref_2</v>
+      </c>
+      <c r="Q8" s="68">
+        <f>M5</f>
+        <v>0.99973991247556415</v>
+      </c>
+      <c r="R8" s="68">
+        <f>N5</f>
+        <v>1.0020859042591113</v>
+      </c>
+      <c r="S8" s="111">
+        <f>size_correction!AF8</f>
+        <v>0.99917068284195976</v>
+      </c>
+      <c r="T8" s="111">
+        <f>size_correction!AG8</f>
+        <v>1.0023860907979212</v>
+      </c>
+      <c r="U8" s="67">
+        <f t="shared" si="0"/>
+        <v>-8.2966123175853173E-4</v>
+      </c>
+      <c r="V8" s="67">
+        <f t="shared" si="1"/>
+        <v>2.3832486035312902E-3</v>
+      </c>
+      <c r="W8" s="67">
+        <f t="shared" si="2"/>
+        <v>-2.6012135306176113E-4</v>
+      </c>
+      <c r="X8" s="67">
+        <f t="shared" si="2"/>
+        <v>2.0837317813513596E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="A9" s="118">
         <v>90454</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="119">
         <v>25.73</v>
       </c>
-      <c r="C9" s="120">
+      <c r="C9" s="119">
         <v>25.44</v>
       </c>
-      <c r="D9" s="120">
+      <c r="D9" s="119">
+        <f t="shared" si="9"/>
+        <v>25.585000000000001</v>
+      </c>
+      <c r="E9" s="119">
+        <v>35.880000000000003</v>
+      </c>
+      <c r="F9" s="119">
+        <f t="shared" si="3"/>
+        <v>0.28999999999999915</v>
+      </c>
+      <c r="G9" s="120">
+        <f t="shared" si="4"/>
+        <v>3.7710963450000002E-3</v>
+      </c>
+      <c r="H9" s="120">
+        <f t="shared" si="4"/>
+        <v>3.7700301599999995E-3</v>
+      </c>
+      <c r="I9" s="120">
+        <f t="shared" si="5"/>
+        <v>2.0771465759999996E-3</v>
+      </c>
+      <c r="J9" s="120">
         <f t="shared" si="6"/>
-        <v>25.585000000000001</v>
-      </c>
-      <c r="E9" s="120">
-        <v>35.880000000000003</v>
-      </c>
-      <c r="F9" s="120">
+        <v>3.8687348777560239E-4</v>
+      </c>
+      <c r="K9" s="121">
+        <f t="shared" si="7"/>
+        <v>7.9279999927756029E-3</v>
+      </c>
+      <c r="L9" s="121">
+        <f t="shared" si="8"/>
+        <v>2.0942811848696616E-3</v>
+      </c>
+      <c r="M9" s="122">
+        <v>1.0241537838167138</v>
+      </c>
+      <c r="N9" s="122">
+        <v>0.9966620412810443</v>
+      </c>
+      <c r="P9" s="63" t="str">
+        <f>size_correction!D9</f>
+        <v>ATM_EQ_SW_2</v>
+      </c>
+      <c r="Q9" s="68">
+        <f>M3</f>
+        <v>1.0059496767117579</v>
+      </c>
+      <c r="R9" s="68">
+        <f>N3</f>
+        <v>1.0044225086731247</v>
+      </c>
+      <c r="S9" s="111">
+        <f>size_correction!AF9</f>
+        <v>1.0050941512728657</v>
+      </c>
+      <c r="T9" s="111">
+        <f>size_correction!AG9</f>
+        <v>1.0057116133646442</v>
+      </c>
+      <c r="U9" s="67">
         <f t="shared" si="0"/>
-        <v>0.28999999999999915</v>
-      </c>
-      <c r="G9" s="121">
+        <v>5.0812199816469847E-3</v>
+      </c>
+      <c r="V9" s="67">
         <f t="shared" si="1"/>
-        <v>3.7710963450000002E-3</v>
-      </c>
-      <c r="H9" s="121">
-        <f t="shared" si="1"/>
-        <v>3.7700301599999995E-3</v>
-      </c>
-      <c r="I9" s="121">
+        <v>5.6953639452707308E-3</v>
+      </c>
+      <c r="W9" s="67">
         <f t="shared" si="2"/>
-        <v>2.0771465759999996E-3</v>
-      </c>
-      <c r="J9" s="121">
-        <f t="shared" si="3"/>
-        <v>3.8687348777560239E-4</v>
-      </c>
-      <c r="K9" s="122">
-        <f t="shared" si="4"/>
-        <v>7.9279999927756029E-3</v>
-      </c>
-      <c r="L9" s="122">
-        <f t="shared" si="5"/>
-        <v>2.0942811848696616E-3</v>
-      </c>
-      <c r="M9" s="123">
-        <v>1.0241537838167138</v>
-      </c>
-      <c r="N9" s="123">
-        <v>0.9966620412810443</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>5.9320472770020231E-3</v>
+      </c>
+      <c r="X9" s="67">
+        <f t="shared" si="2"/>
+        <v>4.412758119012896E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="A10" s="63"/>
       <c r="B10" s="63"/>
       <c r="C10" s="63"/>
@@ -8498,630 +8794,309 @@
       <c r="M10" s="63"/>
       <c r="N10" s="63"/>
       <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="114"/>
-      <c r="B11" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="62"/>
+      <c r="P10" s="63" t="str">
+        <f>size_correction!D10</f>
+        <v>DI</v>
+      </c>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="111">
+        <f>size_correction!AF10</f>
+        <v>0.99092722925764687</v>
+      </c>
+      <c r="T10" s="111">
+        <f>size_correction!AG10</f>
+        <v>1.0049378092932522</v>
+      </c>
+      <c r="U10" s="67">
+        <f t="shared" si="0"/>
+        <v>-9.1141789753790732E-3</v>
+      </c>
+      <c r="V10" s="67">
+        <f t="shared" si="1"/>
+        <v>4.9256582960658154E-3</v>
+      </c>
+      <c r="W10" s="67"/>
+      <c r="X10" s="67"/>
+    </row>
+    <row r="11" spans="1:26" ht="18" thickTop="1" thickBot="1">
       <c r="L11" s="63"/>
       <c r="M11" s="63"/>
-    </row>
-    <row r="12" spans="1:17" s="41" customFormat="1">
-      <c r="A12" s="63" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="H12" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="J12" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="K12" s="41" t="s">
-        <v>107</v>
-      </c>
+      <c r="P11" s="63" t="str">
+        <f>size_correction!D11</f>
+        <v>ATM_EQ_SW_1</v>
+      </c>
+      <c r="Q11" s="68">
+        <f>M3</f>
+        <v>1.0059496767117579</v>
+      </c>
+      <c r="R11" s="68">
+        <f>N3</f>
+        <v>1.0044225086731247</v>
+      </c>
+      <c r="S11" s="111">
+        <f>size_correction!AF11</f>
+        <v>1.0057192814133826</v>
+      </c>
+      <c r="T11" s="111">
+        <f>size_correction!AG11</f>
+        <v>1.0054625917600983</v>
+      </c>
+      <c r="U11" s="67">
+        <f t="shared" si="0"/>
+        <v>5.7029884167436144E-3</v>
+      </c>
+      <c r="V11" s="67">
+        <f t="shared" si="1"/>
+        <v>5.4477259185061388E-3</v>
+      </c>
+      <c r="W11" s="67">
+        <f t="shared" ref="W11:X16" si="10">LN(Q11)</f>
+        <v>5.9320472770020231E-3</v>
+      </c>
+      <c r="X11" s="67">
+        <f t="shared" si="10"/>
+        <v>4.412758119012896E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1">
       <c r="M12" s="63"/>
       <c r="O12" s="63"/>
-    </row>
-    <row r="13" spans="1:17" ht="17" thickBot="1">
-      <c r="A13" s="63" t="str">
-        <f>size_correction!D3</f>
-        <v>ATM_EQ_SW</v>
-      </c>
-      <c r="B13" s="68">
+      <c r="P12" s="63" t="str">
+        <f>size_correction!D12</f>
+        <v>S2_ref_1</v>
+      </c>
+      <c r="Q12" s="68">
+        <f>M4</f>
+        <v>0.99629623559207692</v>
+      </c>
+      <c r="R12" s="68">
+        <f>N4</f>
+        <v>0.99323347721175648</v>
+      </c>
+      <c r="S12" s="111">
+        <f>size_correction!AF12</f>
+        <v>0.99641187878361481</v>
+      </c>
+      <c r="T12" s="111">
+        <f>size_correction!AG12</f>
+        <v>0.99378130442821833</v>
+      </c>
+      <c r="U12" s="67">
+        <f t="shared" si="0"/>
+        <v>-3.5945739634335372E-3</v>
+      </c>
+      <c r="V12" s="67">
+        <f t="shared" si="1"/>
+        <v>-6.2381121983366193E-3</v>
+      </c>
+      <c r="W12" s="67">
+        <f t="shared" si="10"/>
+        <v>-3.7106403264231301E-3</v>
+      </c>
+      <c r="X12" s="67">
+        <f t="shared" si="10"/>
+        <v>-6.7895195007928941E-3</v>
+      </c>
+      <c r="Y12"/>
+      <c r="Z12"/>
+    </row>
+    <row r="13" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="P13" s="63" t="str">
+        <f>size_correction!D13</f>
+        <v>B6_ref_1</v>
+      </c>
+      <c r="Q13" s="68">
+        <f>M5</f>
+        <v>0.99973991247556415</v>
+      </c>
+      <c r="R13" s="68">
+        <f>N5</f>
+        <v>1.0020859042591113</v>
+      </c>
+      <c r="S13" s="111">
+        <f>size_correction!AF13</f>
+        <v>1.0001796848444418</v>
+      </c>
+      <c r="T13" s="111">
+        <f>size_correction!AG13</f>
+        <v>1.0040343543858852</v>
+      </c>
+      <c r="U13" s="67">
+        <f t="shared" si="0"/>
+        <v>1.7966870305363727E-4</v>
+      </c>
+      <c r="V13" s="67">
+        <f t="shared" si="1"/>
+        <v>4.0262381999534996E-3</v>
+      </c>
+      <c r="W13" s="67">
+        <f t="shared" si="10"/>
+        <v>-2.6012135306176113E-4</v>
+      </c>
+      <c r="X13" s="67">
+        <f t="shared" si="10"/>
+        <v>2.0837317813513596E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="P14" s="63" t="str">
+        <f>size_correction!D14</f>
+        <v>ATM_EQ_SW_2</v>
+      </c>
+      <c r="Q14" s="68">
         <f>M3</f>
         <v>1.0059496767117579</v>
       </c>
-      <c r="C13" s="68">
-        <f t="shared" ref="B13:C15" si="7">N3</f>
+      <c r="R14" s="68">
+        <f>N3</f>
         <v>1.0044225086731247</v>
       </c>
-      <c r="D13" s="111">
-        <f>size_correction!AF3</f>
-        <v>1.0056851052976181</v>
-      </c>
-      <c r="E13" s="111">
-        <f>size_correction!AG3</f>
-        <v>1.0075218399408568</v>
-      </c>
-      <c r="F13" s="67">
-        <f t="shared" ref="F13:F27" si="8">LN(D13)</f>
-        <v>5.6690060748599133E-3</v>
-      </c>
-      <c r="G13" s="67">
-        <f t="shared" ref="G13:G27" si="9">LN(E13)</f>
-        <v>7.4936919644022753E-3</v>
-      </c>
-      <c r="H13" s="67">
-        <f t="shared" ref="H13:I19" si="10">LN(B13)</f>
+      <c r="S14" s="111">
+        <f>size_correction!AF14</f>
+        <v>1.0048805539160894</v>
+      </c>
+      <c r="T14" s="111">
+        <f>size_correction!AG14</f>
+        <v>1.0053599727245706</v>
+      </c>
+      <c r="U14" s="67">
+        <f t="shared" si="0"/>
+        <v>4.8686826228146419E-3</v>
+      </c>
+      <c r="V14" s="67">
+        <f t="shared" si="1"/>
+        <v>5.3456591947391319E-3</v>
+      </c>
+      <c r="W14" s="67">
+        <f t="shared" si="10"/>
         <v>5.9320472770020231E-3</v>
       </c>
-      <c r="I13" s="67">
+      <c r="X14" s="67">
         <f t="shared" si="10"/>
         <v>4.412758119012896E-3</v>
       </c>
-      <c r="J13" s="72">
-        <f>SLOPE(H13:H27,F13:F27)</f>
-        <v>1.058002378564959</v>
-      </c>
-      <c r="K13" s="72">
-        <f>SLOPE(I13:I27,G13:G27)</f>
-        <v>0.9378376950888252</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="18" thickTop="1" thickBot="1">
-      <c r="A14" s="63" t="str">
-        <f>size_correction!D4</f>
-        <v>S2_ref_1</v>
-      </c>
-      <c r="B14" s="68">
+    </row>
+    <row r="15" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="P15" s="63" t="str">
+        <f>size_correction!D15</f>
+        <v>ATM_EQ_SW_3</v>
+      </c>
+      <c r="Q15" s="68">
+        <f>M3</f>
+        <v>1.0059496767117579</v>
+      </c>
+      <c r="R15" s="68">
+        <f>N3</f>
+        <v>1.0044225086731247</v>
+      </c>
+      <c r="S15" s="111">
+        <f>size_correction!AF15</f>
+        <v>1.0056387310168626</v>
+      </c>
+      <c r="T15" s="111">
+        <f>size_correction!AG15</f>
+        <v>1.0064676550191509</v>
+      </c>
+      <c r="U15" s="67">
+        <f t="shared" si="0"/>
+        <v>5.6228928832132777E-3</v>
+      </c>
+      <c r="V15" s="67">
+        <f t="shared" si="1"/>
+        <v>6.446829485110093E-3</v>
+      </c>
+      <c r="W15" s="67">
+        <f t="shared" si="10"/>
+        <v>5.9320472770020231E-3</v>
+      </c>
+      <c r="X15" s="67">
+        <f t="shared" si="10"/>
+        <v>4.412758119012896E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="P16" s="63" t="str">
+        <f>size_correction!D16</f>
+        <v>S2_ref_2</v>
+      </c>
+      <c r="Q16" s="68">
         <f>M4</f>
         <v>0.99629623559207692</v>
       </c>
-      <c r="C14" s="68">
-        <f t="shared" si="7"/>
+      <c r="R16" s="68">
+        <f>N4</f>
         <v>0.99323347721175648</v>
       </c>
-      <c r="D14" s="111">
-        <f>size_correction!AF4</f>
-        <v>0.99668972770557829</v>
-      </c>
-      <c r="E14" s="111">
-        <f>size_correction!AG4</f>
-        <v>0.99497700286985102</v>
-      </c>
-      <c r="F14" s="67">
-        <f t="shared" si="8"/>
-        <v>-3.3157633670658081E-3</v>
-      </c>
-      <c r="G14" s="67">
-        <f t="shared" si="9"/>
-        <v>-5.0356547842637621E-3</v>
-      </c>
-      <c r="H14" s="67">
+      <c r="S16" s="111">
+        <f>size_correction!AF16</f>
+        <v>0.99633327484903467</v>
+      </c>
+      <c r="T16" s="111">
+        <f>size_correction!AG16</f>
+        <v>0.99474403428411884</v>
+      </c>
+      <c r="U16" s="67">
+        <f t="shared" si="0"/>
+        <v>-3.6734640658408848E-3</v>
+      </c>
+      <c r="V16" s="67">
+        <f t="shared" si="1"/>
+        <v>-5.2698268942697113E-3</v>
+      </c>
+      <c r="W16" s="67">
         <f t="shared" si="10"/>
         <v>-3.7106403264231301E-3</v>
       </c>
-      <c r="I14" s="67">
+      <c r="X16" s="67">
         <f t="shared" si="10"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" thickTop="1" thickBot="1">
-      <c r="A15" s="63" t="str">
-        <f>size_correction!D5</f>
-        <v>B6_ref_1</v>
-      </c>
-      <c r="B15" s="68">
-        <f t="shared" si="7"/>
-        <v>0.99973991247556415</v>
-      </c>
-      <c r="C15" s="68">
-        <f t="shared" si="7"/>
-        <v>1.0020859042591113</v>
-      </c>
-      <c r="D15" s="111">
-        <f>size_correction!AF5</f>
-        <v>1.0003832772874761</v>
-      </c>
-      <c r="E15" s="111">
-        <f>size_correction!AG5</f>
-        <v>1.0043106480077921</v>
-      </c>
-      <c r="F15" s="67">
-        <f t="shared" si="8"/>
-        <v>3.8320385549917295E-4</v>
-      </c>
-      <c r="G15" s="67">
-        <f t="shared" si="9"/>
-        <v>4.3013837783483656E-3</v>
-      </c>
-      <c r="H15" s="67">
-        <f t="shared" si="10"/>
-        <v>-2.6012135306176113E-4</v>
-      </c>
-      <c r="I15" s="67">
-        <f t="shared" si="10"/>
-        <v>2.0837317813513596E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="18" thickTop="1" thickBot="1">
-      <c r="A16" s="63" t="str">
-        <f>size_correction!D6</f>
-        <v>ATM_EQ_SW_1</v>
-      </c>
-      <c r="B16" s="68">
-        <f t="shared" ref="B16:C18" si="11">M3</f>
-        <v>1.0059496767117579</v>
-      </c>
-      <c r="C16" s="68">
-        <f t="shared" si="11"/>
-        <v>1.0044225086731247</v>
-      </c>
-      <c r="D16" s="111">
-        <f>size_correction!AF6</f>
-        <v>1.0064059824102283</v>
-      </c>
-      <c r="E16" s="111">
-        <f>size_correction!AG6</f>
-        <v>1.0077071570383731</v>
-      </c>
-      <c r="F16" s="67">
-        <f t="shared" si="8"/>
-        <v>6.3855513126554056E-3</v>
-      </c>
-      <c r="G16" s="67">
-        <f t="shared" si="9"/>
-        <v>7.6776086292741075E-3</v>
-      </c>
-      <c r="H16" s="67">
-        <f t="shared" si="10"/>
-        <v>5.9320472770020231E-3</v>
-      </c>
-      <c r="I16" s="67">
-        <f t="shared" si="10"/>
-        <v>4.412758119012896E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A17" s="63" t="str">
-        <f>size_correction!D7</f>
-        <v>S2_ref_2</v>
-      </c>
-      <c r="B17" s="68">
-        <f t="shared" si="11"/>
-        <v>0.99629623559207692</v>
-      </c>
-      <c r="C17" s="68">
-        <f t="shared" si="11"/>
-        <v>0.99323347721175648</v>
-      </c>
-      <c r="D17" s="111">
-        <f>size_correction!AF7</f>
-        <v>0.99663201609671503</v>
-      </c>
-      <c r="E17" s="111">
-        <f>size_correction!AG7</f>
-        <v>0.9951628615034982</v>
-      </c>
-      <c r="F17" s="67">
-        <f t="shared" si="8"/>
-        <v>-3.3736683280273967E-3</v>
-      </c>
-      <c r="G17" s="67">
-        <f t="shared" si="9"/>
-        <v>-4.8488753146248009E-3</v>
-      </c>
-      <c r="H17" s="67">
-        <f t="shared" si="10"/>
-        <v>-3.7106403264231301E-3</v>
-      </c>
-      <c r="I17" s="67">
-        <f t="shared" si="10"/>
-        <v>-6.7895195007928941E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A18" s="63" t="str">
-        <f>size_correction!D8</f>
-        <v>B6_ref_2</v>
-      </c>
-      <c r="B18" s="68">
-        <f t="shared" si="11"/>
-        <v>0.99973991247556415</v>
-      </c>
-      <c r="C18" s="68">
-        <f t="shared" si="11"/>
-        <v>1.0020859042591113</v>
-      </c>
-      <c r="D18" s="111">
-        <f>size_correction!AF8</f>
-        <v>0.99917068284195976</v>
-      </c>
-      <c r="E18" s="111">
-        <f>size_correction!AG8</f>
-        <v>1.0023860907979212</v>
-      </c>
-      <c r="F18" s="67">
-        <f t="shared" si="8"/>
-        <v>-8.2966123175853173E-4</v>
-      </c>
-      <c r="G18" s="67">
-        <f t="shared" si="9"/>
-        <v>2.3832486035312902E-3</v>
-      </c>
-      <c r="H18" s="67">
-        <f t="shared" si="10"/>
-        <v>-2.6012135306176113E-4</v>
-      </c>
-      <c r="I18" s="67">
-        <f t="shared" si="10"/>
-        <v>2.0837317813513596E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A19" s="63" t="str">
-        <f>size_correction!D9</f>
-        <v>ATM_EQ_SW_2</v>
-      </c>
-      <c r="B19" s="68">
-        <f>M3</f>
-        <v>1.0059496767117579</v>
-      </c>
-      <c r="C19" s="68">
-        <f>N3</f>
-        <v>1.0044225086731247</v>
-      </c>
-      <c r="D19" s="111">
-        <f>size_correction!AF9</f>
-        <v>1.0050941512728657</v>
-      </c>
-      <c r="E19" s="111">
-        <f>size_correction!AG9</f>
-        <v>1.0057116133646442</v>
-      </c>
-      <c r="F19" s="67">
-        <f t="shared" si="8"/>
-        <v>5.0812199816469847E-3</v>
-      </c>
-      <c r="G19" s="67">
-        <f t="shared" si="9"/>
-        <v>5.6953639452707308E-3</v>
-      </c>
-      <c r="H19" s="67">
-        <f t="shared" si="10"/>
-        <v>5.9320472770020231E-3</v>
-      </c>
-      <c r="I19" s="67">
-        <f t="shared" si="10"/>
-        <v>4.412758119012896E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A20" s="63" t="str">
-        <f>size_correction!D10</f>
-        <v>DI</v>
-      </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="111">
-        <f>size_correction!AF10</f>
-        <v>0.99092722925764687</v>
-      </c>
-      <c r="E20" s="111">
-        <f>size_correction!AG10</f>
-        <v>1.0049378092932522</v>
-      </c>
-      <c r="F20" s="67">
-        <f t="shared" si="8"/>
-        <v>-9.1141789753790732E-3</v>
-      </c>
-      <c r="G20" s="67">
-        <f t="shared" si="9"/>
-        <v>4.9256582960658154E-3</v>
-      </c>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-    </row>
-    <row r="21" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A21" s="63" t="str">
-        <f>size_correction!D11</f>
-        <v>ATM_EQ_SW_1</v>
-      </c>
-      <c r="B21" s="68">
-        <f t="shared" ref="B21:C23" si="12">M3</f>
-        <v>1.0059496767117579</v>
-      </c>
-      <c r="C21" s="68">
-        <f t="shared" si="12"/>
-        <v>1.0044225086731247</v>
-      </c>
-      <c r="D21" s="111">
-        <f>size_correction!AF11</f>
-        <v>1.0057192814133826</v>
-      </c>
-      <c r="E21" s="111">
-        <f>size_correction!AG11</f>
-        <v>1.0054625917600983</v>
-      </c>
-      <c r="F21" s="67">
-        <f t="shared" si="8"/>
-        <v>5.7029884167436144E-3</v>
-      </c>
-      <c r="G21" s="67">
-        <f t="shared" si="9"/>
-        <v>5.4477259185061388E-3</v>
-      </c>
-      <c r="H21" s="67">
-        <f t="shared" ref="H21:I26" si="13">LN(B21)</f>
-        <v>5.9320472770020231E-3</v>
-      </c>
-      <c r="I21" s="67">
-        <f t="shared" si="13"/>
-        <v>4.412758119012896E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A22" s="63" t="str">
-        <f>size_correction!D12</f>
-        <v>S2_ref_1</v>
-      </c>
-      <c r="B22" s="68">
-        <f t="shared" si="12"/>
-        <v>0.99629623559207692</v>
-      </c>
-      <c r="C22" s="68">
-        <f t="shared" si="12"/>
-        <v>0.99323347721175648</v>
-      </c>
-      <c r="D22" s="111">
-        <f>size_correction!AF12</f>
-        <v>0.99641187878361481</v>
-      </c>
-      <c r="E22" s="111">
-        <f>size_correction!AG12</f>
-        <v>0.99378130442821833</v>
-      </c>
-      <c r="F22" s="67">
-        <f t="shared" si="8"/>
-        <v>-3.5945739634335372E-3</v>
-      </c>
-      <c r="G22" s="67">
-        <f t="shared" si="9"/>
-        <v>-6.2381121983366193E-3</v>
-      </c>
-      <c r="H22" s="67">
-        <f t="shared" si="13"/>
-        <v>-3.7106403264231301E-3</v>
-      </c>
-      <c r="I22" s="67">
-        <f t="shared" si="13"/>
-        <v>-6.7895195007928941E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A23" s="63" t="str">
-        <f>size_correction!D13</f>
-        <v>B6_ref_1</v>
-      </c>
-      <c r="B23" s="68">
-        <f t="shared" si="12"/>
-        <v>0.99973991247556415</v>
-      </c>
-      <c r="C23" s="68">
-        <f t="shared" si="12"/>
-        <v>1.0020859042591113</v>
-      </c>
-      <c r="D23" s="111">
-        <f>size_correction!AF13</f>
-        <v>1.0001796848444418</v>
-      </c>
-      <c r="E23" s="111">
-        <f>size_correction!AG13</f>
-        <v>1.0040343543858852</v>
-      </c>
-      <c r="F23" s="67">
-        <f t="shared" si="8"/>
-        <v>1.7966870305363727E-4</v>
-      </c>
-      <c r="G23" s="67">
-        <f t="shared" si="9"/>
-        <v>4.0262381999534996E-3</v>
-      </c>
-      <c r="H23" s="67">
-        <f t="shared" si="13"/>
-        <v>-2.6012135306176113E-4</v>
-      </c>
-      <c r="I23" s="67">
-        <f t="shared" si="13"/>
-        <v>2.0837317813513596E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A24" s="63" t="str">
-        <f>size_correction!D14</f>
-        <v>ATM_EQ_SW_2</v>
-      </c>
-      <c r="B24" s="68">
-        <f>M3</f>
-        <v>1.0059496767117579</v>
-      </c>
-      <c r="C24" s="68">
-        <f>N3</f>
-        <v>1.0044225086731247</v>
-      </c>
-      <c r="D24" s="111">
-        <f>size_correction!AF14</f>
-        <v>1.0048805539160894</v>
-      </c>
-      <c r="E24" s="111">
-        <f>size_correction!AG14</f>
-        <v>1.0053599727245706</v>
-      </c>
-      <c r="F24" s="67">
-        <f t="shared" si="8"/>
-        <v>4.8686826228146419E-3</v>
-      </c>
-      <c r="G24" s="67">
-        <f t="shared" si="9"/>
-        <v>5.3456591947391319E-3</v>
-      </c>
-      <c r="H24" s="67">
-        <f t="shared" si="13"/>
-        <v>5.9320472770020231E-3</v>
-      </c>
-      <c r="I24" s="67">
-        <f t="shared" si="13"/>
-        <v>4.412758119012896E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A25" s="63" t="str">
-        <f>size_correction!D15</f>
-        <v>ATM_EQ_SW_3</v>
-      </c>
-      <c r="B25" s="68">
-        <f>M3</f>
-        <v>1.0059496767117579</v>
-      </c>
-      <c r="C25" s="68">
-        <f>N3</f>
-        <v>1.0044225086731247</v>
-      </c>
-      <c r="D25" s="111">
-        <f>size_correction!AF15</f>
-        <v>1.0056387310168626</v>
-      </c>
-      <c r="E25" s="111">
-        <f>size_correction!AG15</f>
-        <v>1.0064676550191509</v>
-      </c>
-      <c r="F25" s="67">
-        <f t="shared" si="8"/>
-        <v>5.6228928832132777E-3</v>
-      </c>
-      <c r="G25" s="67">
-        <f t="shared" si="9"/>
-        <v>6.446829485110093E-3</v>
-      </c>
-      <c r="H25" s="67">
-        <f t="shared" si="13"/>
-        <v>5.9320472770020231E-3</v>
-      </c>
-      <c r="I25" s="67">
-        <f t="shared" si="13"/>
-        <v>4.412758119012896E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A26" s="63" t="str">
-        <f>size_correction!D16</f>
-        <v>S2_ref_2</v>
-      </c>
-      <c r="B26" s="68">
-        <f>M4</f>
-        <v>0.99629623559207692</v>
-      </c>
-      <c r="C26" s="68">
-        <f>N4</f>
-        <v>0.99323347721175648</v>
-      </c>
-      <c r="D26" s="111">
-        <f>size_correction!AF16</f>
-        <v>0.99633327484903467</v>
-      </c>
-      <c r="E26" s="111">
-        <f>size_correction!AG16</f>
-        <v>0.99474403428411884</v>
-      </c>
-      <c r="F26" s="67">
-        <f t="shared" si="8"/>
-        <v>-3.6734640658408848E-3</v>
-      </c>
-      <c r="G26" s="67">
-        <f t="shared" si="9"/>
-        <v>-5.2698268942697113E-3</v>
-      </c>
-      <c r="H26" s="67">
-        <f t="shared" si="13"/>
-        <v>-3.7106403264231301E-3</v>
-      </c>
-      <c r="I26" s="67">
-        <f t="shared" si="13"/>
-        <v>-6.7895195007928941E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="18" thickTop="1" thickBot="1">
-      <c r="A27" s="63" t="str">
+    <row r="17" spans="4:24" ht="18" thickTop="1" thickBot="1">
+      <c r="P17" s="63" t="str">
         <f>size_correction!D17</f>
         <v>DI</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="111">
+      <c r="Q17" s="68"/>
+      <c r="R17" s="68"/>
+      <c r="S17" s="111">
         <f>size_correction!AF17</f>
         <v>0.99349493237592013</v>
       </c>
-      <c r="E27" s="111">
+      <c r="T17" s="111">
         <f>size_correction!AG17</f>
         <v>1.0044001925480899</v>
       </c>
-      <c r="F27" s="67">
-        <f t="shared" si="8"/>
+      <c r="U17" s="67">
+        <f t="shared" si="0"/>
         <v>-6.5263177824188435E-3</v>
       </c>
-      <c r="G27" s="67">
-        <f t="shared" si="9"/>
+      <c r="V17" s="67">
+        <f t="shared" si="1"/>
         <v>4.3905400058642007E-3</v>
       </c>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-    </row>
-    <row r="28" spans="1:9" ht="17" thickTop="1">
+      <c r="W17" s="67"/>
+      <c r="X17" s="67"/>
+    </row>
+    <row r="18" spans="4:24" ht="17" thickTop="1"/>
+    <row r="28" spans="4:24">
       <c r="D28" s="63"/>
       <c r="E28" s="64"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="4:24">
       <c r="D29" s="63"/>
       <c r="E29" s="64"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="4:24">
       <c r="D30" s="63"/>
       <c r="E30" s="64"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="4:24">
       <c r="D31" s="63"/>
       <c r="E31" s="64"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="4:24">
       <c r="D32" s="63"/>
       <c r="E32" s="64"/>
     </row>
@@ -9244,22 +9219,22 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="130" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="132" t="s">
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="131" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
       <c r="M3" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
fix template scale normalization columns M & N
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3785D82D-1678-7142-9063-ADD568A6369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2467D374-8DC8-CF4C-AC00-00E8DE3CC9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13140" yWindow="500" windowWidth="15660" windowHeight="15880" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -1151,7 +1151,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1374,7 +1374,6 @@
     <xf numFmtId="2" fontId="23" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="24" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="24" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4038,11 +4037,11 @@
       <c r="AP1" s="58"/>
       <c r="AQ1" s="51"/>
       <c r="AR1" s="45"/>
-      <c r="AT1" s="124" t="s">
+      <c r="AT1" s="123" t="s">
         <v>181</v>
       </c>
-      <c r="AU1" s="124"/>
-      <c r="AV1" s="124"/>
+      <c r="AU1" s="123"/>
+      <c r="AV1" s="123"/>
       <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
@@ -4190,13 +4189,13 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="125" t="s">
+      <c r="AT2" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="126" t="s">
+      <c r="AU2" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="127" t="s">
+      <c r="AV2" s="126" t="s">
         <v>34</v>
       </c>
       <c r="AX2" s="39" t="s">
@@ -4362,7 +4361,7 @@
         <f>AJ3*$Y$3</f>
         <v>2.1161148587211971E-3</v>
       </c>
-      <c r="AO3" s="123">
+      <c r="AO3" s="122">
         <v>0</v>
       </c>
       <c r="AP3" s="56">
@@ -4548,7 +4547,7 @@
         <f t="shared" ref="AN4:AN17" si="9">AJ4*$Y$3</f>
         <v>2.09139498425152E-3</v>
       </c>
-      <c r="AO4" s="123">
+      <c r="AO4" s="122">
         <v>0</v>
       </c>
       <c r="AP4" s="56">
@@ -4739,7 +4738,7 @@
         <f t="shared" si="9"/>
         <v>2.1097889665454826E-3</v>
       </c>
-      <c r="AO5" s="123">
+      <c r="AO5" s="122">
         <v>0</v>
       </c>
       <c r="AP5" s="56">
@@ -4934,7 +4933,7 @@
         <f t="shared" si="9"/>
         <v>2.1164798861162187E-3</v>
       </c>
-      <c r="AO6" s="123">
+      <c r="AO6" s="122">
         <v>0</v>
       </c>
       <c r="AP6" s="56">
@@ -5129,7 +5128,7 @@
         <f t="shared" si="9"/>
         <v>2.0917613635465034E-3</v>
       </c>
-      <c r="AO7" s="123">
+      <c r="AO7" s="122">
         <v>0</v>
       </c>
       <c r="AP7" s="56">
@@ -5315,7 +5314,7 @@
         <f t="shared" si="9"/>
         <v>2.1059970799231576E-3</v>
       </c>
-      <c r="AO8" s="123">
+      <c r="AO8" s="122">
         <v>0</v>
       </c>
       <c r="AP8" s="56">
@@ -5504,7 +5503,7 @@
         <f t="shared" si="9"/>
         <v>2.1125489546459449E-3</v>
       </c>
-      <c r="AO9" s="123">
+      <c r="AO9" s="122">
         <v>0</v>
       </c>
       <c r="AP9" s="56">
@@ -5690,7 +5689,7 @@
         <f t="shared" si="9"/>
         <v>2.1110245425008428E-3</v>
       </c>
-      <c r="AO10" s="123">
+      <c r="AO10" s="122">
         <v>0</v>
       </c>
       <c r="AP10" s="56">
@@ -5882,7 +5881,7 @@
         <f t="shared" si="9"/>
         <v>2.11205838421125E-3</v>
       </c>
-      <c r="AO11" s="123">
+      <c r="AO11" s="122">
         <v>0</v>
       </c>
       <c r="AP11" s="56">
@@ -6066,7 +6065,7 @@
         <f t="shared" si="9"/>
         <v>2.0890378267892978E-3</v>
       </c>
-      <c r="AO12" s="123">
+      <c r="AO12" s="122">
         <v>0</v>
       </c>
       <c r="AP12" s="56">
@@ -6250,7 +6249,7 @@
         <f t="shared" si="9"/>
         <v>2.1092446228371492E-3</v>
       </c>
-      <c r="AO13" s="123">
+      <c r="AO13" s="122">
         <v>0</v>
       </c>
       <c r="AP13" s="56">
@@ -6434,7 +6433,7 @@
         <f t="shared" si="9"/>
         <v>2.1118562233900973E-3</v>
       </c>
-      <c r="AO14" s="123">
+      <c r="AO14" s="122">
         <v>0</v>
       </c>
       <c r="AP14" s="56">
@@ -6618,7 +6617,7 @@
         <f t="shared" si="9"/>
         <v>2.1140383039962136E-3</v>
       </c>
-      <c r="AO15" s="123">
+      <c r="AO15" s="122">
         <v>0</v>
       </c>
       <c r="AP15" s="56">
@@ -6802,7 +6801,7 @@
         <f t="shared" si="9"/>
         <v>2.0909357320700551E-3</v>
       </c>
-      <c r="AO16" s="123">
+      <c r="AO16" s="122">
         <v>0</v>
       </c>
       <c r="AP16" s="56">
@@ -6982,7 +6981,7 @@
         <f t="shared" si="9"/>
         <v>2.1099653819650526E-3</v>
       </c>
-      <c r="AO17" s="123">
+      <c r="AO17" s="122">
         <v>0</v>
       </c>
       <c r="AP17" s="56">
@@ -8009,8 +8008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8035,24 +8034,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="127" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="129" t="s">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="128" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
       <c r="O1" s="115" t="s">
         <v>114</v>
       </c>
@@ -8202,11 +8201,11 @@
         <v>ATM_EQ_SW</v>
       </c>
       <c r="Q3" s="68">
-        <f>M3</f>
+        <f t="shared" ref="Q3:R5" si="0">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="R3" s="68">
-        <f>N3</f>
+        <f t="shared" si="0"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="S3" s="111">
@@ -8218,19 +8217,19 @@
         <v>1.0075218399408568</v>
       </c>
       <c r="U3" s="67">
-        <f t="shared" ref="U3:U17" si="0">LN(S3)</f>
+        <f t="shared" ref="U3:U17" si="1">LN(S3)</f>
         <v>5.6690060748599133E-3</v>
       </c>
       <c r="V3" s="67">
-        <f t="shared" ref="V3:V17" si="1">LN(T3)</f>
+        <f t="shared" ref="V3:V17" si="2">LN(T3)</f>
         <v>7.4936919644022753E-3</v>
       </c>
       <c r="W3" s="67">
-        <f t="shared" ref="W3:X10" si="2">LN(Q3)</f>
+        <f t="shared" ref="W3:X9" si="3">LN(Q3)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X3" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.412758119012896E-3</v>
       </c>
       <c r="Y3" s="72">
@@ -8260,7 +8259,7 @@
         <v>32.729999999999997</v>
       </c>
       <c r="F4" s="69">
-        <f t="shared" ref="F4:F9" si="3">B4-C4</f>
+        <f t="shared" ref="F4:F9" si="4">B4-C4</f>
         <v>18.419999999999998</v>
       </c>
       <c r="G4" s="65">
@@ -8300,11 +8299,11 @@
         <v>S2_ref_1</v>
       </c>
       <c r="Q4" s="68">
-        <f>M4</f>
+        <f t="shared" si="0"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="R4" s="68">
-        <f>N4</f>
+        <f t="shared" si="0"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="S4" s="111">
@@ -8316,19 +8315,19 @@
         <v>0.99497700286985102</v>
       </c>
       <c r="U4" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.3157633670658081E-3</v>
       </c>
       <c r="V4" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.0356547842637621E-3</v>
       </c>
       <c r="W4" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X4" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8350,31 +8349,31 @@
         <v>41.949257311111111</v>
       </c>
       <c r="F5" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.25581632613833338</v>
       </c>
       <c r="G5" s="65">
-        <f t="shared" ref="G5:H9" si="4">(B5/1000+1)*0.0036765</f>
+        <f t="shared" ref="G5:H9" si="5">(B5/1000+1)*0.0036765</f>
         <v>3.6750148213719339E-3</v>
       </c>
       <c r="H5" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6759553300949816E-3</v>
       </c>
       <c r="I5" s="65">
-        <f t="shared" ref="I5:I9" si="5">(E5/1000+1)*0.0020052</f>
+        <f t="shared" ref="I5:I9" si="6">(E5/1000+1)*0.0020052</f>
         <v>2.0893166507602399E-3</v>
       </c>
       <c r="J5" s="65">
-        <f t="shared" ref="J5:J9" si="6">(I5/0.0020052)^0.516*0.0003799</f>
+        <f t="shared" ref="J5:J9" si="7">(I5/0.0020052)^0.516*0.0003799</f>
         <v>3.8804145413997107E-4</v>
       </c>
       <c r="K5" s="66">
-        <f t="shared" ref="K5:K9" si="7">G5+H5+J5</f>
+        <f t="shared" ref="K5:K9" si="8">G5+H5+J5</f>
         <v>7.7390116056068863E-3</v>
       </c>
       <c r="L5" s="66">
-        <f t="shared" ref="L5:L9" si="8">(G5+H5)*J5+I5+G5*H5</f>
+        <f t="shared" ref="L5:L9" si="9">(G5+H5)*J5+I5+G5*H5</f>
         <v>2.1056783222279545E-3</v>
       </c>
       <c r="M5" s="67">
@@ -8390,11 +8389,11 @@
         <v>B6_ref_1</v>
       </c>
       <c r="Q5" s="68">
-        <f>M5</f>
+        <f t="shared" si="0"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="R5" s="68">
-        <f>N5</f>
+        <f t="shared" si="0"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="S5" s="111">
@@ -8406,19 +8405,19 @@
         <v>1.0043106480077921</v>
       </c>
       <c r="U5" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8320385549917295E-4</v>
       </c>
       <c r="V5" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3013837783483656E-3</v>
       </c>
       <c r="W5" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="X5" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8433,38 +8432,38 @@
         <v>-49.28</v>
       </c>
       <c r="D6" s="69">
-        <f t="shared" ref="D6:D9" si="9">AVERAGE(B6:C6)</f>
+        <f t="shared" ref="D6:D9" si="10">AVERAGE(B6:C6)</f>
         <v>-35.745000000000005</v>
       </c>
       <c r="E6" s="69">
         <v>26.94</v>
       </c>
       <c r="F6" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27.07</v>
       </c>
       <c r="G6" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5948449350000004E-3</v>
       </c>
       <c r="H6" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.49532208E-3</v>
       </c>
       <c r="I6" s="65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0592200879999997E-3</v>
       </c>
       <c r="J6" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8514702697154833E-4</v>
       </c>
       <c r="K6" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.4753140419715489E-3</v>
       </c>
       <c r="L6" s="66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0745159856220404E-3</v>
       </c>
       <c r="M6" s="67">
@@ -8480,11 +8479,11 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="Q6" s="68">
-        <f>M3</f>
+        <f t="shared" ref="Q6:R8" si="11">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="R6" s="68">
-        <f>N3</f>
+        <f t="shared" si="11"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="S6" s="111">
@@ -8496,19 +8495,19 @@
         <v>1.0077071570383731</v>
       </c>
       <c r="U6" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.3855513126554056E-3</v>
       </c>
       <c r="V6" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6776086292741075E-3</v>
       </c>
       <c r="W6" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X6" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8523,14 +8522,14 @@
         <v>94.44</v>
       </c>
       <c r="D7" s="69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.074999999999996</v>
       </c>
       <c r="E7" s="69">
         <v>36.01</v>
       </c>
       <c r="F7" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-92.73</v>
       </c>
       <c r="G7" s="65">
@@ -8538,23 +8537,23 @@
         <v>3.6827868150000006E-3</v>
       </c>
       <c r="H7" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0237086600000008E-3</v>
       </c>
       <c r="I7" s="65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0774072520000002E-3</v>
       </c>
       <c r="J7" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8689853960154226E-4</v>
       </c>
       <c r="K7" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8.0933940146015442E-3</v>
       </c>
       <c r="L7" s="66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0952073450451725E-3</v>
       </c>
       <c r="M7" s="67">
@@ -8570,11 +8569,11 @@
         <v>S2_ref_2</v>
       </c>
       <c r="Q7" s="68">
-        <f>M4</f>
+        <f t="shared" si="11"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="R7" s="68">
-        <f>N4</f>
+        <f t="shared" si="11"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="S7" s="111">
@@ -8586,19 +8585,19 @@
         <v>0.9951628615034982</v>
       </c>
       <c r="U7" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.3736683280273967E-3</v>
       </c>
       <c r="V7" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.8488753146248009E-3</v>
       </c>
       <c r="W7" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X7" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -8613,38 +8612,38 @@
         <v>-3.43</v>
       </c>
       <c r="D8" s="69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.84</v>
       </c>
       <c r="E8" s="69">
         <v>35.29</v>
       </c>
       <c r="F8" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20.54</v>
       </c>
       <c r="G8" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7394049149999998E-3</v>
       </c>
       <c r="H8" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6638896049999998E-3</v>
       </c>
       <c r="I8" s="65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0759635080000003E-3</v>
       </c>
       <c r="J8" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8675977189798279E-4</v>
       </c>
       <c r="K8" s="66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.7900542918979817E-3</v>
       </c>
       <c r="L8" s="66">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0925275712968031E-3</v>
       </c>
       <c r="M8" s="67">
@@ -8660,11 +8659,11 @@
         <v>B6_ref_2</v>
       </c>
       <c r="Q8" s="68">
-        <f>M5</f>
+        <f t="shared" si="11"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="R8" s="68">
-        <f>N5</f>
+        <f t="shared" si="11"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="S8" s="111">
@@ -8676,19 +8675,19 @@
         <v>1.0023860907979212</v>
       </c>
       <c r="U8" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.2966123175853173E-4</v>
       </c>
       <c r="V8" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3832486035312902E-3</v>
       </c>
       <c r="W8" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="X8" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8703,44 +8702,46 @@
         <v>25.44</v>
       </c>
       <c r="D9" s="119">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>25.585000000000001</v>
       </c>
       <c r="E9" s="119">
         <v>35.880000000000003</v>
       </c>
       <c r="F9" s="119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.28999999999999915</v>
       </c>
       <c r="G9" s="120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7710963450000002E-3</v>
       </c>
       <c r="H9" s="120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7700301599999995E-3</v>
       </c>
       <c r="I9" s="120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0771465759999996E-3</v>
       </c>
       <c r="J9" s="120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8687348777560239E-4</v>
       </c>
       <c r="K9" s="121">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.9279999927756029E-3</v>
       </c>
       <c r="L9" s="121">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0942811848696616E-3</v>
       </c>
-      <c r="M9" s="122">
+      <c r="M9" s="67">
+        <f>K9/size_correction!X$3</f>
         <v>1.0241537838167138</v>
       </c>
-      <c r="N9" s="122">
+      <c r="N9" s="67">
+        <f>L9/size_correction!Y$3</f>
         <v>0.9966620412810443</v>
       </c>
       <c r="P9" s="63" t="str">
@@ -8764,19 +8765,19 @@
         <v>1.0057116133646442</v>
       </c>
       <c r="U9" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0812199816469847E-3</v>
       </c>
       <c r="V9" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.6953639452707308E-3</v>
       </c>
       <c r="W9" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X9" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8809,11 +8810,11 @@
         <v>1.0049378092932522</v>
       </c>
       <c r="U10" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.1141789753790732E-3</v>
       </c>
       <c r="V10" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9256582960658154E-3</v>
       </c>
       <c r="W10" s="67"/>
@@ -8827,11 +8828,11 @@
         <v>ATM_EQ_SW_1</v>
       </c>
       <c r="Q11" s="68">
-        <f>M3</f>
+        <f t="shared" ref="Q11:R13" si="12">M3</f>
         <v>1.0059496767117579</v>
       </c>
       <c r="R11" s="68">
-        <f>N3</f>
+        <f t="shared" si="12"/>
         <v>1.0044225086731247</v>
       </c>
       <c r="S11" s="111">
@@ -8843,19 +8844,19 @@
         <v>1.0054625917600983</v>
       </c>
       <c r="U11" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7029884167436144E-3</v>
       </c>
       <c r="V11" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.4477259185061388E-3</v>
       </c>
       <c r="W11" s="67">
-        <f t="shared" ref="W11:X16" si="10">LN(Q11)</f>
+        <f t="shared" ref="W11:X16" si="13">LN(Q11)</f>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X11" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8867,11 +8868,11 @@
         <v>S2_ref_1</v>
       </c>
       <c r="Q12" s="68">
-        <f>M4</f>
+        <f t="shared" si="12"/>
         <v>0.99629623559207692</v>
       </c>
       <c r="R12" s="68">
-        <f>N4</f>
+        <f t="shared" si="12"/>
         <v>0.99323347721175648</v>
       </c>
       <c r="S12" s="111">
@@ -8883,19 +8884,19 @@
         <v>0.99378130442821833</v>
       </c>
       <c r="U12" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.5945739634335372E-3</v>
       </c>
       <c r="V12" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.2381121983366193E-3</v>
       </c>
       <c r="W12" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X12" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-6.7895195007928941E-3</v>
       </c>
       <c r="Y12"/>
@@ -8907,11 +8908,11 @@
         <v>B6_ref_1</v>
       </c>
       <c r="Q13" s="68">
-        <f>M5</f>
+        <f t="shared" si="12"/>
         <v>0.99973991247556415</v>
       </c>
       <c r="R13" s="68">
-        <f>N5</f>
+        <f t="shared" si="12"/>
         <v>1.0020859042591113</v>
       </c>
       <c r="S13" s="111">
@@ -8923,19 +8924,19 @@
         <v>1.0040343543858852</v>
       </c>
       <c r="U13" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7966870305363727E-4</v>
       </c>
       <c r="V13" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0262381999534996E-3</v>
       </c>
       <c r="W13" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-2.6012135306176113E-4</v>
       </c>
       <c r="X13" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
@@ -8961,19 +8962,19 @@
         <v>1.0053599727245706</v>
       </c>
       <c r="U14" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8686826228146419E-3</v>
       </c>
       <c r="V14" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.3456591947391319E-3</v>
       </c>
       <c r="W14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X14" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -8999,19 +9000,19 @@
         <v>1.0064676550191509</v>
       </c>
       <c r="U15" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6228928832132777E-3</v>
       </c>
       <c r="V15" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.446829485110093E-3</v>
       </c>
       <c r="W15" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.9320472770020231E-3</v>
       </c>
       <c r="X15" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.412758119012896E-3</v>
       </c>
     </row>
@@ -9037,19 +9038,19 @@
         <v>0.99474403428411884</v>
       </c>
       <c r="U16" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.6734640658408848E-3</v>
       </c>
       <c r="V16" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.2698268942697113E-3</v>
       </c>
       <c r="W16" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-3.7106403264231301E-3</v>
       </c>
       <c r="X16" s="67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
@@ -9069,11 +9070,11 @@
         <v>1.0044001925480899</v>
       </c>
       <c r="U17" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.5263177824188435E-3</v>
       </c>
       <c r="V17" s="67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3905400058642007E-3</v>
       </c>
       <c r="W17" s="67"/>
@@ -9219,22 +9220,22 @@
       <c r="S2" s="78"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="129" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="131" t="s">
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="130" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
-      <c r="J3" s="131"/>
-      <c r="K3" s="131"/>
-      <c r="L3" s="131"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
       <c r="M3" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
add version 3 of data corrections template with intercept for scale normalization
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v2.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2467D374-8DC8-CF4C-AC00-00E8DE3CC9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568945C6-AB5A-884F-9202-39267D1080B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="500" windowWidth="15660" windowHeight="15880" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="15660" windowHeight="15880" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="185">
   <si>
     <t>corrected to m/z=44 peak area of 20 Vs</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>USER INPUTS:</t>
-  </si>
-  <si>
-    <t>SCALE NORMALIZATION 𝜆</t>
   </si>
   <si>
     <t>scale decompressed 45rR/45rR</t>
@@ -613,6 +610,18 @@
   </si>
   <si>
     <t>SCRAMBLING OUTPUT: CHECK VALUES</t>
+  </si>
+  <si>
+    <t>𝜆</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>SCALE NORMALIZATION FACTORS</t>
+  </si>
+  <si>
+    <t>coefficient</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1160,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1297,7 +1306,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1"/>
@@ -1393,6 +1401,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -3977,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AQ12" sqref="AQ12"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4025,11 +4035,11 @@
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
       <c r="AI1" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AJ1" s="74"/>
       <c r="AL1" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AM1" s="51"/>
       <c r="AN1" s="51"/>
@@ -4037,11 +4047,11 @@
       <c r="AP1" s="58"/>
       <c r="AQ1" s="51"/>
       <c r="AR1" s="45"/>
-      <c r="AT1" s="123" t="s">
-        <v>181</v>
-      </c>
-      <c r="AU1" s="123"/>
-      <c r="AV1" s="123"/>
+      <c r="AT1" s="122" t="s">
+        <v>180</v>
+      </c>
+      <c r="AU1" s="122"/>
+      <c r="AV1" s="122"/>
       <c r="AX1" s="38" t="s">
         <v>91</v>
       </c>
@@ -4054,17 +4064,17 @@
       <c r="BC1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="BE1" s="103" t="s">
-        <v>162</v>
-      </c>
-      <c r="BF1" s="103"/>
-      <c r="BG1" s="103"/>
-      <c r="BH1" s="103"/>
-      <c r="BI1" s="104"/>
-      <c r="BJ1" s="105"/>
-      <c r="BK1" s="105"/>
-      <c r="BL1" s="105"/>
-      <c r="BM1" s="105"/>
+      <c r="BE1" s="102" t="s">
+        <v>161</v>
+      </c>
+      <c r="BF1" s="102"/>
+      <c r="BG1" s="102"/>
+      <c r="BH1" s="102"/>
+      <c r="BI1" s="103"/>
+      <c r="BJ1" s="104"/>
+      <c r="BK1" s="104"/>
+      <c r="BL1" s="104"/>
+      <c r="BM1" s="104"/>
     </row>
     <row r="2" spans="1:65" ht="52" thickBot="1">
       <c r="A2" s="8" t="s">
@@ -4159,10 +4169,10 @@
         <v>27</v>
       </c>
       <c r="AI2" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ2" s="75" t="s">
         <v>119</v>
-      </c>
-      <c r="AJ2" s="75" t="s">
-        <v>120</v>
       </c>
       <c r="AK2" s="23"/>
       <c r="AL2" s="55" t="s">
@@ -4175,7 +4185,7 @@
         <v>30</v>
       </c>
       <c r="AO2" s="52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AP2" s="59" t="s">
         <v>94</v>
@@ -4189,13 +4199,13 @@
       <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AT2" s="124" t="s">
+      <c r="AT2" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="125" t="s">
+      <c r="AU2" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="126" t="s">
+      <c r="AV2" s="125" t="s">
         <v>34</v>
       </c>
       <c r="AX2" s="39" t="s">
@@ -4217,32 +4227,32 @@
         <v>34</v>
       </c>
       <c r="BD2" s="44"/>
-      <c r="BE2" s="106" t="s">
+      <c r="BE2" s="105" t="s">
+        <v>162</v>
+      </c>
+      <c r="BF2" s="105" t="s">
         <v>163</v>
       </c>
-      <c r="BF2" s="106" t="s">
+      <c r="BG2" s="105" t="s">
         <v>164</v>
       </c>
-      <c r="BG2" s="106" t="s">
+      <c r="BH2" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="BH2" s="106" t="s">
+      <c r="BI2" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="BI2" s="107" t="s">
+      <c r="BJ2" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="BJ2" s="108" t="s">
+      <c r="BK2" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="BK2" s="109" t="s">
+      <c r="BL2" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="BL2" s="108" t="s">
-        <v>170</v>
-      </c>
-      <c r="BM2" s="110" t="s">
-        <v>169</v>
+      <c r="BM2" s="109" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:65" ht="17" thickBot="1">
@@ -4341,12 +4351,12 @@
         <v>1.0075218399408568</v>
       </c>
       <c r="AI3" s="76">
-        <f>AF3^$X$11</f>
-        <v>1.0060158448599359</v>
-      </c>
-      <c r="AJ3" s="77">
-        <f>AG3^$Y$11</f>
-        <v>1.0070526202093892</v>
+        <f>AF3^$X$11*EXP(X$12)</f>
+        <v>1.0059968914794004</v>
+      </c>
+      <c r="AJ3" s="76">
+        <f>AG3^$Y$11*EXP(Y$12)</f>
+        <v>1.0054928361918907</v>
       </c>
       <c r="AK3" s="32"/>
       <c r="AL3" s="33">
@@ -4355,13 +4365,13 @@
       </c>
       <c r="AM3" s="33">
         <f>AI3*$X$3</f>
-        <v>7.787593754776452E-3</v>
+        <v>7.7874470361848479E-3</v>
       </c>
       <c r="AN3" s="33">
         <f>AJ3*$Y$3</f>
-        <v>2.1161148587211971E-3</v>
-      </c>
-      <c r="AO3" s="122">
+        <v>2.1128372920185372E-3</v>
+      </c>
+      <c r="AO3" s="121">
         <v>0</v>
       </c>
       <c r="AP3" s="56">
@@ -4417,9 +4427,9 @@
         <v>156</v>
       </c>
       <c r="BH3" t="s">
-        <v>171</v>
-      </c>
-      <c r="BI3" s="78">
+        <v>170</v>
+      </c>
+      <c r="BI3" s="77">
         <f>BG3*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
@@ -4527,12 +4537,12 @@
         <v>0.99497700286985102</v>
       </c>
       <c r="AI4" s="76">
-        <f t="shared" ref="AI4:AI17" si="5">AF4^$X$11</f>
-        <v>0.99649806061376012</v>
-      </c>
-      <c r="AJ4" s="77">
-        <f t="shared" ref="AJ4:AJ17" si="6">AG4^$Y$11</f>
-        <v>0.99528850719192319</v>
+        <f t="shared" ref="AI4:AI54" si="5">AF4^$X$11*EXP(X$12)</f>
+        <v>0.99647928654867735</v>
+      </c>
+      <c r="AJ4" s="76">
+        <f t="shared" ref="AJ4:AJ54" si="6">AG4^$Y$11*EXP(Y$12)</f>
+        <v>0.99374694414430875</v>
       </c>
       <c r="AK4" s="32"/>
       <c r="AL4" s="33">
@@ -4541,13 +4551,13 @@
       </c>
       <c r="AM4" s="33">
         <f t="shared" ref="AM4:AM17" si="8">AI4*$X$3</f>
-        <v>7.7139163494616804E-3</v>
+        <v>7.7137710189554686E-3</v>
       </c>
       <c r="AN4" s="33">
         <f t="shared" ref="AN4:AN17" si="9">AJ4*$Y$3</f>
-        <v>2.09139498425152E-3</v>
-      </c>
-      <c r="AO4" s="122">
+        <v>2.0881557051858103E-3</v>
+      </c>
+      <c r="AO4" s="121">
         <v>0</v>
       </c>
       <c r="AP4" s="56">
@@ -4605,7 +4615,7 @@
       <c r="BH4" t="s">
         <v>39</v>
       </c>
-      <c r="BI4" s="78">
+      <c r="BI4" s="77">
         <f>BG4*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -4719,11 +4729,11 @@
       </c>
       <c r="AI5" s="76">
         <f t="shared" si="5"/>
-        <v>1.0004055127886835</v>
-      </c>
-      <c r="AJ5" s="77">
+        <v>1.0003866651070386</v>
+      </c>
+      <c r="AJ5" s="76">
         <f t="shared" si="6"/>
-        <v>1.0040421473777938</v>
+        <v>1.0024870261627283</v>
       </c>
       <c r="AK5" s="32"/>
       <c r="AL5" s="33">
@@ -4732,13 +4742,13 @@
       </c>
       <c r="AM5" s="33">
         <f t="shared" si="8"/>
-        <v>7.7441640342372194E-3</v>
+        <v>7.7440181338633632E-3</v>
       </c>
       <c r="AN5" s="33">
         <f t="shared" si="9"/>
-        <v>2.1097889665454826E-3</v>
-      </c>
-      <c r="AO5" s="122">
+        <v>2.1065211977672944E-3</v>
+      </c>
+      <c r="AO5" s="121">
         <v>0</v>
       </c>
       <c r="AP5" s="56">
@@ -4796,7 +4806,7 @@
       <c r="BH5" t="s">
         <v>39</v>
       </c>
-      <c r="BI5" s="78">
+      <c r="BI5" s="77">
         <f>BG5*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -4914,11 +4924,11 @@
       </c>
       <c r="AI6" s="76">
         <f t="shared" si="5"/>
-        <v>1.0067788012419414</v>
-      </c>
-      <c r="AJ6" s="77">
+        <v>1.0067598334872758</v>
+      </c>
+      <c r="AJ6" s="76">
         <f t="shared" si="6"/>
-        <v>1.0072263356356053</v>
+        <v>1.0056662825571459</v>
       </c>
       <c r="AK6" s="32"/>
       <c r="AL6" s="33">
@@ -4927,13 +4937,13 @@
       </c>
       <c r="AM6" s="33">
         <f t="shared" si="8"/>
-        <v>7.7934998191650307E-3</v>
+        <v>7.793352989302926E-3</v>
       </c>
       <c r="AN6" s="33">
         <f t="shared" si="9"/>
-        <v>2.1164798861162187E-3</v>
-      </c>
-      <c r="AO6" s="122">
+        <v>2.1132017540370475E-3</v>
+      </c>
+      <c r="AO6" s="121">
         <v>0</v>
       </c>
       <c r="AP6" s="56">
@@ -4989,9 +4999,9 @@
         <v>156</v>
       </c>
       <c r="BH6" t="s">
-        <v>171</v>
-      </c>
-      <c r="BI6" s="78">
+        <v>170</v>
+      </c>
+      <c r="BI6" s="77">
         <f>BG6*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
@@ -5109,11 +5119,11 @@
       </c>
       <c r="AI7" s="76">
         <f t="shared" si="5"/>
-        <v>0.99643701343870184</v>
-      </c>
-      <c r="AJ7" s="77">
+        <v>0.99641824052375039</v>
+      </c>
+      <c r="AJ7" s="76">
         <f t="shared" si="6"/>
-        <v>0.99546286598321598</v>
+        <v>0.99392103287815814</v>
       </c>
       <c r="AK7" s="32"/>
       <c r="AL7" s="33">
@@ -5122,13 +5132,13 @@
       </c>
       <c r="AM7" s="33">
         <f t="shared" si="8"/>
-        <v>7.7134437817564508E-3</v>
+        <v>7.713298460153434E-3</v>
       </c>
       <c r="AN7" s="33">
         <f t="shared" si="9"/>
-        <v>2.0917613635465034E-3</v>
-      </c>
-      <c r="AO7" s="122">
+        <v>2.0885215170103784E-3</v>
+      </c>
+      <c r="AO7" s="121">
         <v>0</v>
       </c>
       <c r="AP7" s="56">
@@ -5186,7 +5196,7 @@
       <c r="BH7" t="s">
         <v>39</v>
       </c>
-      <c r="BI7" s="78">
+      <c r="BI7" s="77">
         <f>BG7*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -5295,11 +5305,11 @@
       </c>
       <c r="AI8" s="76">
         <f t="shared" si="5"/>
-        <v>0.99912260158268462</v>
-      </c>
-      <c r="AJ8" s="77">
+        <v>0.99910377807114037</v>
+      </c>
+      <c r="AJ8" s="76">
         <f t="shared" si="6"/>
-        <v>1.0022376000760198</v>
+        <v>1.0006852738529772</v>
       </c>
       <c r="AK8" s="32"/>
       <c r="AL8" s="33">
@@ -5308,13 +5318,13 @@
       </c>
       <c r="AM8" s="33">
         <f t="shared" si="8"/>
-        <v>7.7342329865834319E-3</v>
+        <v>7.7340872733109283E-3</v>
       </c>
       <c r="AN8" s="33">
         <f t="shared" si="9"/>
-        <v>2.1059970799231576E-3</v>
-      </c>
-      <c r="AO8" s="122">
+        <v>2.1027351842483515E-3</v>
+      </c>
+      <c r="AO8" s="121">
         <v>0</v>
       </c>
       <c r="AP8" s="56">
@@ -5372,7 +5382,7 @@
       <c r="BH8" t="s">
         <v>39</v>
       </c>
-      <c r="BI8" s="78">
+      <c r="BI8" s="77">
         <f>BG8*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -5455,9 +5465,10 @@
       <c r="U9" s="24">
         <v>0.42850050000000001</v>
       </c>
-      <c r="X9" s="71" t="s">
-        <v>118</v>
-      </c>
+      <c r="W9" s="71" t="s">
+        <v>183</v>
+      </c>
+      <c r="X9" s="2"/>
       <c r="Y9" s="3"/>
       <c r="AA9" s="28">
         <f t="shared" si="1"/>
@@ -5485,11 +5496,11 @@
       </c>
       <c r="AI9" s="76">
         <f t="shared" si="5"/>
-        <v>1.0053904191368781</v>
-      </c>
-      <c r="AJ9" s="77">
+        <v>1.0053714775393894</v>
+      </c>
+      <c r="AJ9" s="76">
         <f t="shared" si="6"/>
-        <v>1.0053556173139186</v>
+        <v>1.0037984617171607</v>
       </c>
       <c r="AL9" s="33">
         <f t="shared" si="7"/>
@@ -5497,13 +5508,13 @@
       </c>
       <c r="AM9" s="33">
         <f t="shared" si="8"/>
-        <v>7.7827523186501267E-3</v>
+        <v>7.7826056912713801E-3</v>
       </c>
       <c r="AN9" s="33">
         <f t="shared" si="9"/>
-        <v>2.1125489546459449E-3</v>
-      </c>
-      <c r="AO9" s="122">
+        <v>2.1092769110312277E-3</v>
+      </c>
+      <c r="AO9" s="121">
         <v>0</v>
       </c>
       <c r="AP9" s="56">
@@ -5558,9 +5569,9 @@
         <v>156</v>
       </c>
       <c r="BH9" t="s">
-        <v>171</v>
-      </c>
-      <c r="BI9" s="78">
+        <v>170</v>
+      </c>
+      <c r="BI9" s="77">
         <f>BG9*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
@@ -5639,7 +5650,10 @@
       <c r="U10" s="24">
         <v>0.42850440000000001</v>
       </c>
-      <c r="X10" s="15" t="s">
+      <c r="W10" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="X10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="Y10" s="17" t="s">
@@ -5671,11 +5685,11 @@
       </c>
       <c r="AI10" s="76">
         <f t="shared" si="5"/>
-        <v>0.99040351990487752</v>
-      </c>
-      <c r="AJ10" s="77">
+        <v>0.99038486066119624</v>
+      </c>
+      <c r="AJ10" s="76">
         <f t="shared" si="6"/>
-        <v>1.0046301542140887</v>
+        <v>1.0030741222584652</v>
       </c>
       <c r="AL10" s="33">
         <f t="shared" si="7"/>
@@ -5683,13 +5697,13 @@
       </c>
       <c r="AM10" s="33">
         <f t="shared" si="8"/>
-        <v>7.6667383577777295E-3</v>
+        <v>7.666593916106852E-3</v>
       </c>
       <c r="AN10" s="33">
         <f t="shared" si="9"/>
-        <v>2.1110245425008428E-3</v>
-      </c>
-      <c r="AO10" s="122">
+        <v>2.107754859987872E-3</v>
+      </c>
+      <c r="AO10" s="121">
         <v>0</v>
       </c>
       <c r="AP10" s="56">
@@ -5746,7 +5760,7 @@
       <c r="BH10" t="s">
         <v>39</v>
       </c>
-      <c r="BI10" s="78">
+      <c r="BI10" s="77">
         <f>BG10*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -5767,7 +5781,7 @@
         <v>2.386599244350319</v>
       </c>
     </row>
-    <row r="11" spans="1:65" ht="17" thickBot="1">
+    <row r="11" spans="1:65">
       <c r="A11">
         <v>201207</v>
       </c>
@@ -5829,11 +5843,14 @@
       <c r="U11">
         <v>0.42918780000000001</v>
       </c>
-      <c r="X11" s="34">
+      <c r="W11" s="130" t="s">
+        <v>181</v>
+      </c>
+      <c r="X11">
         <f>scale_normalization!Y3</f>
         <v>1.058002378564959</v>
       </c>
-      <c r="Y11" s="36">
+      <c r="Y11" s="131">
         <f>scale_normalization!Z3</f>
         <v>0.9378376950888252</v>
       </c>
@@ -5863,11 +5880,11 @@
       </c>
       <c r="AI11" s="76">
         <f t="shared" si="5"/>
-        <v>1.0060520151987653</v>
-      </c>
-      <c r="AJ11" s="77">
+        <v>1.0060330611367791</v>
+      </c>
+      <c r="AJ11" s="76">
         <f t="shared" si="6"/>
-        <v>1.0051221563372517</v>
+        <v>1.0035653623389771</v>
       </c>
       <c r="AL11" s="33">
         <f t="shared" si="7"/>
@@ -5875,13 +5892,13 @@
       </c>
       <c r="AM11" s="33">
         <f t="shared" si="8"/>
-        <v>7.7878737502717673E-3</v>
+        <v>7.7877270264050356E-3</v>
       </c>
       <c r="AN11" s="33">
         <f t="shared" si="9"/>
-        <v>2.11205838421125E-3</v>
-      </c>
-      <c r="AO11" s="122">
+        <v>2.1087871004216979E-3</v>
+      </c>
+      <c r="AO11" s="121">
         <v>0</v>
       </c>
       <c r="AP11" s="56">
@@ -5936,9 +5953,9 @@
         <v>156</v>
       </c>
       <c r="BH11" t="s">
-        <v>171</v>
-      </c>
-      <c r="BI11" s="78">
+        <v>170</v>
+      </c>
+      <c r="BI11" s="77">
         <f>BG11*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
@@ -5959,7 +5976,7 @@
         <v>2.151751302319628</v>
       </c>
     </row>
-    <row r="12" spans="1:65">
+    <row r="12" spans="1:65" ht="17" thickBot="1">
       <c r="A12">
         <v>201207</v>
       </c>
@@ -6021,6 +6038,17 @@
       <c r="U12">
         <v>0.42925489999999999</v>
       </c>
+      <c r="W12" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="X12" s="35">
+        <f>scale_normalization!Y4</f>
+        <v>-1.8840219242949102E-5</v>
+      </c>
+      <c r="Y12" s="36">
+        <f>scale_normalization!Z4</f>
+        <v>-1.5500612170959347E-3</v>
+      </c>
       <c r="AA12" s="28">
         <f t="shared" si="1"/>
         <v>0.99606571006022826</v>
@@ -6047,11 +6075,11 @@
       </c>
       <c r="AI12" s="76">
         <f t="shared" si="5"/>
-        <v>0.99620415470032642</v>
-      </c>
-      <c r="AJ12" s="77">
+        <v>0.99618538617244334</v>
+      </c>
+      <c r="AJ12" s="76">
         <f t="shared" si="6"/>
-        <v>0.9941667431303961</v>
+        <v>0.99262691753881871</v>
       </c>
       <c r="AL12" s="33">
         <f t="shared" si="7"/>
@@ -6059,13 +6087,13 @@
       </c>
       <c r="AM12" s="33">
         <f t="shared" si="8"/>
-        <v>7.7116412164529484E-3</v>
+        <v>7.7114959288103382E-3</v>
       </c>
       <c r="AN12" s="33">
         <f t="shared" si="9"/>
-        <v>2.0890378267892978E-3</v>
-      </c>
-      <c r="AO12" s="122">
+        <v>2.0858021986316566E-3</v>
+      </c>
+      <c r="AO12" s="121">
         <v>0</v>
       </c>
       <c r="AP12" s="56">
@@ -6122,7 +6150,7 @@
       <c r="BH12" t="s">
         <v>39</v>
       </c>
-      <c r="BI12" s="78">
+      <c r="BI12" s="77">
         <f>BG12*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -6231,11 +6259,11 @@
       </c>
       <c r="AI13" s="76">
         <f t="shared" si="5"/>
-        <v>1.0001901079834172</v>
-      </c>
-      <c r="AJ13" s="77">
+        <v>1.0001712643600078</v>
+      </c>
+      <c r="AJ13" s="76">
         <f t="shared" si="6"/>
-        <v>1.003783095863878</v>
+        <v>1.002228375883468</v>
       </c>
       <c r="AL13" s="33">
         <f t="shared" si="7"/>
@@ -6243,13 +6271,13 @@
       </c>
       <c r="AM13" s="33">
         <f t="shared" si="8"/>
-        <v>7.742496580265385E-3</v>
+        <v>7.7423507113064316E-3</v>
       </c>
       <c r="AN13" s="33">
         <f t="shared" si="9"/>
-        <v>2.1092446228371492E-3</v>
-      </c>
-      <c r="AO13" s="122">
+        <v>2.1059776971714254E-3</v>
+      </c>
+      <c r="AO13" s="121">
         <v>0</v>
       </c>
       <c r="AP13" s="56">
@@ -6306,7 +6334,7 @@
       <c r="BH13" t="s">
         <v>39</v>
       </c>
-      <c r="BI13" s="78">
+      <c r="BI13" s="77">
         <f>BG13*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -6415,11 +6443,11 @@
       </c>
       <c r="AI14" s="76">
         <f t="shared" si="5"/>
-        <v>1.0051643674054496</v>
-      </c>
-      <c r="AJ14" s="77">
+        <v>1.0051454300667848</v>
+      </c>
+      <c r="AJ14" s="76">
         <f t="shared" si="6"/>
-        <v>1.0050259486178046</v>
+        <v>1.0034693036318658</v>
       </c>
       <c r="AL14" s="33">
         <f t="shared" si="7"/>
@@ -6427,13 +6455,13 @@
       </c>
       <c r="AM14" s="33">
         <f t="shared" si="8"/>
-        <v>7.7810024465572326E-3</v>
+        <v>7.7808558521461494E-3</v>
       </c>
       <c r="AN14" s="33">
         <f t="shared" si="9"/>
-        <v>2.1118562233900973E-3</v>
-      </c>
-      <c r="AO14" s="122">
+        <v>2.1085852527194544E-3</v>
+      </c>
+      <c r="AO14" s="121">
         <v>0</v>
       </c>
       <c r="AP14" s="56">
@@ -6488,9 +6516,9 @@
         <v>156</v>
       </c>
       <c r="BH14" t="s">
-        <v>171</v>
-      </c>
-      <c r="BI14" s="78">
+        <v>170</v>
+      </c>
+      <c r="BI14" s="77">
         <f>BG14*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
@@ -6599,11 +6627,11 @@
       </c>
       <c r="AI15" s="76">
         <f t="shared" si="5"/>
-        <v>1.005966764690523</v>
-      </c>
-      <c r="AJ15" s="77">
+        <v>1.0059478122346599</v>
+      </c>
+      <c r="AJ15" s="76">
         <f t="shared" si="6"/>
-        <v>1.006064394136412</v>
+        <v>1.0045061407432356</v>
       </c>
       <c r="AL15" s="33">
         <f t="shared" si="7"/>
@@ -6611,13 +6639,13 @@
       </c>
       <c r="AM15" s="33">
         <f t="shared" si="8"/>
-        <v>7.7872138239604956E-3</v>
+        <v>7.7870671125268029E-3</v>
       </c>
       <c r="AN15" s="33">
         <f t="shared" si="9"/>
-        <v>2.1140383039962136E-3</v>
-      </c>
-      <c r="AO15" s="122">
+        <v>2.110763953587128E-3</v>
+      </c>
+      <c r="AO15" s="121">
         <v>0</v>
       </c>
       <c r="AP15" s="56">
@@ -6672,9 +6700,9 @@
         <v>156</v>
       </c>
       <c r="BH15" t="s">
-        <v>171</v>
-      </c>
-      <c r="BI15" s="78">
+        <v>170</v>
+      </c>
+      <c r="BI15" s="77">
         <f>BG15*concentration_constants!$B$6</f>
         <v>0.15204678362573099</v>
       </c>
@@ -6783,11 +6811,11 @@
       </c>
       <c r="AI16" s="76">
         <f t="shared" si="5"/>
-        <v>0.99612100907800016</v>
-      </c>
-      <c r="AJ16" s="77">
+        <v>0.99610224211658405</v>
+      </c>
+      <c r="AJ16" s="76">
         <f t="shared" si="6"/>
-        <v>0.99506995047664126</v>
+        <v>0.99352872594288855</v>
       </c>
       <c r="AL16" s="33">
         <f t="shared" si="7"/>
@@ -6795,13 +6823,13 @@
       </c>
       <c r="AM16" s="33">
         <f t="shared" si="8"/>
-        <v>7.7109975841160696E-3</v>
+        <v>7.7108523085995181E-3</v>
       </c>
       <c r="AN16" s="33">
         <f t="shared" si="9"/>
-        <v>2.0909357320700551E-3</v>
-      </c>
-      <c r="AO16" s="122">
+        <v>2.0876971643219054E-3</v>
+      </c>
+      <c r="AO16" s="121">
         <v>0</v>
       </c>
       <c r="AP16" s="56">
@@ -6858,7 +6886,7 @@
       <c r="BH16" t="s">
         <v>39</v>
       </c>
-      <c r="BI16" s="78">
+      <c r="BI16" s="77">
         <f>BG16*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -6963,11 +6991,11 @@
       </c>
       <c r="AI17" s="76">
         <f t="shared" si="5"/>
-        <v>0.99311892403423885</v>
-      </c>
-      <c r="AJ17" s="77">
+        <v>0.99310021363223033</v>
+      </c>
+      <c r="AJ17" s="76">
         <f t="shared" si="6"/>
-        <v>1.0041261029389918</v>
+        <v>1.0025708516884744</v>
       </c>
       <c r="AL17" s="33">
         <f t="shared" si="7"/>
@@ -6975,13 +7003,13 @@
       </c>
       <c r="AM17" s="33">
         <f t="shared" si="8"/>
-        <v>7.6877583688914237E-3</v>
+        <v>7.6876135312026585E-3</v>
       </c>
       <c r="AN17" s="33">
         <f t="shared" si="9"/>
-        <v>2.1099653819650526E-3</v>
-      </c>
-      <c r="AO17" s="122">
+        <v>2.1066973399439907E-3</v>
+      </c>
+      <c r="AO17" s="121">
         <v>0</v>
       </c>
       <c r="AP17" s="56">
@@ -7038,7 +7066,7 @@
       <c r="BH17" t="s">
         <v>39</v>
       </c>
-      <c r="BI17" s="78">
+      <c r="BI17" s="77">
         <f>BG17*concentration_constants!$F$6</f>
         <v>0.15628130635143259</v>
       </c>
@@ -7084,8 +7112,8 @@
       <c r="AE18" s="31"/>
       <c r="AF18" s="31"/>
       <c r="AG18" s="31"/>
-      <c r="AI18" s="74"/>
-      <c r="AJ18" s="74"/>
+      <c r="AI18" s="76"/>
+      <c r="AJ18" s="76"/>
       <c r="AL18" s="33"/>
       <c r="AM18" s="33"/>
       <c r="AN18" s="33"/>
@@ -7126,8 +7154,8 @@
       <c r="AE19" s="31"/>
       <c r="AF19" s="31"/>
       <c r="AG19" s="31"/>
-      <c r="AI19" s="74"/>
-      <c r="AJ19" s="74"/>
+      <c r="AI19" s="76"/>
+      <c r="AJ19" s="76"/>
       <c r="AL19" s="33"/>
       <c r="AM19" s="33"/>
       <c r="AN19" s="33"/>
@@ -7168,8 +7196,8 @@
       <c r="AE20" s="31"/>
       <c r="AF20" s="31"/>
       <c r="AG20" s="31"/>
-      <c r="AI20" s="74"/>
-      <c r="AJ20" s="74"/>
+      <c r="AI20" s="76"/>
+      <c r="AJ20" s="76"/>
       <c r="AL20" s="33"/>
       <c r="AM20" s="33"/>
       <c r="AN20" s="33"/>
@@ -7210,8 +7238,8 @@
       <c r="AE21" s="31"/>
       <c r="AF21" s="31"/>
       <c r="AG21" s="31"/>
-      <c r="AI21" s="74"/>
-      <c r="AJ21" s="74"/>
+      <c r="AI21" s="76"/>
+      <c r="AJ21" s="76"/>
       <c r="AL21" s="33"/>
       <c r="AM21" s="33"/>
       <c r="AN21" s="33"/>
@@ -7252,8 +7280,8 @@
       <c r="AE22" s="31"/>
       <c r="AF22" s="31"/>
       <c r="AG22" s="31"/>
-      <c r="AI22" s="74"/>
-      <c r="AJ22" s="74"/>
+      <c r="AI22" s="76"/>
+      <c r="AJ22" s="76"/>
       <c r="AL22" s="33"/>
       <c r="AM22" s="33"/>
       <c r="AN22" s="33"/>
@@ -7294,8 +7322,8 @@
       <c r="AE23" s="31"/>
       <c r="AF23" s="31"/>
       <c r="AG23" s="31"/>
-      <c r="AI23" s="74"/>
-      <c r="AJ23" s="74"/>
+      <c r="AI23" s="76"/>
+      <c r="AJ23" s="76"/>
       <c r="AL23" s="33"/>
       <c r="AM23" s="33"/>
       <c r="AN23" s="33"/>
@@ -7336,8 +7364,8 @@
       <c r="AE24" s="31"/>
       <c r="AF24" s="31"/>
       <c r="AG24" s="31"/>
-      <c r="AI24" s="74"/>
-      <c r="AJ24" s="74"/>
+      <c r="AI24" s="76"/>
+      <c r="AJ24" s="76"/>
       <c r="AL24" s="33"/>
       <c r="AM24" s="33"/>
       <c r="AN24" s="33"/>
@@ -7378,8 +7406,8 @@
       <c r="AE25" s="31"/>
       <c r="AF25" s="31"/>
       <c r="AG25" s="31"/>
-      <c r="AI25" s="74"/>
-      <c r="AJ25" s="74"/>
+      <c r="AI25" s="76"/>
+      <c r="AJ25" s="76"/>
       <c r="AL25" s="33"/>
       <c r="AM25" s="33"/>
       <c r="AN25" s="33"/>
@@ -7420,8 +7448,8 @@
       <c r="AE26" s="31"/>
       <c r="AF26" s="31"/>
       <c r="AG26" s="31"/>
-      <c r="AI26" s="74"/>
-      <c r="AJ26" s="74"/>
+      <c r="AI26" s="76"/>
+      <c r="AJ26" s="76"/>
       <c r="AL26" s="33"/>
       <c r="AM26" s="33"/>
       <c r="AN26" s="33"/>
@@ -7462,8 +7490,8 @@
       <c r="AE27" s="31"/>
       <c r="AF27" s="31"/>
       <c r="AG27" s="31"/>
-      <c r="AI27" s="74"/>
-      <c r="AJ27" s="74"/>
+      <c r="AI27" s="76"/>
+      <c r="AJ27" s="76"/>
       <c r="AL27" s="33"/>
       <c r="AM27" s="33"/>
       <c r="AN27" s="33"/>
@@ -7504,8 +7532,8 @@
       <c r="AE28" s="31"/>
       <c r="AF28" s="31"/>
       <c r="AG28" s="31"/>
-      <c r="AI28" s="74"/>
-      <c r="AJ28" s="74"/>
+      <c r="AI28" s="76"/>
+      <c r="AJ28" s="76"/>
       <c r="AL28" s="33"/>
       <c r="AM28" s="33"/>
       <c r="AN28" s="33"/>
@@ -7546,8 +7574,8 @@
       <c r="AE29" s="31"/>
       <c r="AF29" s="31"/>
       <c r="AG29" s="31"/>
-      <c r="AI29" s="74"/>
-      <c r="AJ29" s="74"/>
+      <c r="AI29" s="76"/>
+      <c r="AJ29" s="76"/>
       <c r="AL29" s="33"/>
       <c r="AM29" s="33"/>
       <c r="AN29" s="33"/>
@@ -7588,8 +7616,8 @@
       <c r="AE30" s="31"/>
       <c r="AF30" s="31"/>
       <c r="AG30" s="31"/>
-      <c r="AI30" s="74"/>
-      <c r="AJ30" s="74"/>
+      <c r="AI30" s="76"/>
+      <c r="AJ30" s="76"/>
       <c r="AL30" s="33"/>
       <c r="AM30" s="33"/>
       <c r="AN30" s="33"/>
@@ -7630,8 +7658,8 @@
       <c r="AE31" s="31"/>
       <c r="AF31" s="31"/>
       <c r="AG31" s="31"/>
-      <c r="AI31" s="74"/>
-      <c r="AJ31" s="74"/>
+      <c r="AI31" s="76"/>
+      <c r="AJ31" s="76"/>
       <c r="AL31" s="33"/>
       <c r="AM31" s="33"/>
       <c r="AN31" s="33"/>
@@ -7670,8 +7698,8 @@
       <c r="AE32" s="31"/>
       <c r="AF32" s="31"/>
       <c r="AG32" s="31"/>
-      <c r="AI32" s="74"/>
-      <c r="AJ32" s="74"/>
+      <c r="AI32" s="76"/>
+      <c r="AJ32" s="76"/>
       <c r="AL32" s="33"/>
       <c r="AM32" s="33"/>
       <c r="AN32" s="33"/>
@@ -7698,8 +7726,8 @@
       <c r="AE33" s="31"/>
       <c r="AF33" s="31"/>
       <c r="AG33" s="31"/>
-      <c r="AI33" s="74"/>
-      <c r="AJ33" s="74"/>
+      <c r="AI33" s="76"/>
+      <c r="AJ33" s="76"/>
       <c r="AL33" s="33"/>
       <c r="AM33" s="33"/>
       <c r="AN33" s="33"/>
@@ -7726,8 +7754,8 @@
       <c r="AE34" s="31"/>
       <c r="AF34" s="31"/>
       <c r="AG34" s="31"/>
-      <c r="AI34" s="74"/>
-      <c r="AJ34" s="74"/>
+      <c r="AI34" s="76"/>
+      <c r="AJ34" s="76"/>
       <c r="AL34" s="33"/>
       <c r="AM34" s="33"/>
       <c r="AN34" s="33"/>
@@ -7754,8 +7782,8 @@
       <c r="AE35" s="31"/>
       <c r="AF35" s="31"/>
       <c r="AG35" s="31"/>
-      <c r="AI35" s="74"/>
-      <c r="AJ35" s="74"/>
+      <c r="AI35" s="76"/>
+      <c r="AJ35" s="76"/>
       <c r="AL35" s="33"/>
       <c r="AM35" s="33"/>
       <c r="AN35" s="33"/>
@@ -7794,8 +7822,8 @@
       <c r="AE36" s="31"/>
       <c r="AF36" s="31"/>
       <c r="AG36" s="31"/>
-      <c r="AI36" s="74"/>
-      <c r="AJ36" s="74"/>
+      <c r="AI36" s="76"/>
+      <c r="AJ36" s="76"/>
       <c r="AL36" s="33"/>
       <c r="AM36" s="33"/>
       <c r="AN36" s="33"/>
@@ -7834,8 +7862,8 @@
       <c r="AE37" s="31"/>
       <c r="AF37" s="31"/>
       <c r="AG37" s="31"/>
-      <c r="AI37" s="74"/>
-      <c r="AJ37" s="74"/>
+      <c r="AI37" s="76"/>
+      <c r="AJ37" s="76"/>
       <c r="AL37" s="33"/>
       <c r="AM37" s="33"/>
       <c r="AN37" s="33"/>
@@ -7874,8 +7902,8 @@
       <c r="AE38" s="31"/>
       <c r="AF38" s="31"/>
       <c r="AG38" s="31"/>
-      <c r="AI38" s="74"/>
-      <c r="AJ38" s="74"/>
+      <c r="AI38" s="76"/>
+      <c r="AJ38" s="76"/>
       <c r="AL38" s="33"/>
       <c r="AM38" s="33"/>
       <c r="AN38" s="33"/>
@@ -7914,8 +7942,8 @@
       <c r="AE39" s="31"/>
       <c r="AF39" s="31"/>
       <c r="AG39" s="31"/>
-      <c r="AI39" s="74"/>
-      <c r="AJ39" s="74"/>
+      <c r="AI39" s="76"/>
+      <c r="AJ39" s="76"/>
       <c r="AL39" s="33"/>
       <c r="AM39" s="33"/>
       <c r="AN39" s="33"/>
@@ -7931,8 +7959,8 @@
     </row>
     <row r="40" spans="3:55">
       <c r="AA40" s="28"/>
-      <c r="AI40" s="74"/>
-      <c r="AJ40" s="74"/>
+      <c r="AI40" s="76"/>
+      <c r="AJ40" s="76"/>
       <c r="AR40" s="45"/>
       <c r="AS40" s="45"/>
       <c r="AX40" s="45"/>
@@ -7943,60 +7971,60 @@
       <c r="BC40" s="45"/>
     </row>
     <row r="41" spans="3:55">
-      <c r="AI41" s="74"/>
-      <c r="AJ41" s="74"/>
+      <c r="AI41" s="76"/>
+      <c r="AJ41" s="76"/>
     </row>
     <row r="42" spans="3:55">
-      <c r="AI42" s="74"/>
-      <c r="AJ42" s="74"/>
+      <c r="AI42" s="76"/>
+      <c r="AJ42" s="76"/>
     </row>
     <row r="43" spans="3:55">
-      <c r="AI43" s="74"/>
-      <c r="AJ43" s="74"/>
+      <c r="AI43" s="76"/>
+      <c r="AJ43" s="76"/>
     </row>
     <row r="44" spans="3:55">
-      <c r="AI44" s="74"/>
-      <c r="AJ44" s="74"/>
+      <c r="AI44" s="76"/>
+      <c r="AJ44" s="76"/>
     </row>
     <row r="45" spans="3:55">
-      <c r="AI45" s="74"/>
-      <c r="AJ45" s="74"/>
+      <c r="AI45" s="76"/>
+      <c r="AJ45" s="76"/>
     </row>
     <row r="46" spans="3:55">
-      <c r="AI46" s="74"/>
-      <c r="AJ46" s="74"/>
+      <c r="AI46" s="76"/>
+      <c r="AJ46" s="76"/>
     </row>
     <row r="47" spans="3:55">
-      <c r="AI47" s="74"/>
-      <c r="AJ47" s="74"/>
+      <c r="AI47" s="76"/>
+      <c r="AJ47" s="76"/>
     </row>
     <row r="48" spans="3:55">
-      <c r="AI48" s="74"/>
-      <c r="AJ48" s="74"/>
+      <c r="AI48" s="76"/>
+      <c r="AJ48" s="76"/>
     </row>
     <row r="49" spans="35:36">
-      <c r="AI49" s="74"/>
-      <c r="AJ49" s="74"/>
+      <c r="AI49" s="76"/>
+      <c r="AJ49" s="76"/>
     </row>
     <row r="50" spans="35:36">
-      <c r="AI50" s="74"/>
-      <c r="AJ50" s="74"/>
+      <c r="AI50" s="76"/>
+      <c r="AJ50" s="76"/>
     </row>
     <row r="51" spans="35:36">
-      <c r="AI51" s="74"/>
-      <c r="AJ51" s="74"/>
+      <c r="AI51" s="76"/>
+      <c r="AJ51" s="76"/>
     </row>
     <row r="52" spans="35:36">
-      <c r="AI52" s="74"/>
-      <c r="AJ52" s="74"/>
+      <c r="AI52" s="76"/>
+      <c r="AJ52" s="76"/>
     </row>
     <row r="53" spans="35:36">
-      <c r="AI53" s="74"/>
-      <c r="AJ53" s="74"/>
+      <c r="AI53" s="76"/>
+      <c r="AJ53" s="76"/>
     </row>
     <row r="54" spans="35:36">
-      <c r="AI54" s="74"/>
-      <c r="AJ54" s="74"/>
+      <c r="AI54" s="76"/>
+      <c r="AJ54" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8006,10 +8034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8031,82 +8059,83 @@
     <col min="17" max="17" width="26.1640625" customWidth="1"/>
     <col min="18" max="18" width="24.1640625" customWidth="1"/>
     <col min="19" max="20" width="18.6640625" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="127" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="128" t="s">
+    <row r="1" spans="1:27">
+      <c r="A1" s="126" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="127" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="115" t="s">
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="114" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="114"/>
+      <c r="P1" s="113"/>
       <c r="Q1" s="70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R1" s="70"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
+      <c r="S1" s="113"/>
+      <c r="T1" s="113"/>
       <c r="W1" s="37"/>
       <c r="X1" s="63"/>
       <c r="Y1" s="62"/>
     </row>
-    <row r="2" spans="1:26" ht="17">
-      <c r="A2" s="116" t="s">
+    <row r="2" spans="1:27" ht="17">
+      <c r="A2" s="115" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="116" t="s">
+      <c r="D2" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="116" t="s">
+      <c r="E2" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="116" t="s">
+      <c r="F2" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="G2" s="116" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="117" t="s">
+      <c r="H2" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="117" t="s">
+      <c r="I2" s="116" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="117" t="s">
+      <c r="J2" s="116" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="117" t="s">
+      <c r="K2" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="L2" s="117" t="s">
+      <c r="L2" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="117" t="s">
+      <c r="M2" s="116" t="s">
         <v>104</v>
       </c>
-      <c r="N2" s="117" t="s">
+      <c r="N2" s="116" t="s">
         <v>105</v>
       </c>
       <c r="P2" s="63" t="s">
@@ -8136,14 +8165,14 @@
       <c r="X2" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="Y2" s="41" t="s">
+      <c r="Y2" t="s">
         <v>106</v>
       </c>
-      <c r="Z2" s="41" t="s">
+      <c r="Z2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="17" thickBot="1">
+    <row r="3" spans="1:27" ht="17" thickBot="1">
       <c r="A3" s="68" t="s">
         <v>36</v>
       </c>
@@ -8208,11 +8237,11 @@
         <f t="shared" si="0"/>
         <v>1.0044225086731247</v>
       </c>
-      <c r="S3" s="111">
+      <c r="S3" s="110">
         <f>size_correction!AF3</f>
         <v>1.0056851052976181</v>
       </c>
-      <c r="T3" s="111">
+      <c r="T3" s="110">
         <f>size_correction!AG3</f>
         <v>1.0075218399408568</v>
       </c>
@@ -8233,15 +8262,18 @@
         <v>4.412758119012896E-3</v>
       </c>
       <c r="Y3" s="72">
-        <f>SLOPE(W3:W17,U3:U17)</f>
+        <f>SLOPE(W3:W54,U3:U54)</f>
         <v>1.058002378564959</v>
       </c>
       <c r="Z3" s="72">
-        <f>SLOPE(X3:X17,V3:V17)</f>
+        <f>SLOPE(X3:X54,V3:V54)</f>
         <v>0.9378376950888252</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="AA3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="A4" s="68" t="s">
         <v>38</v>
       </c>
@@ -8306,11 +8338,11 @@
         <f t="shared" si="0"/>
         <v>0.99323347721175648</v>
       </c>
-      <c r="S4" s="111">
+      <c r="S4" s="110">
         <f>size_correction!AF4</f>
         <v>0.99668972770557829</v>
       </c>
-      <c r="T4" s="111">
+      <c r="T4" s="110">
         <f>size_correction!AG4</f>
         <v>0.99497700286985102</v>
       </c>
@@ -8330,8 +8362,19 @@
         <f t="shared" si="3"/>
         <v>-6.7895195007928941E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="18" thickTop="1" thickBot="1">
+      <c r="Y4" s="72">
+        <f>INTERCEPT(W3:W54,U3:U54)</f>
+        <v>-1.8840219242949102E-5</v>
+      </c>
+      <c r="Z4" s="72">
+        <f>INTERCEPT(X3:X54,V3:V54)</f>
+        <v>-1.5500612170959347E-3</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="A5" s="68" t="s">
         <v>37</v>
       </c>
@@ -8396,11 +8439,11 @@
         <f t="shared" si="0"/>
         <v>1.0020859042591113</v>
       </c>
-      <c r="S5" s="111">
+      <c r="S5" s="110">
         <f>size_correction!AF5</f>
         <v>1.0003832772874761</v>
       </c>
-      <c r="T5" s="111">
+      <c r="T5" s="110">
         <f>size_correction!AG5</f>
         <v>1.0043106480077921</v>
       </c>
@@ -8421,9 +8464,9 @@
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="6" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="A6" s="68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6" s="69">
         <v>-22.21</v>
@@ -8486,11 +8529,11 @@
         <f t="shared" si="11"/>
         <v>1.0044225086731247</v>
       </c>
-      <c r="S6" s="111">
+      <c r="S6" s="110">
         <f>size_correction!AF6</f>
         <v>1.0064059824102283</v>
       </c>
-      <c r="T6" s="111">
+      <c r="T6" s="110">
         <f>size_correction!AG6</f>
         <v>1.0077071570383731</v>
       </c>
@@ -8511,7 +8554,7 @@
         <v>4.412758119012896E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="7" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="A7" s="68">
         <v>53504</v>
       </c>
@@ -8576,11 +8619,11 @@
         <f t="shared" si="11"/>
         <v>0.99323347721175648</v>
       </c>
-      <c r="S7" s="111">
+      <c r="S7" s="110">
         <f>size_correction!AF7</f>
         <v>0.99663201609671503</v>
       </c>
-      <c r="T7" s="111">
+      <c r="T7" s="110">
         <f>size_correction!AG7</f>
         <v>0.9951628615034982</v>
       </c>
@@ -8601,9 +8644,9 @@
         <v>-6.7895195007928941E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="8" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="A8" s="68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8" s="69">
         <v>17.11</v>
@@ -8666,11 +8709,11 @@
         <f t="shared" si="11"/>
         <v>1.0020859042591113</v>
       </c>
-      <c r="S8" s="111">
+      <c r="S8" s="110">
         <f>size_correction!AF8</f>
         <v>0.99917068284195976</v>
       </c>
-      <c r="T8" s="111">
+      <c r="T8" s="110">
         <f>size_correction!AG8</f>
         <v>1.0023860907979212</v>
       </c>
@@ -8691,48 +8734,48 @@
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="18" thickTop="1" thickBot="1">
-      <c r="A9" s="118">
+    <row r="9" spans="1:27" ht="18" thickTop="1" thickBot="1">
+      <c r="A9" s="117">
         <v>90454</v>
       </c>
-      <c r="B9" s="119">
+      <c r="B9" s="118">
         <v>25.73</v>
       </c>
-      <c r="C9" s="119">
+      <c r="C9" s="118">
         <v>25.44</v>
       </c>
-      <c r="D9" s="119">
+      <c r="D9" s="118">
         <f t="shared" si="10"/>
         <v>25.585000000000001</v>
       </c>
-      <c r="E9" s="119">
+      <c r="E9" s="118">
         <v>35.880000000000003</v>
       </c>
-      <c r="F9" s="119">
+      <c r="F9" s="118">
         <f t="shared" si="4"/>
         <v>0.28999999999999915</v>
       </c>
-      <c r="G9" s="120">
+      <c r="G9" s="119">
         <f t="shared" si="5"/>
         <v>3.7710963450000002E-3</v>
       </c>
-      <c r="H9" s="120">
+      <c r="H9" s="119">
         <f t="shared" si="5"/>
         <v>3.7700301599999995E-3</v>
       </c>
-      <c r="I9" s="120">
+      <c r="I9" s="119">
         <f t="shared" si="6"/>
         <v>2.0771465759999996E-3</v>
       </c>
-      <c r="J9" s="120">
+      <c r="J9" s="119">
         <f t="shared" si="7"/>
         <v>3.8687348777560239E-4</v>
       </c>
-      <c r="K9" s="121">
+      <c r="K9" s="120">
         <f t="shared" si="8"/>
         <v>7.9279999927756029E-3</v>
       </c>
-      <c r="L9" s="121">
+      <c r="L9" s="120">
         <f t="shared" si="9"/>
         <v>2.0942811848696616E-3</v>
       </c>
@@ -8756,11 +8799,11 @@
         <f>N3</f>
         <v>1.0044225086731247</v>
       </c>
-      <c r="S9" s="111">
+      <c r="S9" s="110">
         <f>size_correction!AF9</f>
         <v>1.0050941512728657</v>
       </c>
-      <c r="T9" s="111">
+      <c r="T9" s="110">
         <f>size_correction!AG9</f>
         <v>1.0057116133646442</v>
       </c>
@@ -8781,7 +8824,7 @@
         <v>4.412758119012896E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="10" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="A10" s="63"/>
       <c r="B10" s="63"/>
       <c r="C10" s="63"/>
@@ -8801,11 +8844,11 @@
       </c>
       <c r="Q10" s="68"/>
       <c r="R10" s="68"/>
-      <c r="S10" s="111">
+      <c r="S10" s="110">
         <f>size_correction!AF10</f>
         <v>0.99092722925764687</v>
       </c>
-      <c r="T10" s="111">
+      <c r="T10" s="110">
         <f>size_correction!AG10</f>
         <v>1.0049378092932522</v>
       </c>
@@ -8820,7 +8863,7 @@
       <c r="W10" s="67"/>
       <c r="X10" s="67"/>
     </row>
-    <row r="11" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="11" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="L11" s="63"/>
       <c r="M11" s="63"/>
       <c r="P11" s="63" t="str">
@@ -8835,11 +8878,11 @@
         <f t="shared" si="12"/>
         <v>1.0044225086731247</v>
       </c>
-      <c r="S11" s="111">
+      <c r="S11" s="110">
         <f>size_correction!AF11</f>
         <v>1.0057192814133826</v>
       </c>
-      <c r="T11" s="111">
+      <c r="T11" s="110">
         <f>size_correction!AG11</f>
         <v>1.0054625917600983</v>
       </c>
@@ -8860,7 +8903,7 @@
         <v>4.412758119012896E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1">
+    <row r="12" spans="1:27" s="41" customFormat="1" ht="18" thickTop="1" thickBot="1">
       <c r="M12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63" t="str">
@@ -8875,11 +8918,11 @@
         <f t="shared" si="12"/>
         <v>0.99323347721175648</v>
       </c>
-      <c r="S12" s="111">
+      <c r="S12" s="110">
         <f>size_correction!AF12</f>
         <v>0.99641187878361481</v>
       </c>
-      <c r="T12" s="111">
+      <c r="T12" s="110">
         <f>size_correction!AG12</f>
         <v>0.99378130442821833</v>
       </c>
@@ -8902,7 +8945,7 @@
       <c r="Y12"/>
       <c r="Z12"/>
     </row>
-    <row r="13" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="13" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="P13" s="63" t="str">
         <f>size_correction!D13</f>
         <v>B6_ref_1</v>
@@ -8915,11 +8958,11 @@
         <f t="shared" si="12"/>
         <v>1.0020859042591113</v>
       </c>
-      <c r="S13" s="111">
+      <c r="S13" s="110">
         <f>size_correction!AF13</f>
         <v>1.0001796848444418</v>
       </c>
-      <c r="T13" s="111">
+      <c r="T13" s="110">
         <f>size_correction!AG13</f>
         <v>1.0040343543858852</v>
       </c>
@@ -8940,7 +8983,7 @@
         <v>2.0837317813513596E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="14" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="P14" s="63" t="str">
         <f>size_correction!D14</f>
         <v>ATM_EQ_SW_2</v>
@@ -8953,11 +8996,11 @@
         <f>N3</f>
         <v>1.0044225086731247</v>
       </c>
-      <c r="S14" s="111">
+      <c r="S14" s="110">
         <f>size_correction!AF14</f>
         <v>1.0048805539160894</v>
       </c>
-      <c r="T14" s="111">
+      <c r="T14" s="110">
         <f>size_correction!AG14</f>
         <v>1.0053599727245706</v>
       </c>
@@ -8978,7 +9021,7 @@
         <v>4.412758119012896E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="15" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="P15" s="63" t="str">
         <f>size_correction!D15</f>
         <v>ATM_EQ_SW_3</v>
@@ -8991,11 +9034,11 @@
         <f>N3</f>
         <v>1.0044225086731247</v>
       </c>
-      <c r="S15" s="111">
+      <c r="S15" s="110">
         <f>size_correction!AF15</f>
         <v>1.0056387310168626</v>
       </c>
-      <c r="T15" s="111">
+      <c r="T15" s="110">
         <f>size_correction!AG15</f>
         <v>1.0064676550191509</v>
       </c>
@@ -9016,7 +9059,7 @@
         <v>4.412758119012896E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="18" thickTop="1" thickBot="1">
+    <row r="16" spans="1:27" ht="18" thickTop="1" thickBot="1">
       <c r="P16" s="63" t="str">
         <f>size_correction!D16</f>
         <v>S2_ref_2</v>
@@ -9029,11 +9072,11 @@
         <f>N4</f>
         <v>0.99323347721175648</v>
       </c>
-      <c r="S16" s="111">
+      <c r="S16" s="110">
         <f>size_correction!AF16</f>
         <v>0.99633327484903467</v>
       </c>
-      <c r="T16" s="111">
+      <c r="T16" s="110">
         <f>size_correction!AG16</f>
         <v>0.99474403428411884</v>
       </c>
@@ -9061,11 +9104,11 @@
       </c>
       <c r="Q17" s="68"/>
       <c r="R17" s="68"/>
-      <c r="S17" s="111">
+      <c r="S17" s="110">
         <f>size_correction!AF17</f>
         <v>0.99349493237592013</v>
       </c>
-      <c r="T17" s="111">
+      <c r="T17" s="110">
         <f>size_correction!AG17</f>
         <v>1.0044001925480899</v>
       </c>
@@ -9175,7 +9218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A9B09D-1008-4441-AE31-949281019A29}">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -9190,118 +9233,118 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N1">
         <v>3.7990000000000002E-4</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N2">
         <v>2.0052E-3</v>
       </c>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="128" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="129" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="130" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="129"/>
       <c r="M3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N3">
         <v>0.51600000000000001</v>
       </c>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="112" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="112" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="112" t="s">
+        <v>138</v>
+      </c>
+      <c r="N4" s="112" t="s">
+        <v>141</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" s="113" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="L4" s="113" t="s">
-        <v>141</v>
-      </c>
-      <c r="M4" s="113" t="s">
-        <v>139</v>
-      </c>
-      <c r="N4" s="113" t="s">
-        <v>142</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q4" s="113" t="s">
+      <c r="Q4" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="R4" s="113" t="s">
+      <c r="R4" s="112" t="s">
         <v>95</v>
       </c>
-      <c r="V4" s="113"/>
-      <c r="Y4" s="113"/>
+      <c r="V4" s="112"/>
+      <c r="Y4" s="112"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="68">
@@ -9316,7 +9359,7 @@
       <c r="D5" s="68">
         <v>7.7934998191650307E-3</v>
       </c>
-      <c r="E5" s="112">
+      <c r="E5" s="111">
         <v>2.1164798861162191E-3</v>
       </c>
       <c r="F5" s="68">
@@ -9334,7 +9377,7 @@
       <c r="J5" s="68">
         <v>7.7441640342372194E-3</v>
       </c>
-      <c r="K5" s="112">
+      <c r="K5" s="111">
         <v>2.109788966545483E-3</v>
       </c>
       <c r="L5" s="68">
@@ -9356,11 +9399,11 @@
         <f>$N$1*(N5/$N$2)^$N$3</f>
         <v>3.8843308121852137E-4</v>
       </c>
-      <c r="Q5" s="85">
+      <c r="Q5" s="84">
         <f>(A5+R5*B5+A5*B5-(C5-O5)*(1+(1-R5)*B5))/(A5*(1+C5-O5))</f>
         <v>0.20872209614007559</v>
       </c>
-      <c r="R5" s="85">
+      <c r="R5" s="84">
         <f>((A5-C5+O5)*(1+B5)/(A5*(1+C5-O5)) - (G5-I5+P5)*(1+H5)/(G5*(1+I5-P5)))/(H5/G5-B5/A5)</f>
         <v>0.1159684103244177</v>
       </c>
@@ -9378,7 +9421,7 @@
       <c r="D6" s="68">
         <v>7.7934998191650307E-3</v>
       </c>
-      <c r="E6" s="112">
+      <c r="E6" s="111">
         <v>2.1164798861162191E-3</v>
       </c>
       <c r="F6" s="68">
@@ -9396,7 +9439,7 @@
       <c r="J6" s="68">
         <v>7.7342329865834319E-3</v>
       </c>
-      <c r="K6" s="112">
+      <c r="K6" s="111">
         <v>2.105997079923158E-3</v>
       </c>
       <c r="L6" s="68">
@@ -9418,11 +9461,11 @@
         <f>$N$1*(N6/$N$2)^$N$3</f>
         <v>3.8807385113215798E-4</v>
       </c>
-      <c r="Q6" s="85">
+      <c r="Q6" s="84">
         <f>(A6+R6*B6+A6*B6-(C6-O6)*(1+(1-R6)*B6))/(A6*(1+C6-O6))</f>
         <v>0.17329677501906443</v>
       </c>
-      <c r="R6" s="85">
+      <c r="R6" s="84">
         <f>((A6-C6+O6)*(1+B6)/(A6*(1+C6-O6)) - (G6-I6+P6)*(1+H6)/(G6*(1+I6-P6)))/(H6/G6-B6/A6)</f>
         <v>7.9867779580351114E-2</v>
       </c>
@@ -9480,11 +9523,11 @@
         <f t="shared" ref="P7:P11" si="1">$N$1*(N7/$N$2)^$N$3</f>
         <v>3.8843308121852137E-4</v>
       </c>
-      <c r="Q7" s="85">
+      <c r="Q7" s="84">
         <f t="shared" ref="Q7:Q11" si="2">(A7+R7*B7+A7*B7-(C7-O7)*(1+(1-R7)*B7))/(A7*(1+C7-O7))</f>
         <v>0.17733587859609368</v>
       </c>
-      <c r="R7" s="85">
+      <c r="R7" s="84">
         <f t="shared" ref="R7:R11" si="3">((A7-C7+O7)*(1+B7)/(A7*(1+C7-O7)) - (G7-I7+P7)*(1+H7)/(G7*(1+I7-P7)))/(H7/G7-B7/A7)</f>
         <v>8.4590223076979915E-2</v>
       </c>
@@ -9542,11 +9585,11 @@
         <f t="shared" si="1"/>
         <v>3.8807385113215798E-4</v>
       </c>
-      <c r="Q8" s="85">
+      <c r="Q8" s="84">
         <f t="shared" si="2"/>
         <v>0.14191055747508233</v>
       </c>
-      <c r="R8" s="85">
+      <c r="R8" s="84">
         <f t="shared" si="3"/>
         <v>4.8489592332913341E-2</v>
       </c>
@@ -9604,11 +9647,11 @@
         <f t="shared" si="1"/>
         <v>3.883816255649651E-4</v>
       </c>
-      <c r="Q9" s="85">
+      <c r="Q9" s="84">
         <f t="shared" si="2"/>
         <v>0.14994727862657609</v>
       </c>
-      <c r="R9" s="85">
+      <c r="R9" s="84">
         <f t="shared" si="3"/>
         <v>5.7620461575761298E-2</v>
       </c>
@@ -9666,11 +9709,11 @@
         <f t="shared" si="1"/>
         <v>3.883816255649651E-4</v>
       </c>
-      <c r="Q10" s="85">
+      <c r="Q10" s="84">
         <f t="shared" si="2"/>
         <v>0.26277357755180591</v>
       </c>
-      <c r="R10" s="85">
+      <c r="R10" s="84">
         <f t="shared" si="3"/>
         <v>0.17041789341507743</v>
       </c>
@@ -9728,31 +9771,31 @@
         <f t="shared" si="1"/>
         <v>3.883816255649651E-4</v>
       </c>
-      <c r="Q11" s="85">
+      <c r="Q11" s="84">
         <f t="shared" si="2"/>
         <v>0.16880903099141051</v>
       </c>
-      <c r="R11" s="85">
+      <c r="R11" s="84">
         <f t="shared" si="3"/>
         <v>7.6477388081454753E-2</v>
       </c>
     </row>
     <row r="13" spans="1:25">
-      <c r="Q13" s="85">
+      <c r="Q13" s="84">
         <f>AVERAGE(Q5:Q11)</f>
         <v>0.18325645634287266</v>
       </c>
-      <c r="R13" s="85">
+      <c r="R13" s="84">
         <f>AVERAGE(R5:R11)</f>
         <v>9.0490249769565087E-2</v>
       </c>
     </row>
     <row r="14" spans="1:25">
-      <c r="Q14" s="85">
+      <c r="Q14" s="84">
         <f>STDEV(Q5:Q11)</f>
         <v>4.1096294725866948E-2</v>
       </c>
-      <c r="R14" s="85">
+      <c r="R14" s="84">
         <f>STDEV(R5:R11)</f>
         <v>4.1283674266355812E-2</v>
       </c>
@@ -9786,187 +9829,187 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+        <v>142</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="81">
+        <v>143</v>
+      </c>
+      <c r="B2" s="80">
         <f>B12</f>
         <v>0.4623614635092998</v>
       </c>
-      <c r="C2" s="79" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="81">
+      <c r="C2" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="80">
         <f>C12</f>
         <v>0.10975712247295455</v>
       </c>
       <c r="F2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G2" s="50">
         <f>1/B2</f>
         <v>2.1628100067208269</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
-      </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+        <v>159</v>
+      </c>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
       <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="81">
+        <v>145</v>
+      </c>
+      <c r="B3" s="80">
         <f>B13</f>
         <v>8.0186890671505306E-3</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="81">
+      <c r="C3" s="78"/>
+      <c r="D3" s="80">
         <f>C13</f>
         <v>0.30903560626553517</v>
       </c>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="80">
+        <v>1.026</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="E4" s="78" t="s">
         <v>147</v>
-      </c>
-      <c r="B4" s="81">
-        <v>1.026</v>
-      </c>
-      <c r="C4" s="79"/>
-      <c r="E4" s="79" t="s">
-        <v>148</v>
       </c>
       <c r="F4">
         <v>0.99819999999999998</v>
       </c>
-      <c r="H4" s="79" t="s">
-        <v>149</v>
+      <c r="H4" s="78" t="s">
+        <v>148</v>
       </c>
       <c r="I4">
         <v>1.002</v>
       </c>
-      <c r="L4" s="82"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="85">
+        <v>149</v>
+      </c>
+      <c r="B5" s="84">
         <f>1/B4</f>
         <v>0.97465886939571145</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="E5" s="79" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="85">
+      <c r="C5" s="78"/>
+      <c r="E5" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="84">
         <f>1/F4</f>
         <v>1.0018032458425166</v>
       </c>
-      <c r="H5" s="79" t="s">
-        <v>152</v>
-      </c>
-      <c r="I5" s="85">
+      <c r="H5" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="84">
         <f>1/I4</f>
         <v>0.99800399201596801</v>
       </c>
-      <c r="L5" s="82"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="87"/>
-      <c r="R5" s="82"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="81"/>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" s="88">
+        <v>152</v>
+      </c>
+      <c r="B6" s="87">
         <f>B5/1000</f>
         <v>9.7465886939571145E-4</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="E6" s="79" t="s">
-        <v>154</v>
-      </c>
-      <c r="F6" s="88">
+      <c r="C6" s="78"/>
+      <c r="E6" s="78" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="87">
         <f>F5/1000</f>
         <v>1.0018032458425166E-3</v>
       </c>
-      <c r="H6" s="79" t="s">
-        <v>155</v>
-      </c>
-      <c r="I6" s="88">
+      <c r="H6" s="78" t="s">
+        <v>154</v>
+      </c>
+      <c r="I6" s="87">
         <f>I5/1000</f>
         <v>9.9800399201596798E-4</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="87"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="86"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="L7" s="82"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="82"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" spans="1:18" ht="18">
-      <c r="L8" s="82"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="82"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="81"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="M9" s="92"/>
-      <c r="N9" s="82"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="81"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="93" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="95"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="97"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="82"/>
+      <c r="A10" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="94"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="96"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="81"/>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F11" s="79"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
@@ -9983,7 +10026,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13">
         <v>8.0186890671505306E-3</v>
@@ -10001,8 +10044,8 @@
         <v>0.96347094633189312</v>
       </c>
       <c r="D14" s="50"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="99"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="98"/>
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
       <c r="I14" s="50"/>
@@ -10028,21 +10071,21 @@
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="50"/>
-      <c r="F16" s="100"/>
+      <c r="F16" s="99"/>
       <c r="G16" s="50"/>
       <c r="I16" s="50"/>
     </row>
     <row r="17" spans="4:10">
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
-      <c r="F17" s="100"/>
+      <c r="F17" s="99"/>
     </row>
     <row r="18" spans="4:10">
       <c r="G18" s="50"/>
-      <c r="I18" s="101"/>
+      <c r="I18" s="100"/>
     </row>
     <row r="20" spans="4:10">
-      <c r="J20" s="102"/>
+      <c r="J20" s="101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>